<commit_message>
add custom stylesheet, temp videos, fontawesome
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -14,10 +14,37 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
+    <t>HEADLINE</t>
+  </si>
+  <si>
+    <t>LOCATION</t>
+  </si>
+  <si>
+    <t>YOUTUBE_ID</t>
+  </si>
+  <si>
+    <t>SHORT_DESC</t>
+  </si>
+  <si>
+    <t>DATE_PUBLISHED</t>
+  </si>
+  <si>
+    <t>A New Bid to End Texting While Driving</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
     <t>Series</t>
   </si>
   <si>
-    <t>HEADLINE</t>
+    <t>INV9hShE-Bg</t>
+  </si>
+  <si>
+    <t>For the fifth straight legislative session, Texas lawmakers will consider bills proposing a statewide ban on texting while driving. There’s more momentum than ever to get it passed, but a difference of opinions among the state’s new leadership could stand in its way.</t>
+  </si>
+  <si>
+    <t>Jan. 20, 2015</t>
   </si>
   <si>
     <t>Subtitle</t>
@@ -26,18 +53,6 @@
     <t>facebook_text</t>
   </si>
   <si>
-    <t>LOCATION</t>
-  </si>
-  <si>
-    <t>YOUTUBE_ID</t>
-  </si>
-  <si>
-    <t>SHORT_DESC</t>
-  </si>
-  <si>
-    <t>DATE_PUBLISHED</t>
-  </si>
-  <si>
     <t>twitter_text</t>
   </si>
   <si>
@@ -45,21 +60,6 @@
   </si>
   <si>
     <t>Community Concerns Come to the Capitol</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur </t>
-  </si>
-  <si>
-    <t>Texas</t>
-  </si>
-  <si>
-    <t>_XhNS2Vk9OQ</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Sed at lectus et justo pharetra congue quis id arcu. Vestibulum feugiat lectus id urna accumsan tincidunt. Integer eleifend odio vitae nisi cursus convallis. </t>
-  </si>
-  <si>
-    <t>Jan. 20, 2015</t>
   </si>
   <si>
     <t>Lorem ipsum dolor sit amet, consectetur </t>
@@ -176,9 +176,6 @@
       <sz val="10.0"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <b/>
-    </font>
     <font/>
     <font>
       <b/>
@@ -186,6 +183,9 @@
     </font>
     <font>
       <sz val="10.0"/>
+    </font>
+    <font>
+      <b/>
     </font>
   </fonts>
   <fills count="2">
@@ -222,14 +222,14 @@
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
       <alignment/>
     </xf>
+    <xf fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1"/>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3">
       <alignment/>
     </xf>
-    <xf fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2"/>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="4">
       <alignment/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
       <alignment/>
     </xf>
   </cellXfs>
@@ -260,25 +260,25 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c t="s" s="1" r="A1">
-        <v>0</v>
-      </c>
-      <c t="s" s="1" r="B1">
-        <v>2</v>
-      </c>
-      <c t="s" s="2" r="C1">
-        <v>3</v>
-      </c>
-      <c t="s" s="2" r="D1">
-        <v>8</v>
+      <c t="s" s="5" r="A1">
+        <v>7</v>
+      </c>
+      <c t="s" s="5" r="B1">
+        <v>11</v>
+      </c>
+      <c t="s" s="1" r="C1">
+        <v>12</v>
+      </c>
+      <c t="s" s="1" r="D1">
+        <v>13</v>
       </c>
     </row>
     <row r="2">
-      <c t="s" s="2" r="A2">
-        <v>9</v>
-      </c>
-      <c t="s" s="2" r="B2">
-        <v>10</v>
+      <c t="s" s="1" r="A2">
+        <v>14</v>
+      </c>
+      <c t="s" s="1" r="B2">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -297,50 +297,50 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c t="s" s="2" r="A1">
+      <c t="s" s="1" r="A1">
+        <v>0</v>
+      </c>
+      <c t="s" s="2" r="B1">
         <v>1</v>
       </c>
-      <c t="s" s="3" r="B1">
+      <c t="s" s="1" r="C1">
+        <v>2</v>
+      </c>
+      <c t="s" s="1" r="D1">
+        <v>3</v>
+      </c>
+      <c t="s" s="3" r="E1">
         <v>4</v>
       </c>
-      <c t="s" s="2" r="C1">
+    </row>
+    <row r="2">
+      <c t="s" s="1" r="A2">
         <v>5</v>
       </c>
-      <c t="s" s="2" r="D1">
+      <c t="s" s="4" r="B2">
         <v>6</v>
       </c>
-      <c t="s" s="4" r="E1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2">
-      <c t="s" s="2" r="A2">
-        <v>11</v>
-      </c>
-      <c t="s" s="5" r="B2">
-        <v>12</v>
-      </c>
-      <c t="s" s="2" r="C2">
-        <v>13</v>
-      </c>
-      <c t="s" s="2" r="D2">
-        <v>14</v>
+      <c t="s" s="1" r="C2">
+        <v>8</v>
+      </c>
+      <c t="s" s="1" r="D2">
+        <v>9</v>
       </c>
       <c t="s" s="6" r="E2">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
-      <c t="s" s="2" r="A3">
+      <c t="s" s="1" r="A3">
         <v>16</v>
       </c>
-      <c t="s" s="5" r="B3">
+      <c t="s" s="4" r="B3">
         <v>17</v>
       </c>
-      <c t="s" s="2" r="C3">
+      <c t="s" s="1" r="C3">
         <v>18</v>
       </c>
-      <c t="s" s="2" r="D3">
+      <c t="s" s="1" r="D3">
         <v>19</v>
       </c>
       <c t="s" s="6" r="E3">
@@ -348,16 +348,16 @@
       </c>
     </row>
     <row r="4">
-      <c t="s" s="2" r="A4">
+      <c t="s" s="1" r="A4">
         <v>21</v>
       </c>
-      <c t="s" s="5" r="B4">
+      <c t="s" s="4" r="B4">
         <v>22</v>
       </c>
-      <c t="s" s="2" r="C4">
+      <c t="s" s="1" r="C4">
         <v>23</v>
       </c>
-      <c t="s" s="2" r="D4">
+      <c t="s" s="1" r="D4">
         <v>24</v>
       </c>
       <c t="s" s="6" r="E4">
@@ -365,16 +365,16 @@
       </c>
     </row>
     <row r="5">
-      <c t="s" s="2" r="A5">
+      <c t="s" s="1" r="A5">
         <v>26</v>
       </c>
-      <c t="s" s="5" r="B5">
+      <c t="s" s="4" r="B5">
         <v>27</v>
       </c>
-      <c t="s" s="2" r="C5">
+      <c t="s" s="1" r="C5">
         <v>28</v>
       </c>
-      <c t="s" s="2" r="D5">
+      <c t="s" s="1" r="D5">
         <v>29</v>
       </c>
       <c t="s" s="6" r="E5">
@@ -382,16 +382,16 @@
       </c>
     </row>
     <row r="6">
-      <c t="s" s="2" r="A6">
+      <c t="s" s="1" r="A6">
         <v>31</v>
       </c>
-      <c t="s" s="5" r="B6">
+      <c t="s" s="4" r="B6">
         <v>32</v>
       </c>
-      <c t="s" s="2" r="C6">
+      <c t="s" s="1" r="C6">
         <v>33</v>
       </c>
-      <c t="s" s="2" r="D6">
+      <c t="s" s="1" r="D6">
         <v>34</v>
       </c>
       <c t="s" s="6" r="E6">
@@ -399,16 +399,16 @@
       </c>
     </row>
     <row r="7">
-      <c t="s" s="2" r="A7">
+      <c t="s" s="1" r="A7">
         <v>36</v>
       </c>
-      <c t="s" s="5" r="B7">
+      <c t="s" s="4" r="B7">
         <v>37</v>
       </c>
-      <c t="s" s="2" r="C7">
+      <c t="s" s="1" r="C7">
         <v>38</v>
       </c>
-      <c t="s" s="2" r="D7">
+      <c t="s" s="1" r="D7">
         <v>39</v>
       </c>
       <c t="s" s="6" r="E7">
@@ -416,16 +416,16 @@
       </c>
     </row>
     <row r="8">
-      <c t="s" s="2" r="A8">
+      <c t="s" s="1" r="A8">
         <v>41</v>
       </c>
-      <c t="s" s="5" r="B8">
+      <c t="s" s="4" r="B8">
         <v>42</v>
       </c>
-      <c t="s" s="2" r="C8">
+      <c t="s" s="1" r="C8">
         <v>43</v>
       </c>
-      <c t="s" s="2" r="D8">
+      <c t="s" s="1" r="D8">
         <v>44</v>
       </c>
       <c t="s" s="6" r="E8">
@@ -433,16 +433,16 @@
       </c>
     </row>
     <row r="9">
-      <c t="s" s="2" r="A9">
+      <c t="s" s="1" r="A9">
         <v>46</v>
       </c>
-      <c t="s" s="5" r="B9">
+      <c t="s" s="4" r="B9">
         <v>47</v>
       </c>
-      <c t="s" s="2" r="C9">
+      <c t="s" s="1" r="C9">
         <v>48</v>
       </c>
-      <c t="s" s="2" r="D9">
+      <c t="s" s="1" r="D9">
         <v>49</v>
       </c>
       <c t="s" s="6" r="E9">
@@ -450,2977 +450,2977 @@
       </c>
     </row>
     <row r="10">
-      <c s="4" r="E10"/>
+      <c s="3" r="E10"/>
     </row>
     <row r="11">
-      <c s="4" r="E11"/>
+      <c s="3" r="E11"/>
     </row>
     <row r="12">
-      <c s="4" r="E12"/>
+      <c s="3" r="E12"/>
     </row>
     <row r="13">
-      <c s="4" r="E13"/>
+      <c s="3" r="E13"/>
     </row>
     <row r="14">
-      <c s="4" r="E14"/>
+      <c s="3" r="E14"/>
     </row>
     <row r="15">
-      <c s="4" r="E15"/>
+      <c s="3" r="E15"/>
     </row>
     <row r="16">
-      <c s="4" r="E16"/>
+      <c s="3" r="E16"/>
     </row>
     <row r="17">
-      <c s="4" r="E17"/>
+      <c s="3" r="E17"/>
     </row>
     <row r="18">
-      <c s="4" r="E18"/>
+      <c s="3" r="E18"/>
     </row>
     <row r="19">
-      <c s="4" r="E19"/>
+      <c s="3" r="E19"/>
     </row>
     <row r="20">
-      <c s="4" r="E20"/>
+      <c s="3" r="E20"/>
     </row>
     <row r="21">
-      <c s="4" r="E21"/>
+      <c s="3" r="E21"/>
     </row>
     <row r="22">
-      <c s="4" r="E22"/>
+      <c s="3" r="E22"/>
     </row>
     <row r="23">
-      <c s="4" r="E23"/>
+      <c s="3" r="E23"/>
     </row>
     <row r="24">
-      <c s="4" r="E24"/>
+      <c s="3" r="E24"/>
     </row>
     <row r="25">
-      <c s="4" r="E25"/>
+      <c s="3" r="E25"/>
     </row>
     <row r="26">
-      <c s="4" r="E26"/>
+      <c s="3" r="E26"/>
     </row>
     <row r="27">
-      <c s="4" r="E27"/>
+      <c s="3" r="E27"/>
     </row>
     <row r="28">
-      <c s="4" r="E28"/>
+      <c s="3" r="E28"/>
     </row>
     <row r="29">
-      <c s="4" r="E29"/>
+      <c s="3" r="E29"/>
     </row>
     <row r="30">
-      <c s="4" r="E30"/>
+      <c s="3" r="E30"/>
     </row>
     <row r="31">
-      <c s="4" r="E31"/>
+      <c s="3" r="E31"/>
     </row>
     <row r="32">
-      <c s="4" r="E32"/>
+      <c s="3" r="E32"/>
     </row>
     <row r="33">
-      <c s="4" r="E33"/>
+      <c s="3" r="E33"/>
     </row>
     <row r="34">
-      <c s="4" r="E34"/>
+      <c s="3" r="E34"/>
     </row>
     <row r="35">
-      <c s="4" r="E35"/>
+      <c s="3" r="E35"/>
     </row>
     <row r="36">
-      <c s="4" r="E36"/>
+      <c s="3" r="E36"/>
     </row>
     <row r="37">
-      <c s="4" r="E37"/>
+      <c s="3" r="E37"/>
     </row>
     <row r="38">
-      <c s="4" r="E38"/>
+      <c s="3" r="E38"/>
     </row>
     <row r="39">
-      <c s="4" r="E39"/>
+      <c s="3" r="E39"/>
     </row>
     <row r="40">
-      <c s="4" r="E40"/>
+      <c s="3" r="E40"/>
     </row>
     <row r="41">
-      <c s="4" r="E41"/>
+      <c s="3" r="E41"/>
     </row>
     <row r="42">
-      <c s="4" r="E42"/>
+      <c s="3" r="E42"/>
     </row>
     <row r="43">
-      <c s="4" r="E43"/>
+      <c s="3" r="E43"/>
     </row>
     <row r="44">
-      <c s="4" r="E44"/>
+      <c s="3" r="E44"/>
     </row>
     <row r="45">
-      <c s="4" r="E45"/>
+      <c s="3" r="E45"/>
     </row>
     <row r="46">
-      <c s="4" r="E46"/>
+      <c s="3" r="E46"/>
     </row>
     <row r="47">
-      <c s="4" r="E47"/>
+      <c s="3" r="E47"/>
     </row>
     <row r="48">
-      <c s="4" r="E48"/>
+      <c s="3" r="E48"/>
     </row>
     <row r="49">
-      <c s="4" r="E49"/>
+      <c s="3" r="E49"/>
     </row>
     <row r="50">
-      <c s="4" r="E50"/>
+      <c s="3" r="E50"/>
     </row>
     <row r="51">
-      <c s="4" r="E51"/>
+      <c s="3" r="E51"/>
     </row>
     <row r="52">
-      <c s="4" r="E52"/>
+      <c s="3" r="E52"/>
     </row>
     <row r="53">
-      <c s="4" r="E53"/>
+      <c s="3" r="E53"/>
     </row>
     <row r="54">
-      <c s="4" r="E54"/>
+      <c s="3" r="E54"/>
     </row>
     <row r="55">
-      <c s="4" r="E55"/>
+      <c s="3" r="E55"/>
     </row>
     <row r="56">
-      <c s="4" r="E56"/>
+      <c s="3" r="E56"/>
     </row>
     <row r="57">
-      <c s="4" r="E57"/>
+      <c s="3" r="E57"/>
     </row>
     <row r="58">
-      <c s="4" r="E58"/>
+      <c s="3" r="E58"/>
     </row>
     <row r="59">
-      <c s="4" r="E59"/>
+      <c s="3" r="E59"/>
     </row>
     <row r="60">
-      <c s="4" r="E60"/>
+      <c s="3" r="E60"/>
     </row>
     <row r="61">
-      <c s="4" r="E61"/>
+      <c s="3" r="E61"/>
     </row>
     <row r="62">
-      <c s="4" r="E62"/>
+      <c s="3" r="E62"/>
     </row>
     <row r="63">
-      <c s="4" r="E63"/>
+      <c s="3" r="E63"/>
     </row>
     <row r="64">
-      <c s="4" r="E64"/>
+      <c s="3" r="E64"/>
     </row>
     <row r="65">
-      <c s="4" r="E65"/>
+      <c s="3" r="E65"/>
     </row>
     <row r="66">
-      <c s="4" r="E66"/>
+      <c s="3" r="E66"/>
     </row>
     <row r="67">
-      <c s="4" r="E67"/>
+      <c s="3" r="E67"/>
     </row>
     <row r="68">
-      <c s="4" r="E68"/>
+      <c s="3" r="E68"/>
     </row>
     <row r="69">
-      <c s="4" r="E69"/>
+      <c s="3" r="E69"/>
     </row>
     <row r="70">
-      <c s="4" r="E70"/>
+      <c s="3" r="E70"/>
     </row>
     <row r="71">
-      <c s="4" r="E71"/>
+      <c s="3" r="E71"/>
     </row>
     <row r="72">
-      <c s="4" r="E72"/>
+      <c s="3" r="E72"/>
     </row>
     <row r="73">
-      <c s="4" r="E73"/>
+      <c s="3" r="E73"/>
     </row>
     <row r="74">
-      <c s="4" r="E74"/>
+      <c s="3" r="E74"/>
     </row>
     <row r="75">
-      <c s="4" r="E75"/>
+      <c s="3" r="E75"/>
     </row>
     <row r="76">
-      <c s="4" r="E76"/>
+      <c s="3" r="E76"/>
     </row>
     <row r="77">
-      <c s="4" r="E77"/>
+      <c s="3" r="E77"/>
     </row>
     <row r="78">
-      <c s="4" r="E78"/>
+      <c s="3" r="E78"/>
     </row>
     <row r="79">
-      <c s="4" r="E79"/>
+      <c s="3" r="E79"/>
     </row>
     <row r="80">
-      <c s="4" r="E80"/>
+      <c s="3" r="E80"/>
     </row>
     <row r="81">
-      <c s="4" r="E81"/>
+      <c s="3" r="E81"/>
     </row>
     <row r="82">
-      <c s="4" r="E82"/>
+      <c s="3" r="E82"/>
     </row>
     <row r="83">
-      <c s="4" r="E83"/>
+      <c s="3" r="E83"/>
     </row>
     <row r="84">
-      <c s="4" r="E84"/>
+      <c s="3" r="E84"/>
     </row>
     <row r="85">
-      <c s="4" r="E85"/>
+      <c s="3" r="E85"/>
     </row>
     <row r="86">
-      <c s="4" r="E86"/>
+      <c s="3" r="E86"/>
     </row>
     <row r="87">
-      <c s="4" r="E87"/>
+      <c s="3" r="E87"/>
     </row>
     <row r="88">
-      <c s="4" r="E88"/>
+      <c s="3" r="E88"/>
     </row>
     <row r="89">
-      <c s="4" r="E89"/>
+      <c s="3" r="E89"/>
     </row>
     <row r="90">
-      <c s="4" r="E90"/>
+      <c s="3" r="E90"/>
     </row>
     <row r="91">
-      <c s="4" r="E91"/>
+      <c s="3" r="E91"/>
     </row>
     <row r="92">
-      <c s="4" r="E92"/>
+      <c s="3" r="E92"/>
     </row>
     <row r="93">
-      <c s="4" r="E93"/>
+      <c s="3" r="E93"/>
     </row>
     <row r="94">
-      <c s="4" r="E94"/>
+      <c s="3" r="E94"/>
     </row>
     <row r="95">
-      <c s="4" r="E95"/>
+      <c s="3" r="E95"/>
     </row>
     <row r="96">
-      <c s="4" r="E96"/>
+      <c s="3" r="E96"/>
     </row>
     <row r="97">
-      <c s="4" r="E97"/>
+      <c s="3" r="E97"/>
     </row>
     <row r="98">
-      <c s="4" r="E98"/>
+      <c s="3" r="E98"/>
     </row>
     <row r="99">
-      <c s="4" r="E99"/>
+      <c s="3" r="E99"/>
     </row>
     <row r="100">
-      <c s="4" r="E100"/>
+      <c s="3" r="E100"/>
     </row>
     <row r="101">
-      <c s="4" r="E101"/>
+      <c s="3" r="E101"/>
     </row>
     <row r="102">
-      <c s="4" r="E102"/>
+      <c s="3" r="E102"/>
     </row>
     <row r="103">
-      <c s="4" r="E103"/>
+      <c s="3" r="E103"/>
     </row>
     <row r="104">
-      <c s="4" r="E104"/>
+      <c s="3" r="E104"/>
     </row>
     <row r="105">
-      <c s="4" r="E105"/>
+      <c s="3" r="E105"/>
     </row>
     <row r="106">
-      <c s="4" r="E106"/>
+      <c s="3" r="E106"/>
     </row>
     <row r="107">
-      <c s="4" r="E107"/>
+      <c s="3" r="E107"/>
     </row>
     <row r="108">
-      <c s="4" r="E108"/>
+      <c s="3" r="E108"/>
     </row>
     <row r="109">
-      <c s="4" r="E109"/>
+      <c s="3" r="E109"/>
     </row>
     <row r="110">
-      <c s="4" r="E110"/>
+      <c s="3" r="E110"/>
     </row>
     <row r="111">
-      <c s="4" r="E111"/>
+      <c s="3" r="E111"/>
     </row>
     <row r="112">
-      <c s="4" r="E112"/>
+      <c s="3" r="E112"/>
     </row>
     <row r="113">
-      <c s="4" r="E113"/>
+      <c s="3" r="E113"/>
     </row>
     <row r="114">
-      <c s="4" r="E114"/>
+      <c s="3" r="E114"/>
     </row>
     <row r="115">
-      <c s="4" r="E115"/>
+      <c s="3" r="E115"/>
     </row>
     <row r="116">
-      <c s="4" r="E116"/>
+      <c s="3" r="E116"/>
     </row>
     <row r="117">
-      <c s="4" r="E117"/>
+      <c s="3" r="E117"/>
     </row>
     <row r="118">
-      <c s="4" r="E118"/>
+      <c s="3" r="E118"/>
     </row>
     <row r="119">
-      <c s="4" r="E119"/>
+      <c s="3" r="E119"/>
     </row>
     <row r="120">
-      <c s="4" r="E120"/>
+      <c s="3" r="E120"/>
     </row>
     <row r="121">
-      <c s="4" r="E121"/>
+      <c s="3" r="E121"/>
     </row>
     <row r="122">
-      <c s="4" r="E122"/>
+      <c s="3" r="E122"/>
     </row>
     <row r="123">
-      <c s="4" r="E123"/>
+      <c s="3" r="E123"/>
     </row>
     <row r="124">
-      <c s="4" r="E124"/>
+      <c s="3" r="E124"/>
     </row>
     <row r="125">
-      <c s="4" r="E125"/>
+      <c s="3" r="E125"/>
     </row>
     <row r="126">
-      <c s="4" r="E126"/>
+      <c s="3" r="E126"/>
     </row>
     <row r="127">
-      <c s="4" r="E127"/>
+      <c s="3" r="E127"/>
     </row>
     <row r="128">
-      <c s="4" r="E128"/>
+      <c s="3" r="E128"/>
     </row>
     <row r="129">
-      <c s="4" r="E129"/>
+      <c s="3" r="E129"/>
     </row>
     <row r="130">
-      <c s="4" r="E130"/>
+      <c s="3" r="E130"/>
     </row>
     <row r="131">
-      <c s="4" r="E131"/>
+      <c s="3" r="E131"/>
     </row>
     <row r="132">
-      <c s="4" r="E132"/>
+      <c s="3" r="E132"/>
     </row>
     <row r="133">
-      <c s="4" r="E133"/>
+      <c s="3" r="E133"/>
     </row>
     <row r="134">
-      <c s="4" r="E134"/>
+      <c s="3" r="E134"/>
     </row>
     <row r="135">
-      <c s="4" r="E135"/>
+      <c s="3" r="E135"/>
     </row>
     <row r="136">
-      <c s="4" r="E136"/>
+      <c s="3" r="E136"/>
     </row>
     <row r="137">
-      <c s="4" r="E137"/>
+      <c s="3" r="E137"/>
     </row>
     <row r="138">
-      <c s="4" r="E138"/>
+      <c s="3" r="E138"/>
     </row>
     <row r="139">
-      <c s="4" r="E139"/>
+      <c s="3" r="E139"/>
     </row>
     <row r="140">
-      <c s="4" r="E140"/>
+      <c s="3" r="E140"/>
     </row>
     <row r="141">
-      <c s="4" r="E141"/>
+      <c s="3" r="E141"/>
     </row>
     <row r="142">
-      <c s="4" r="E142"/>
+      <c s="3" r="E142"/>
     </row>
     <row r="143">
-      <c s="4" r="E143"/>
+      <c s="3" r="E143"/>
     </row>
     <row r="144">
-      <c s="4" r="E144"/>
+      <c s="3" r="E144"/>
     </row>
     <row r="145">
-      <c s="4" r="E145"/>
+      <c s="3" r="E145"/>
     </row>
     <row r="146">
-      <c s="4" r="E146"/>
+      <c s="3" r="E146"/>
     </row>
     <row r="147">
-      <c s="4" r="E147"/>
+      <c s="3" r="E147"/>
     </row>
     <row r="148">
-      <c s="4" r="E148"/>
+      <c s="3" r="E148"/>
     </row>
     <row r="149">
-      <c s="4" r="E149"/>
+      <c s="3" r="E149"/>
     </row>
     <row r="150">
-      <c s="4" r="E150"/>
+      <c s="3" r="E150"/>
     </row>
     <row r="151">
-      <c s="4" r="E151"/>
+      <c s="3" r="E151"/>
     </row>
     <row r="152">
-      <c s="4" r="E152"/>
+      <c s="3" r="E152"/>
     </row>
     <row r="153">
-      <c s="4" r="E153"/>
+      <c s="3" r="E153"/>
     </row>
     <row r="154">
-      <c s="4" r="E154"/>
+      <c s="3" r="E154"/>
     </row>
     <row r="155">
-      <c s="4" r="E155"/>
+      <c s="3" r="E155"/>
     </row>
     <row r="156">
-      <c s="4" r="E156"/>
+      <c s="3" r="E156"/>
     </row>
     <row r="157">
-      <c s="4" r="E157"/>
+      <c s="3" r="E157"/>
     </row>
     <row r="158">
-      <c s="4" r="E158"/>
+      <c s="3" r="E158"/>
     </row>
     <row r="159">
-      <c s="4" r="E159"/>
+      <c s="3" r="E159"/>
     </row>
     <row r="160">
-      <c s="4" r="E160"/>
+      <c s="3" r="E160"/>
     </row>
     <row r="161">
-      <c s="4" r="E161"/>
+      <c s="3" r="E161"/>
     </row>
     <row r="162">
-      <c s="4" r="E162"/>
+      <c s="3" r="E162"/>
     </row>
     <row r="163">
-      <c s="4" r="E163"/>
+      <c s="3" r="E163"/>
     </row>
     <row r="164">
-      <c s="4" r="E164"/>
+      <c s="3" r="E164"/>
     </row>
     <row r="165">
-      <c s="4" r="E165"/>
+      <c s="3" r="E165"/>
     </row>
     <row r="166">
-      <c s="4" r="E166"/>
+      <c s="3" r="E166"/>
     </row>
     <row r="167">
-      <c s="4" r="E167"/>
+      <c s="3" r="E167"/>
     </row>
     <row r="168">
-      <c s="4" r="E168"/>
+      <c s="3" r="E168"/>
     </row>
     <row r="169">
-      <c s="4" r="E169"/>
+      <c s="3" r="E169"/>
     </row>
     <row r="170">
-      <c s="4" r="E170"/>
+      <c s="3" r="E170"/>
     </row>
     <row r="171">
-      <c s="4" r="E171"/>
+      <c s="3" r="E171"/>
     </row>
     <row r="172">
-      <c s="4" r="E172"/>
+      <c s="3" r="E172"/>
     </row>
     <row r="173">
-      <c s="4" r="E173"/>
+      <c s="3" r="E173"/>
     </row>
     <row r="174">
-      <c s="4" r="E174"/>
+      <c s="3" r="E174"/>
     </row>
     <row r="175">
-      <c s="4" r="E175"/>
+      <c s="3" r="E175"/>
     </row>
     <row r="176">
-      <c s="4" r="E176"/>
+      <c s="3" r="E176"/>
     </row>
     <row r="177">
-      <c s="4" r="E177"/>
+      <c s="3" r="E177"/>
     </row>
     <row r="178">
-      <c s="4" r="E178"/>
+      <c s="3" r="E178"/>
     </row>
     <row r="179">
-      <c s="4" r="E179"/>
+      <c s="3" r="E179"/>
     </row>
     <row r="180">
-      <c s="4" r="E180"/>
+      <c s="3" r="E180"/>
     </row>
     <row r="181">
-      <c s="4" r="E181"/>
+      <c s="3" r="E181"/>
     </row>
     <row r="182">
-      <c s="4" r="E182"/>
+      <c s="3" r="E182"/>
     </row>
     <row r="183">
-      <c s="4" r="E183"/>
+      <c s="3" r="E183"/>
     </row>
     <row r="184">
-      <c s="4" r="E184"/>
+      <c s="3" r="E184"/>
     </row>
     <row r="185">
-      <c s="4" r="E185"/>
+      <c s="3" r="E185"/>
     </row>
     <row r="186">
-      <c s="4" r="E186"/>
+      <c s="3" r="E186"/>
     </row>
     <row r="187">
-      <c s="4" r="E187"/>
+      <c s="3" r="E187"/>
     </row>
     <row r="188">
-      <c s="4" r="E188"/>
+      <c s="3" r="E188"/>
     </row>
     <row r="189">
-      <c s="4" r="E189"/>
+      <c s="3" r="E189"/>
     </row>
     <row r="190">
-      <c s="4" r="E190"/>
+      <c s="3" r="E190"/>
     </row>
     <row r="191">
-      <c s="4" r="E191"/>
+      <c s="3" r="E191"/>
     </row>
     <row r="192">
-      <c s="4" r="E192"/>
+      <c s="3" r="E192"/>
     </row>
     <row r="193">
-      <c s="4" r="E193"/>
+      <c s="3" r="E193"/>
     </row>
     <row r="194">
-      <c s="4" r="E194"/>
+      <c s="3" r="E194"/>
     </row>
     <row r="195">
-      <c s="4" r="E195"/>
+      <c s="3" r="E195"/>
     </row>
     <row r="196">
-      <c s="4" r="E196"/>
+      <c s="3" r="E196"/>
     </row>
     <row r="197">
-      <c s="4" r="E197"/>
+      <c s="3" r="E197"/>
     </row>
     <row r="198">
-      <c s="4" r="E198"/>
+      <c s="3" r="E198"/>
     </row>
     <row r="199">
-      <c s="4" r="E199"/>
+      <c s="3" r="E199"/>
     </row>
     <row r="200">
-      <c s="4" r="E200"/>
+      <c s="3" r="E200"/>
     </row>
     <row r="201">
-      <c s="4" r="E201"/>
+      <c s="3" r="E201"/>
     </row>
     <row r="202">
-      <c s="4" r="E202"/>
+      <c s="3" r="E202"/>
     </row>
     <row r="203">
-      <c s="4" r="E203"/>
+      <c s="3" r="E203"/>
     </row>
     <row r="204">
-      <c s="4" r="E204"/>
+      <c s="3" r="E204"/>
     </row>
     <row r="205">
-      <c s="4" r="E205"/>
+      <c s="3" r="E205"/>
     </row>
     <row r="206">
-      <c s="4" r="E206"/>
+      <c s="3" r="E206"/>
     </row>
     <row r="207">
-      <c s="4" r="E207"/>
+      <c s="3" r="E207"/>
     </row>
     <row r="208">
-      <c s="4" r="E208"/>
+      <c s="3" r="E208"/>
     </row>
     <row r="209">
-      <c s="4" r="E209"/>
+      <c s="3" r="E209"/>
     </row>
     <row r="210">
-      <c s="4" r="E210"/>
+      <c s="3" r="E210"/>
     </row>
     <row r="211">
-      <c s="4" r="E211"/>
+      <c s="3" r="E211"/>
     </row>
     <row r="212">
-      <c s="4" r="E212"/>
+      <c s="3" r="E212"/>
     </row>
     <row r="213">
-      <c s="4" r="E213"/>
+      <c s="3" r="E213"/>
     </row>
     <row r="214">
-      <c s="4" r="E214"/>
+      <c s="3" r="E214"/>
     </row>
     <row r="215">
-      <c s="4" r="E215"/>
+      <c s="3" r="E215"/>
     </row>
     <row r="216">
-      <c s="4" r="E216"/>
+      <c s="3" r="E216"/>
     </row>
     <row r="217">
-      <c s="4" r="E217"/>
+      <c s="3" r="E217"/>
     </row>
     <row r="218">
-      <c s="4" r="E218"/>
+      <c s="3" r="E218"/>
     </row>
     <row r="219">
-      <c s="4" r="E219"/>
+      <c s="3" r="E219"/>
     </row>
     <row r="220">
-      <c s="4" r="E220"/>
+      <c s="3" r="E220"/>
     </row>
     <row r="221">
-      <c s="4" r="E221"/>
+      <c s="3" r="E221"/>
     </row>
     <row r="222">
-      <c s="4" r="E222"/>
+      <c s="3" r="E222"/>
     </row>
     <row r="223">
-      <c s="4" r="E223"/>
+      <c s="3" r="E223"/>
     </row>
     <row r="224">
-      <c s="4" r="E224"/>
+      <c s="3" r="E224"/>
     </row>
     <row r="225">
-      <c s="4" r="E225"/>
+      <c s="3" r="E225"/>
     </row>
     <row r="226">
-      <c s="4" r="E226"/>
+      <c s="3" r="E226"/>
     </row>
     <row r="227">
-      <c s="4" r="E227"/>
+      <c s="3" r="E227"/>
     </row>
     <row r="228">
-      <c s="4" r="E228"/>
+      <c s="3" r="E228"/>
     </row>
     <row r="229">
-      <c s="4" r="E229"/>
+      <c s="3" r="E229"/>
     </row>
     <row r="230">
-      <c s="4" r="E230"/>
+      <c s="3" r="E230"/>
     </row>
     <row r="231">
-      <c s="4" r="E231"/>
+      <c s="3" r="E231"/>
     </row>
     <row r="232">
-      <c s="4" r="E232"/>
+      <c s="3" r="E232"/>
     </row>
     <row r="233">
-      <c s="4" r="E233"/>
+      <c s="3" r="E233"/>
     </row>
     <row r="234">
-      <c s="4" r="E234"/>
+      <c s="3" r="E234"/>
     </row>
     <row r="235">
-      <c s="4" r="E235"/>
+      <c s="3" r="E235"/>
     </row>
     <row r="236">
-      <c s="4" r="E236"/>
+      <c s="3" r="E236"/>
     </row>
     <row r="237">
-      <c s="4" r="E237"/>
+      <c s="3" r="E237"/>
     </row>
     <row r="238">
-      <c s="4" r="E238"/>
+      <c s="3" r="E238"/>
     </row>
     <row r="239">
-      <c s="4" r="E239"/>
+      <c s="3" r="E239"/>
     </row>
     <row r="240">
-      <c s="4" r="E240"/>
+      <c s="3" r="E240"/>
     </row>
     <row r="241">
-      <c s="4" r="E241"/>
+      <c s="3" r="E241"/>
     </row>
     <row r="242">
-      <c s="4" r="E242"/>
+      <c s="3" r="E242"/>
     </row>
     <row r="243">
-      <c s="4" r="E243"/>
+      <c s="3" r="E243"/>
     </row>
     <row r="244">
-      <c s="4" r="E244"/>
+      <c s="3" r="E244"/>
     </row>
     <row r="245">
-      <c s="4" r="E245"/>
+      <c s="3" r="E245"/>
     </row>
     <row r="246">
-      <c s="4" r="E246"/>
+      <c s="3" r="E246"/>
     </row>
     <row r="247">
-      <c s="4" r="E247"/>
+      <c s="3" r="E247"/>
     </row>
     <row r="248">
-      <c s="4" r="E248"/>
+      <c s="3" r="E248"/>
     </row>
     <row r="249">
-      <c s="4" r="E249"/>
+      <c s="3" r="E249"/>
     </row>
     <row r="250">
-      <c s="4" r="E250"/>
+      <c s="3" r="E250"/>
     </row>
     <row r="251">
-      <c s="4" r="E251"/>
+      <c s="3" r="E251"/>
     </row>
     <row r="252">
-      <c s="4" r="E252"/>
+      <c s="3" r="E252"/>
     </row>
     <row r="253">
-      <c s="4" r="E253"/>
+      <c s="3" r="E253"/>
     </row>
     <row r="254">
-      <c s="4" r="E254"/>
+      <c s="3" r="E254"/>
     </row>
     <row r="255">
-      <c s="4" r="E255"/>
+      <c s="3" r="E255"/>
     </row>
     <row r="256">
-      <c s="4" r="E256"/>
+      <c s="3" r="E256"/>
     </row>
     <row r="257">
-      <c s="4" r="E257"/>
+      <c s="3" r="E257"/>
     </row>
     <row r="258">
-      <c s="4" r="E258"/>
+      <c s="3" r="E258"/>
     </row>
     <row r="259">
-      <c s="4" r="E259"/>
+      <c s="3" r="E259"/>
     </row>
     <row r="260">
-      <c s="4" r="E260"/>
+      <c s="3" r="E260"/>
     </row>
     <row r="261">
-      <c s="4" r="E261"/>
+      <c s="3" r="E261"/>
     </row>
     <row r="262">
-      <c s="4" r="E262"/>
+      <c s="3" r="E262"/>
     </row>
     <row r="263">
-      <c s="4" r="E263"/>
+      <c s="3" r="E263"/>
     </row>
     <row r="264">
-      <c s="4" r="E264"/>
+      <c s="3" r="E264"/>
     </row>
     <row r="265">
-      <c s="4" r="E265"/>
+      <c s="3" r="E265"/>
     </row>
     <row r="266">
-      <c s="4" r="E266"/>
+      <c s="3" r="E266"/>
     </row>
     <row r="267">
-      <c s="4" r="E267"/>
+      <c s="3" r="E267"/>
     </row>
     <row r="268">
-      <c s="4" r="E268"/>
+      <c s="3" r="E268"/>
     </row>
     <row r="269">
-      <c s="4" r="E269"/>
+      <c s="3" r="E269"/>
     </row>
     <row r="270">
-      <c s="4" r="E270"/>
+      <c s="3" r="E270"/>
     </row>
     <row r="271">
-      <c s="4" r="E271"/>
+      <c s="3" r="E271"/>
     </row>
     <row r="272">
-      <c s="4" r="E272"/>
+      <c s="3" r="E272"/>
     </row>
     <row r="273">
-      <c s="4" r="E273"/>
+      <c s="3" r="E273"/>
     </row>
     <row r="274">
-      <c s="4" r="E274"/>
+      <c s="3" r="E274"/>
     </row>
     <row r="275">
-      <c s="4" r="E275"/>
+      <c s="3" r="E275"/>
     </row>
     <row r="276">
-      <c s="4" r="E276"/>
+      <c s="3" r="E276"/>
     </row>
     <row r="277">
-      <c s="4" r="E277"/>
+      <c s="3" r="E277"/>
     </row>
     <row r="278">
-      <c s="4" r="E278"/>
+      <c s="3" r="E278"/>
     </row>
     <row r="279">
-      <c s="4" r="E279"/>
+      <c s="3" r="E279"/>
     </row>
     <row r="280">
-      <c s="4" r="E280"/>
+      <c s="3" r="E280"/>
     </row>
     <row r="281">
-      <c s="4" r="E281"/>
+      <c s="3" r="E281"/>
     </row>
     <row r="282">
-      <c s="4" r="E282"/>
+      <c s="3" r="E282"/>
     </row>
     <row r="283">
-      <c s="4" r="E283"/>
+      <c s="3" r="E283"/>
     </row>
     <row r="284">
-      <c s="4" r="E284"/>
+      <c s="3" r="E284"/>
     </row>
     <row r="285">
-      <c s="4" r="E285"/>
+      <c s="3" r="E285"/>
     </row>
     <row r="286">
-      <c s="4" r="E286"/>
+      <c s="3" r="E286"/>
     </row>
     <row r="287">
-      <c s="4" r="E287"/>
+      <c s="3" r="E287"/>
     </row>
     <row r="288">
-      <c s="4" r="E288"/>
+      <c s="3" r="E288"/>
     </row>
     <row r="289">
-      <c s="4" r="E289"/>
+      <c s="3" r="E289"/>
     </row>
     <row r="290">
-      <c s="4" r="E290"/>
+      <c s="3" r="E290"/>
     </row>
     <row r="291">
-      <c s="4" r="E291"/>
+      <c s="3" r="E291"/>
     </row>
     <row r="292">
-      <c s="4" r="E292"/>
+      <c s="3" r="E292"/>
     </row>
     <row r="293">
-      <c s="4" r="E293"/>
+      <c s="3" r="E293"/>
     </row>
     <row r="294">
-      <c s="4" r="E294"/>
+      <c s="3" r="E294"/>
     </row>
     <row r="295">
-      <c s="4" r="E295"/>
+      <c s="3" r="E295"/>
     </row>
     <row r="296">
-      <c s="4" r="E296"/>
+      <c s="3" r="E296"/>
     </row>
     <row r="297">
-      <c s="4" r="E297"/>
+      <c s="3" r="E297"/>
     </row>
     <row r="298">
-      <c s="4" r="E298"/>
+      <c s="3" r="E298"/>
     </row>
     <row r="299">
-      <c s="4" r="E299"/>
+      <c s="3" r="E299"/>
     </row>
     <row r="300">
-      <c s="4" r="E300"/>
+      <c s="3" r="E300"/>
     </row>
     <row r="301">
-      <c s="4" r="E301"/>
+      <c s="3" r="E301"/>
     </row>
     <row r="302">
-      <c s="4" r="E302"/>
+      <c s="3" r="E302"/>
     </row>
     <row r="303">
-      <c s="4" r="E303"/>
+      <c s="3" r="E303"/>
     </row>
     <row r="304">
-      <c s="4" r="E304"/>
+      <c s="3" r="E304"/>
     </row>
     <row r="305">
-      <c s="4" r="E305"/>
+      <c s="3" r="E305"/>
     </row>
     <row r="306">
-      <c s="4" r="E306"/>
+      <c s="3" r="E306"/>
     </row>
     <row r="307">
-      <c s="4" r="E307"/>
+      <c s="3" r="E307"/>
     </row>
     <row r="308">
-      <c s="4" r="E308"/>
+      <c s="3" r="E308"/>
     </row>
     <row r="309">
-      <c s="4" r="E309"/>
+      <c s="3" r="E309"/>
     </row>
     <row r="310">
-      <c s="4" r="E310"/>
+      <c s="3" r="E310"/>
     </row>
     <row r="311">
-      <c s="4" r="E311"/>
+      <c s="3" r="E311"/>
     </row>
     <row r="312">
-      <c s="4" r="E312"/>
+      <c s="3" r="E312"/>
     </row>
     <row r="313">
-      <c s="4" r="E313"/>
+      <c s="3" r="E313"/>
     </row>
     <row r="314">
-      <c s="4" r="E314"/>
+      <c s="3" r="E314"/>
     </row>
     <row r="315">
-      <c s="4" r="E315"/>
+      <c s="3" r="E315"/>
     </row>
     <row r="316">
-      <c s="4" r="E316"/>
+      <c s="3" r="E316"/>
     </row>
     <row r="317">
-      <c s="4" r="E317"/>
+      <c s="3" r="E317"/>
     </row>
     <row r="318">
-      <c s="4" r="E318"/>
+      <c s="3" r="E318"/>
     </row>
     <row r="319">
-      <c s="4" r="E319"/>
+      <c s="3" r="E319"/>
     </row>
     <row r="320">
-      <c s="4" r="E320"/>
+      <c s="3" r="E320"/>
     </row>
     <row r="321">
-      <c s="4" r="E321"/>
+      <c s="3" r="E321"/>
     </row>
     <row r="322">
-      <c s="4" r="E322"/>
+      <c s="3" r="E322"/>
     </row>
     <row r="323">
-      <c s="4" r="E323"/>
+      <c s="3" r="E323"/>
     </row>
     <row r="324">
-      <c s="4" r="E324"/>
+      <c s="3" r="E324"/>
     </row>
     <row r="325">
-      <c s="4" r="E325"/>
+      <c s="3" r="E325"/>
     </row>
     <row r="326">
-      <c s="4" r="E326"/>
+      <c s="3" r="E326"/>
     </row>
     <row r="327">
-      <c s="4" r="E327"/>
+      <c s="3" r="E327"/>
     </row>
     <row r="328">
-      <c s="4" r="E328"/>
+      <c s="3" r="E328"/>
     </row>
     <row r="329">
-      <c s="4" r="E329"/>
+      <c s="3" r="E329"/>
     </row>
     <row r="330">
-      <c s="4" r="E330"/>
+      <c s="3" r="E330"/>
     </row>
     <row r="331">
-      <c s="4" r="E331"/>
+      <c s="3" r="E331"/>
     </row>
     <row r="332">
-      <c s="4" r="E332"/>
+      <c s="3" r="E332"/>
     </row>
     <row r="333">
-      <c s="4" r="E333"/>
+      <c s="3" r="E333"/>
     </row>
     <row r="334">
-      <c s="4" r="E334"/>
+      <c s="3" r="E334"/>
     </row>
     <row r="335">
-      <c s="4" r="E335"/>
+      <c s="3" r="E335"/>
     </row>
     <row r="336">
-      <c s="4" r="E336"/>
+      <c s="3" r="E336"/>
     </row>
     <row r="337">
-      <c s="4" r="E337"/>
+      <c s="3" r="E337"/>
     </row>
     <row r="338">
-      <c s="4" r="E338"/>
+      <c s="3" r="E338"/>
     </row>
     <row r="339">
-      <c s="4" r="E339"/>
+      <c s="3" r="E339"/>
     </row>
     <row r="340">
-      <c s="4" r="E340"/>
+      <c s="3" r="E340"/>
     </row>
     <row r="341">
-      <c s="4" r="E341"/>
+      <c s="3" r="E341"/>
     </row>
     <row r="342">
-      <c s="4" r="E342"/>
+      <c s="3" r="E342"/>
     </row>
     <row r="343">
-      <c s="4" r="E343"/>
+      <c s="3" r="E343"/>
     </row>
     <row r="344">
-      <c s="4" r="E344"/>
+      <c s="3" r="E344"/>
     </row>
     <row r="345">
-      <c s="4" r="E345"/>
+      <c s="3" r="E345"/>
     </row>
     <row r="346">
-      <c s="4" r="E346"/>
+      <c s="3" r="E346"/>
     </row>
     <row r="347">
-      <c s="4" r="E347"/>
+      <c s="3" r="E347"/>
     </row>
     <row r="348">
-      <c s="4" r="E348"/>
+      <c s="3" r="E348"/>
     </row>
     <row r="349">
-      <c s="4" r="E349"/>
+      <c s="3" r="E349"/>
     </row>
     <row r="350">
-      <c s="4" r="E350"/>
+      <c s="3" r="E350"/>
     </row>
     <row r="351">
-      <c s="4" r="E351"/>
+      <c s="3" r="E351"/>
     </row>
     <row r="352">
-      <c s="4" r="E352"/>
+      <c s="3" r="E352"/>
     </row>
     <row r="353">
-      <c s="4" r="E353"/>
+      <c s="3" r="E353"/>
     </row>
     <row r="354">
-      <c s="4" r="E354"/>
+      <c s="3" r="E354"/>
     </row>
     <row r="355">
-      <c s="4" r="E355"/>
+      <c s="3" r="E355"/>
     </row>
     <row r="356">
-      <c s="4" r="E356"/>
+      <c s="3" r="E356"/>
     </row>
     <row r="357">
-      <c s="4" r="E357"/>
+      <c s="3" r="E357"/>
     </row>
     <row r="358">
-      <c s="4" r="E358"/>
+      <c s="3" r="E358"/>
     </row>
     <row r="359">
-      <c s="4" r="E359"/>
+      <c s="3" r="E359"/>
     </row>
     <row r="360">
-      <c s="4" r="E360"/>
+      <c s="3" r="E360"/>
     </row>
     <row r="361">
-      <c s="4" r="E361"/>
+      <c s="3" r="E361"/>
     </row>
     <row r="362">
-      <c s="4" r="E362"/>
+      <c s="3" r="E362"/>
     </row>
     <row r="363">
-      <c s="4" r="E363"/>
+      <c s="3" r="E363"/>
     </row>
     <row r="364">
-      <c s="4" r="E364"/>
+      <c s="3" r="E364"/>
     </row>
     <row r="365">
-      <c s="4" r="E365"/>
+      <c s="3" r="E365"/>
     </row>
     <row r="366">
-      <c s="4" r="E366"/>
+      <c s="3" r="E366"/>
     </row>
     <row r="367">
-      <c s="4" r="E367"/>
+      <c s="3" r="E367"/>
     </row>
     <row r="368">
-      <c s="4" r="E368"/>
+      <c s="3" r="E368"/>
     </row>
     <row r="369">
-      <c s="4" r="E369"/>
+      <c s="3" r="E369"/>
     </row>
     <row r="370">
-      <c s="4" r="E370"/>
+      <c s="3" r="E370"/>
     </row>
     <row r="371">
-      <c s="4" r="E371"/>
+      <c s="3" r="E371"/>
     </row>
     <row r="372">
-      <c s="4" r="E372"/>
+      <c s="3" r="E372"/>
     </row>
     <row r="373">
-      <c s="4" r="E373"/>
+      <c s="3" r="E373"/>
     </row>
     <row r="374">
-      <c s="4" r="E374"/>
+      <c s="3" r="E374"/>
     </row>
     <row r="375">
-      <c s="4" r="E375"/>
+      <c s="3" r="E375"/>
     </row>
     <row r="376">
-      <c s="4" r="E376"/>
+      <c s="3" r="E376"/>
     </row>
     <row r="377">
-      <c s="4" r="E377"/>
+      <c s="3" r="E377"/>
     </row>
     <row r="378">
-      <c s="4" r="E378"/>
+      <c s="3" r="E378"/>
     </row>
     <row r="379">
-      <c s="4" r="E379"/>
+      <c s="3" r="E379"/>
     </row>
     <row r="380">
-      <c s="4" r="E380"/>
+      <c s="3" r="E380"/>
     </row>
     <row r="381">
-      <c s="4" r="E381"/>
+      <c s="3" r="E381"/>
     </row>
     <row r="382">
-      <c s="4" r="E382"/>
+      <c s="3" r="E382"/>
     </row>
     <row r="383">
-      <c s="4" r="E383"/>
+      <c s="3" r="E383"/>
     </row>
     <row r="384">
-      <c s="4" r="E384"/>
+      <c s="3" r="E384"/>
     </row>
     <row r="385">
-      <c s="4" r="E385"/>
+      <c s="3" r="E385"/>
     </row>
     <row r="386">
-      <c s="4" r="E386"/>
+      <c s="3" r="E386"/>
     </row>
     <row r="387">
-      <c s="4" r="E387"/>
+      <c s="3" r="E387"/>
     </row>
     <row r="388">
-      <c s="4" r="E388"/>
+      <c s="3" r="E388"/>
     </row>
     <row r="389">
-      <c s="4" r="E389"/>
+      <c s="3" r="E389"/>
     </row>
     <row r="390">
-      <c s="4" r="E390"/>
+      <c s="3" r="E390"/>
     </row>
     <row r="391">
-      <c s="4" r="E391"/>
+      <c s="3" r="E391"/>
     </row>
     <row r="392">
-      <c s="4" r="E392"/>
+      <c s="3" r="E392"/>
     </row>
     <row r="393">
-      <c s="4" r="E393"/>
+      <c s="3" r="E393"/>
     </row>
     <row r="394">
-      <c s="4" r="E394"/>
+      <c s="3" r="E394"/>
     </row>
     <row r="395">
-      <c s="4" r="E395"/>
+      <c s="3" r="E395"/>
     </row>
     <row r="396">
-      <c s="4" r="E396"/>
+      <c s="3" r="E396"/>
     </row>
     <row r="397">
-      <c s="4" r="E397"/>
+      <c s="3" r="E397"/>
     </row>
     <row r="398">
-      <c s="4" r="E398"/>
+      <c s="3" r="E398"/>
     </row>
     <row r="399">
-      <c s="4" r="E399"/>
+      <c s="3" r="E399"/>
     </row>
     <row r="400">
-      <c s="4" r="E400"/>
+      <c s="3" r="E400"/>
     </row>
     <row r="401">
-      <c s="4" r="E401"/>
+      <c s="3" r="E401"/>
     </row>
     <row r="402">
-      <c s="4" r="E402"/>
+      <c s="3" r="E402"/>
     </row>
     <row r="403">
-      <c s="4" r="E403"/>
+      <c s="3" r="E403"/>
     </row>
     <row r="404">
-      <c s="4" r="E404"/>
+      <c s="3" r="E404"/>
     </row>
     <row r="405">
-      <c s="4" r="E405"/>
+      <c s="3" r="E405"/>
     </row>
     <row r="406">
-      <c s="4" r="E406"/>
+      <c s="3" r="E406"/>
     </row>
     <row r="407">
-      <c s="4" r="E407"/>
+      <c s="3" r="E407"/>
     </row>
     <row r="408">
-      <c s="4" r="E408"/>
+      <c s="3" r="E408"/>
     </row>
     <row r="409">
-      <c s="4" r="E409"/>
+      <c s="3" r="E409"/>
     </row>
     <row r="410">
-      <c s="4" r="E410"/>
+      <c s="3" r="E410"/>
     </row>
     <row r="411">
-      <c s="4" r="E411"/>
+      <c s="3" r="E411"/>
     </row>
     <row r="412">
-      <c s="4" r="E412"/>
+      <c s="3" r="E412"/>
     </row>
     <row r="413">
-      <c s="4" r="E413"/>
+      <c s="3" r="E413"/>
     </row>
     <row r="414">
-      <c s="4" r="E414"/>
+      <c s="3" r="E414"/>
     </row>
     <row r="415">
-      <c s="4" r="E415"/>
+      <c s="3" r="E415"/>
     </row>
     <row r="416">
-      <c s="4" r="E416"/>
+      <c s="3" r="E416"/>
     </row>
     <row r="417">
-      <c s="4" r="E417"/>
+      <c s="3" r="E417"/>
     </row>
     <row r="418">
-      <c s="4" r="E418"/>
+      <c s="3" r="E418"/>
     </row>
     <row r="419">
-      <c s="4" r="E419"/>
+      <c s="3" r="E419"/>
     </row>
     <row r="420">
-      <c s="4" r="E420"/>
+      <c s="3" r="E420"/>
     </row>
     <row r="421">
-      <c s="4" r="E421"/>
+      <c s="3" r="E421"/>
     </row>
     <row r="422">
-      <c s="4" r="E422"/>
+      <c s="3" r="E422"/>
     </row>
     <row r="423">
-      <c s="4" r="E423"/>
+      <c s="3" r="E423"/>
     </row>
     <row r="424">
-      <c s="4" r="E424"/>
+      <c s="3" r="E424"/>
     </row>
     <row r="425">
-      <c s="4" r="E425"/>
+      <c s="3" r="E425"/>
     </row>
     <row r="426">
-      <c s="4" r="E426"/>
+      <c s="3" r="E426"/>
     </row>
     <row r="427">
-      <c s="4" r="E427"/>
+      <c s="3" r="E427"/>
     </row>
     <row r="428">
-      <c s="4" r="E428"/>
+      <c s="3" r="E428"/>
     </row>
     <row r="429">
-      <c s="4" r="E429"/>
+      <c s="3" r="E429"/>
     </row>
     <row r="430">
-      <c s="4" r="E430"/>
+      <c s="3" r="E430"/>
     </row>
     <row r="431">
-      <c s="4" r="E431"/>
+      <c s="3" r="E431"/>
     </row>
     <row r="432">
-      <c s="4" r="E432"/>
+      <c s="3" r="E432"/>
     </row>
     <row r="433">
-      <c s="4" r="E433"/>
+      <c s="3" r="E433"/>
     </row>
     <row r="434">
-      <c s="4" r="E434"/>
+      <c s="3" r="E434"/>
     </row>
     <row r="435">
-      <c s="4" r="E435"/>
+      <c s="3" r="E435"/>
     </row>
     <row r="436">
-      <c s="4" r="E436"/>
+      <c s="3" r="E436"/>
     </row>
     <row r="437">
-      <c s="4" r="E437"/>
+      <c s="3" r="E437"/>
     </row>
     <row r="438">
-      <c s="4" r="E438"/>
+      <c s="3" r="E438"/>
     </row>
     <row r="439">
-      <c s="4" r="E439"/>
+      <c s="3" r="E439"/>
     </row>
     <row r="440">
-      <c s="4" r="E440"/>
+      <c s="3" r="E440"/>
     </row>
     <row r="441">
-      <c s="4" r="E441"/>
+      <c s="3" r="E441"/>
     </row>
     <row r="442">
-      <c s="4" r="E442"/>
+      <c s="3" r="E442"/>
     </row>
     <row r="443">
-      <c s="4" r="E443"/>
+      <c s="3" r="E443"/>
     </row>
     <row r="444">
-      <c s="4" r="E444"/>
+      <c s="3" r="E444"/>
     </row>
     <row r="445">
-      <c s="4" r="E445"/>
+      <c s="3" r="E445"/>
     </row>
     <row r="446">
-      <c s="4" r="E446"/>
+      <c s="3" r="E446"/>
     </row>
     <row r="447">
-      <c s="4" r="E447"/>
+      <c s="3" r="E447"/>
     </row>
     <row r="448">
-      <c s="4" r="E448"/>
+      <c s="3" r="E448"/>
     </row>
     <row r="449">
-      <c s="4" r="E449"/>
+      <c s="3" r="E449"/>
     </row>
     <row r="450">
-      <c s="4" r="E450"/>
+      <c s="3" r="E450"/>
     </row>
     <row r="451">
-      <c s="4" r="E451"/>
+      <c s="3" r="E451"/>
     </row>
     <row r="452">
-      <c s="4" r="E452"/>
+      <c s="3" r="E452"/>
     </row>
     <row r="453">
-      <c s="4" r="E453"/>
+      <c s="3" r="E453"/>
     </row>
     <row r="454">
-      <c s="4" r="E454"/>
+      <c s="3" r="E454"/>
     </row>
     <row r="455">
-      <c s="4" r="E455"/>
+      <c s="3" r="E455"/>
     </row>
     <row r="456">
-      <c s="4" r="E456"/>
+      <c s="3" r="E456"/>
     </row>
     <row r="457">
-      <c s="4" r="E457"/>
+      <c s="3" r="E457"/>
     </row>
     <row r="458">
-      <c s="4" r="E458"/>
+      <c s="3" r="E458"/>
     </row>
     <row r="459">
-      <c s="4" r="E459"/>
+      <c s="3" r="E459"/>
     </row>
     <row r="460">
-      <c s="4" r="E460"/>
+      <c s="3" r="E460"/>
     </row>
     <row r="461">
-      <c s="4" r="E461"/>
+      <c s="3" r="E461"/>
     </row>
     <row r="462">
-      <c s="4" r="E462"/>
+      <c s="3" r="E462"/>
     </row>
     <row r="463">
-      <c s="4" r="E463"/>
+      <c s="3" r="E463"/>
     </row>
     <row r="464">
-      <c s="4" r="E464"/>
+      <c s="3" r="E464"/>
     </row>
     <row r="465">
-      <c s="4" r="E465"/>
+      <c s="3" r="E465"/>
     </row>
     <row r="466">
-      <c s="4" r="E466"/>
+      <c s="3" r="E466"/>
     </row>
     <row r="467">
-      <c s="4" r="E467"/>
+      <c s="3" r="E467"/>
     </row>
     <row r="468">
-      <c s="4" r="E468"/>
+      <c s="3" r="E468"/>
     </row>
     <row r="469">
-      <c s="4" r="E469"/>
+      <c s="3" r="E469"/>
     </row>
     <row r="470">
-      <c s="4" r="E470"/>
+      <c s="3" r="E470"/>
     </row>
     <row r="471">
-      <c s="4" r="E471"/>
+      <c s="3" r="E471"/>
     </row>
     <row r="472">
-      <c s="4" r="E472"/>
+      <c s="3" r="E472"/>
     </row>
     <row r="473">
-      <c s="4" r="E473"/>
+      <c s="3" r="E473"/>
     </row>
     <row r="474">
-      <c s="4" r="E474"/>
+      <c s="3" r="E474"/>
     </row>
     <row r="475">
-      <c s="4" r="E475"/>
+      <c s="3" r="E475"/>
     </row>
     <row r="476">
-      <c s="4" r="E476"/>
+      <c s="3" r="E476"/>
     </row>
     <row r="477">
-      <c s="4" r="E477"/>
+      <c s="3" r="E477"/>
     </row>
     <row r="478">
-      <c s="4" r="E478"/>
+      <c s="3" r="E478"/>
     </row>
     <row r="479">
-      <c s="4" r="E479"/>
+      <c s="3" r="E479"/>
     </row>
     <row r="480">
-      <c s="4" r="E480"/>
+      <c s="3" r="E480"/>
     </row>
     <row r="481">
-      <c s="4" r="E481"/>
+      <c s="3" r="E481"/>
     </row>
     <row r="482">
-      <c s="4" r="E482"/>
+      <c s="3" r="E482"/>
     </row>
     <row r="483">
-      <c s="4" r="E483"/>
+      <c s="3" r="E483"/>
     </row>
     <row r="484">
-      <c s="4" r="E484"/>
+      <c s="3" r="E484"/>
     </row>
     <row r="485">
-      <c s="4" r="E485"/>
+      <c s="3" r="E485"/>
     </row>
     <row r="486">
-      <c s="4" r="E486"/>
+      <c s="3" r="E486"/>
     </row>
     <row r="487">
-      <c s="4" r="E487"/>
+      <c s="3" r="E487"/>
     </row>
     <row r="488">
-      <c s="4" r="E488"/>
+      <c s="3" r="E488"/>
     </row>
     <row r="489">
-      <c s="4" r="E489"/>
+      <c s="3" r="E489"/>
     </row>
     <row r="490">
-      <c s="4" r="E490"/>
+      <c s="3" r="E490"/>
     </row>
     <row r="491">
-      <c s="4" r="E491"/>
+      <c s="3" r="E491"/>
     </row>
     <row r="492">
-      <c s="4" r="E492"/>
+      <c s="3" r="E492"/>
     </row>
     <row r="493">
-      <c s="4" r="E493"/>
+      <c s="3" r="E493"/>
     </row>
     <row r="494">
-      <c s="4" r="E494"/>
+      <c s="3" r="E494"/>
     </row>
     <row r="495">
-      <c s="4" r="E495"/>
+      <c s="3" r="E495"/>
     </row>
     <row r="496">
-      <c s="4" r="E496"/>
+      <c s="3" r="E496"/>
     </row>
     <row r="497">
-      <c s="4" r="E497"/>
+      <c s="3" r="E497"/>
     </row>
     <row r="498">
-      <c s="4" r="E498"/>
+      <c s="3" r="E498"/>
     </row>
     <row r="499">
-      <c s="4" r="E499"/>
+      <c s="3" r="E499"/>
     </row>
     <row r="500">
-      <c s="4" r="E500"/>
+      <c s="3" r="E500"/>
     </row>
     <row r="501">
-      <c s="4" r="E501"/>
+      <c s="3" r="E501"/>
     </row>
     <row r="502">
-      <c s="4" r="E502"/>
+      <c s="3" r="E502"/>
     </row>
     <row r="503">
-      <c s="4" r="E503"/>
+      <c s="3" r="E503"/>
     </row>
     <row r="504">
-      <c s="4" r="E504"/>
+      <c s="3" r="E504"/>
     </row>
     <row r="505">
-      <c s="4" r="E505"/>
+      <c s="3" r="E505"/>
     </row>
     <row r="506">
-      <c s="4" r="E506"/>
+      <c s="3" r="E506"/>
     </row>
     <row r="507">
-      <c s="4" r="E507"/>
+      <c s="3" r="E507"/>
     </row>
     <row r="508">
-      <c s="4" r="E508"/>
+      <c s="3" r="E508"/>
     </row>
     <row r="509">
-      <c s="4" r="E509"/>
+      <c s="3" r="E509"/>
     </row>
     <row r="510">
-      <c s="4" r="E510"/>
+      <c s="3" r="E510"/>
     </row>
     <row r="511">
-      <c s="4" r="E511"/>
+      <c s="3" r="E511"/>
     </row>
     <row r="512">
-      <c s="4" r="E512"/>
+      <c s="3" r="E512"/>
     </row>
     <row r="513">
-      <c s="4" r="E513"/>
+      <c s="3" r="E513"/>
     </row>
     <row r="514">
-      <c s="4" r="E514"/>
+      <c s="3" r="E514"/>
     </row>
     <row r="515">
-      <c s="4" r="E515"/>
+      <c s="3" r="E515"/>
     </row>
     <row r="516">
-      <c s="4" r="E516"/>
+      <c s="3" r="E516"/>
     </row>
     <row r="517">
-      <c s="4" r="E517"/>
+      <c s="3" r="E517"/>
     </row>
     <row r="518">
-      <c s="4" r="E518"/>
+      <c s="3" r="E518"/>
     </row>
     <row r="519">
-      <c s="4" r="E519"/>
+      <c s="3" r="E519"/>
     </row>
     <row r="520">
-      <c s="4" r="E520"/>
+      <c s="3" r="E520"/>
     </row>
     <row r="521">
-      <c s="4" r="E521"/>
+      <c s="3" r="E521"/>
     </row>
     <row r="522">
-      <c s="4" r="E522"/>
+      <c s="3" r="E522"/>
     </row>
     <row r="523">
-      <c s="4" r="E523"/>
+      <c s="3" r="E523"/>
     </row>
     <row r="524">
-      <c s="4" r="E524"/>
+      <c s="3" r="E524"/>
     </row>
     <row r="525">
-      <c s="4" r="E525"/>
+      <c s="3" r="E525"/>
     </row>
     <row r="526">
-      <c s="4" r="E526"/>
+      <c s="3" r="E526"/>
     </row>
     <row r="527">
-      <c s="4" r="E527"/>
+      <c s="3" r="E527"/>
     </row>
     <row r="528">
-      <c s="4" r="E528"/>
+      <c s="3" r="E528"/>
     </row>
     <row r="529">
-      <c s="4" r="E529"/>
+      <c s="3" r="E529"/>
     </row>
     <row r="530">
-      <c s="4" r="E530"/>
+      <c s="3" r="E530"/>
     </row>
     <row r="531">
-      <c s="4" r="E531"/>
+      <c s="3" r="E531"/>
     </row>
     <row r="532">
-      <c s="4" r="E532"/>
+      <c s="3" r="E532"/>
     </row>
     <row r="533">
-      <c s="4" r="E533"/>
+      <c s="3" r="E533"/>
     </row>
     <row r="534">
-      <c s="4" r="E534"/>
+      <c s="3" r="E534"/>
     </row>
     <row r="535">
-      <c s="4" r="E535"/>
+      <c s="3" r="E535"/>
     </row>
     <row r="536">
-      <c s="4" r="E536"/>
+      <c s="3" r="E536"/>
     </row>
     <row r="537">
-      <c s="4" r="E537"/>
+      <c s="3" r="E537"/>
     </row>
     <row r="538">
-      <c s="4" r="E538"/>
+      <c s="3" r="E538"/>
     </row>
     <row r="539">
-      <c s="4" r="E539"/>
+      <c s="3" r="E539"/>
     </row>
     <row r="540">
-      <c s="4" r="E540"/>
+      <c s="3" r="E540"/>
     </row>
     <row r="541">
-      <c s="4" r="E541"/>
+      <c s="3" r="E541"/>
     </row>
     <row r="542">
-      <c s="4" r="E542"/>
+      <c s="3" r="E542"/>
     </row>
     <row r="543">
-      <c s="4" r="E543"/>
+      <c s="3" r="E543"/>
     </row>
     <row r="544">
-      <c s="4" r="E544"/>
+      <c s="3" r="E544"/>
     </row>
     <row r="545">
-      <c s="4" r="E545"/>
+      <c s="3" r="E545"/>
     </row>
     <row r="546">
-      <c s="4" r="E546"/>
+      <c s="3" r="E546"/>
     </row>
     <row r="547">
-      <c s="4" r="E547"/>
+      <c s="3" r="E547"/>
     </row>
     <row r="548">
-      <c s="4" r="E548"/>
+      <c s="3" r="E548"/>
     </row>
     <row r="549">
-      <c s="4" r="E549"/>
+      <c s="3" r="E549"/>
     </row>
     <row r="550">
-      <c s="4" r="E550"/>
+      <c s="3" r="E550"/>
     </row>
     <row r="551">
-      <c s="4" r="E551"/>
+      <c s="3" r="E551"/>
     </row>
     <row r="552">
-      <c s="4" r="E552"/>
+      <c s="3" r="E552"/>
     </row>
     <row r="553">
-      <c s="4" r="E553"/>
+      <c s="3" r="E553"/>
     </row>
     <row r="554">
-      <c s="4" r="E554"/>
+      <c s="3" r="E554"/>
     </row>
     <row r="555">
-      <c s="4" r="E555"/>
+      <c s="3" r="E555"/>
     </row>
     <row r="556">
-      <c s="4" r="E556"/>
+      <c s="3" r="E556"/>
     </row>
     <row r="557">
-      <c s="4" r="E557"/>
+      <c s="3" r="E557"/>
     </row>
     <row r="558">
-      <c s="4" r="E558"/>
+      <c s="3" r="E558"/>
     </row>
     <row r="559">
-      <c s="4" r="E559"/>
+      <c s="3" r="E559"/>
     </row>
     <row r="560">
-      <c s="4" r="E560"/>
+      <c s="3" r="E560"/>
     </row>
     <row r="561">
-      <c s="4" r="E561"/>
+      <c s="3" r="E561"/>
     </row>
     <row r="562">
-      <c s="4" r="E562"/>
+      <c s="3" r="E562"/>
     </row>
     <row r="563">
-      <c s="4" r="E563"/>
+      <c s="3" r="E563"/>
     </row>
     <row r="564">
-      <c s="4" r="E564"/>
+      <c s="3" r="E564"/>
     </row>
     <row r="565">
-      <c s="4" r="E565"/>
+      <c s="3" r="E565"/>
     </row>
     <row r="566">
-      <c s="4" r="E566"/>
+      <c s="3" r="E566"/>
     </row>
     <row r="567">
-      <c s="4" r="E567"/>
+      <c s="3" r="E567"/>
     </row>
     <row r="568">
-      <c s="4" r="E568"/>
+      <c s="3" r="E568"/>
     </row>
     <row r="569">
-      <c s="4" r="E569"/>
+      <c s="3" r="E569"/>
     </row>
     <row r="570">
-      <c s="4" r="E570"/>
+      <c s="3" r="E570"/>
     </row>
     <row r="571">
-      <c s="4" r="E571"/>
+      <c s="3" r="E571"/>
     </row>
     <row r="572">
-      <c s="4" r="E572"/>
+      <c s="3" r="E572"/>
     </row>
     <row r="573">
-      <c s="4" r="E573"/>
+      <c s="3" r="E573"/>
     </row>
     <row r="574">
-      <c s="4" r="E574"/>
+      <c s="3" r="E574"/>
     </row>
     <row r="575">
-      <c s="4" r="E575"/>
+      <c s="3" r="E575"/>
     </row>
     <row r="576">
-      <c s="4" r="E576"/>
+      <c s="3" r="E576"/>
     </row>
     <row r="577">
-      <c s="4" r="E577"/>
+      <c s="3" r="E577"/>
     </row>
     <row r="578">
-      <c s="4" r="E578"/>
+      <c s="3" r="E578"/>
     </row>
     <row r="579">
-      <c s="4" r="E579"/>
+      <c s="3" r="E579"/>
     </row>
     <row r="580">
-      <c s="4" r="E580"/>
+      <c s="3" r="E580"/>
     </row>
     <row r="581">
-      <c s="4" r="E581"/>
+      <c s="3" r="E581"/>
     </row>
     <row r="582">
-      <c s="4" r="E582"/>
+      <c s="3" r="E582"/>
     </row>
     <row r="583">
-      <c s="4" r="E583"/>
+      <c s="3" r="E583"/>
     </row>
     <row r="584">
-      <c s="4" r="E584"/>
+      <c s="3" r="E584"/>
     </row>
     <row r="585">
-      <c s="4" r="E585"/>
+      <c s="3" r="E585"/>
     </row>
     <row r="586">
-      <c s="4" r="E586"/>
+      <c s="3" r="E586"/>
     </row>
     <row r="587">
-      <c s="4" r="E587"/>
+      <c s="3" r="E587"/>
     </row>
     <row r="588">
-      <c s="4" r="E588"/>
+      <c s="3" r="E588"/>
     </row>
     <row r="589">
-      <c s="4" r="E589"/>
+      <c s="3" r="E589"/>
     </row>
     <row r="590">
-      <c s="4" r="E590"/>
+      <c s="3" r="E590"/>
     </row>
     <row r="591">
-      <c s="4" r="E591"/>
+      <c s="3" r="E591"/>
     </row>
     <row r="592">
-      <c s="4" r="E592"/>
+      <c s="3" r="E592"/>
     </row>
     <row r="593">
-      <c s="4" r="E593"/>
+      <c s="3" r="E593"/>
     </row>
     <row r="594">
-      <c s="4" r="E594"/>
+      <c s="3" r="E594"/>
     </row>
     <row r="595">
-      <c s="4" r="E595"/>
+      <c s="3" r="E595"/>
     </row>
     <row r="596">
-      <c s="4" r="E596"/>
+      <c s="3" r="E596"/>
     </row>
     <row r="597">
-      <c s="4" r="E597"/>
+      <c s="3" r="E597"/>
     </row>
     <row r="598">
-      <c s="4" r="E598"/>
+      <c s="3" r="E598"/>
     </row>
     <row r="599">
-      <c s="4" r="E599"/>
+      <c s="3" r="E599"/>
     </row>
     <row r="600">
-      <c s="4" r="E600"/>
+      <c s="3" r="E600"/>
     </row>
     <row r="601">
-      <c s="4" r="E601"/>
+      <c s="3" r="E601"/>
     </row>
     <row r="602">
-      <c s="4" r="E602"/>
+      <c s="3" r="E602"/>
     </row>
     <row r="603">
-      <c s="4" r="E603"/>
+      <c s="3" r="E603"/>
     </row>
     <row r="604">
-      <c s="4" r="E604"/>
+      <c s="3" r="E604"/>
     </row>
     <row r="605">
-      <c s="4" r="E605"/>
+      <c s="3" r="E605"/>
     </row>
     <row r="606">
-      <c s="4" r="E606"/>
+      <c s="3" r="E606"/>
     </row>
     <row r="607">
-      <c s="4" r="E607"/>
+      <c s="3" r="E607"/>
     </row>
     <row r="608">
-      <c s="4" r="E608"/>
+      <c s="3" r="E608"/>
     </row>
     <row r="609">
-      <c s="4" r="E609"/>
+      <c s="3" r="E609"/>
     </row>
     <row r="610">
-      <c s="4" r="E610"/>
+      <c s="3" r="E610"/>
     </row>
     <row r="611">
-      <c s="4" r="E611"/>
+      <c s="3" r="E611"/>
     </row>
     <row r="612">
-      <c s="4" r="E612"/>
+      <c s="3" r="E612"/>
     </row>
     <row r="613">
-      <c s="4" r="E613"/>
+      <c s="3" r="E613"/>
     </row>
     <row r="614">
-      <c s="4" r="E614"/>
+      <c s="3" r="E614"/>
     </row>
     <row r="615">
-      <c s="4" r="E615"/>
+      <c s="3" r="E615"/>
     </row>
     <row r="616">
-      <c s="4" r="E616"/>
+      <c s="3" r="E616"/>
     </row>
     <row r="617">
-      <c s="4" r="E617"/>
+      <c s="3" r="E617"/>
     </row>
     <row r="618">
-      <c s="4" r="E618"/>
+      <c s="3" r="E618"/>
     </row>
     <row r="619">
-      <c s="4" r="E619"/>
+      <c s="3" r="E619"/>
     </row>
     <row r="620">
-      <c s="4" r="E620"/>
+      <c s="3" r="E620"/>
     </row>
     <row r="621">
-      <c s="4" r="E621"/>
+      <c s="3" r="E621"/>
     </row>
     <row r="622">
-      <c s="4" r="E622"/>
+      <c s="3" r="E622"/>
     </row>
     <row r="623">
-      <c s="4" r="E623"/>
+      <c s="3" r="E623"/>
     </row>
     <row r="624">
-      <c s="4" r="E624"/>
+      <c s="3" r="E624"/>
     </row>
     <row r="625">
-      <c s="4" r="E625"/>
+      <c s="3" r="E625"/>
     </row>
     <row r="626">
-      <c s="4" r="E626"/>
+      <c s="3" r="E626"/>
     </row>
     <row r="627">
-      <c s="4" r="E627"/>
+      <c s="3" r="E627"/>
     </row>
     <row r="628">
-      <c s="4" r="E628"/>
+      <c s="3" r="E628"/>
     </row>
     <row r="629">
-      <c s="4" r="E629"/>
+      <c s="3" r="E629"/>
     </row>
     <row r="630">
-      <c s="4" r="E630"/>
+      <c s="3" r="E630"/>
     </row>
     <row r="631">
-      <c s="4" r="E631"/>
+      <c s="3" r="E631"/>
     </row>
     <row r="632">
-      <c s="4" r="E632"/>
+      <c s="3" r="E632"/>
     </row>
     <row r="633">
-      <c s="4" r="E633"/>
+      <c s="3" r="E633"/>
     </row>
     <row r="634">
-      <c s="4" r="E634"/>
+      <c s="3" r="E634"/>
     </row>
     <row r="635">
-      <c s="4" r="E635"/>
+      <c s="3" r="E635"/>
     </row>
     <row r="636">
-      <c s="4" r="E636"/>
+      <c s="3" r="E636"/>
     </row>
     <row r="637">
-      <c s="4" r="E637"/>
+      <c s="3" r="E637"/>
     </row>
     <row r="638">
-      <c s="4" r="E638"/>
+      <c s="3" r="E638"/>
     </row>
     <row r="639">
-      <c s="4" r="E639"/>
+      <c s="3" r="E639"/>
     </row>
     <row r="640">
-      <c s="4" r="E640"/>
+      <c s="3" r="E640"/>
     </row>
     <row r="641">
-      <c s="4" r="E641"/>
+      <c s="3" r="E641"/>
     </row>
     <row r="642">
-      <c s="4" r="E642"/>
+      <c s="3" r="E642"/>
     </row>
     <row r="643">
-      <c s="4" r="E643"/>
+      <c s="3" r="E643"/>
     </row>
     <row r="644">
-      <c s="4" r="E644"/>
+      <c s="3" r="E644"/>
     </row>
     <row r="645">
-      <c s="4" r="E645"/>
+      <c s="3" r="E645"/>
     </row>
     <row r="646">
-      <c s="4" r="E646"/>
+      <c s="3" r="E646"/>
     </row>
     <row r="647">
-      <c s="4" r="E647"/>
+      <c s="3" r="E647"/>
     </row>
     <row r="648">
-      <c s="4" r="E648"/>
+      <c s="3" r="E648"/>
     </row>
     <row r="649">
-      <c s="4" r="E649"/>
+      <c s="3" r="E649"/>
     </row>
     <row r="650">
-      <c s="4" r="E650"/>
+      <c s="3" r="E650"/>
     </row>
     <row r="651">
-      <c s="4" r="E651"/>
+      <c s="3" r="E651"/>
     </row>
     <row r="652">
-      <c s="4" r="E652"/>
+      <c s="3" r="E652"/>
     </row>
     <row r="653">
-      <c s="4" r="E653"/>
+      <c s="3" r="E653"/>
     </row>
     <row r="654">
-      <c s="4" r="E654"/>
+      <c s="3" r="E654"/>
     </row>
     <row r="655">
-      <c s="4" r="E655"/>
+      <c s="3" r="E655"/>
     </row>
     <row r="656">
-      <c s="4" r="E656"/>
+      <c s="3" r="E656"/>
     </row>
     <row r="657">
-      <c s="4" r="E657"/>
+      <c s="3" r="E657"/>
     </row>
     <row r="658">
-      <c s="4" r="E658"/>
+      <c s="3" r="E658"/>
     </row>
     <row r="659">
-      <c s="4" r="E659"/>
+      <c s="3" r="E659"/>
     </row>
     <row r="660">
-      <c s="4" r="E660"/>
+      <c s="3" r="E660"/>
     </row>
     <row r="661">
-      <c s="4" r="E661"/>
+      <c s="3" r="E661"/>
     </row>
     <row r="662">
-      <c s="4" r="E662"/>
+      <c s="3" r="E662"/>
     </row>
     <row r="663">
-      <c s="4" r="E663"/>
+      <c s="3" r="E663"/>
     </row>
     <row r="664">
-      <c s="4" r="E664"/>
+      <c s="3" r="E664"/>
     </row>
     <row r="665">
-      <c s="4" r="E665"/>
+      <c s="3" r="E665"/>
     </row>
     <row r="666">
-      <c s="4" r="E666"/>
+      <c s="3" r="E666"/>
     </row>
     <row r="667">
-      <c s="4" r="E667"/>
+      <c s="3" r="E667"/>
     </row>
     <row r="668">
-      <c s="4" r="E668"/>
+      <c s="3" r="E668"/>
     </row>
     <row r="669">
-      <c s="4" r="E669"/>
+      <c s="3" r="E669"/>
     </row>
     <row r="670">
-      <c s="4" r="E670"/>
+      <c s="3" r="E670"/>
     </row>
     <row r="671">
-      <c s="4" r="E671"/>
+      <c s="3" r="E671"/>
     </row>
     <row r="672">
-      <c s="4" r="E672"/>
+      <c s="3" r="E672"/>
     </row>
     <row r="673">
-      <c s="4" r="E673"/>
+      <c s="3" r="E673"/>
     </row>
     <row r="674">
-      <c s="4" r="E674"/>
+      <c s="3" r="E674"/>
     </row>
     <row r="675">
-      <c s="4" r="E675"/>
+      <c s="3" r="E675"/>
     </row>
     <row r="676">
-      <c s="4" r="E676"/>
+      <c s="3" r="E676"/>
     </row>
     <row r="677">
-      <c s="4" r="E677"/>
+      <c s="3" r="E677"/>
     </row>
     <row r="678">
-      <c s="4" r="E678"/>
+      <c s="3" r="E678"/>
     </row>
     <row r="679">
-      <c s="4" r="E679"/>
+      <c s="3" r="E679"/>
     </row>
     <row r="680">
-      <c s="4" r="E680"/>
+      <c s="3" r="E680"/>
     </row>
     <row r="681">
-      <c s="4" r="E681"/>
+      <c s="3" r="E681"/>
     </row>
     <row r="682">
-      <c s="4" r="E682"/>
+      <c s="3" r="E682"/>
     </row>
     <row r="683">
-      <c s="4" r="E683"/>
+      <c s="3" r="E683"/>
     </row>
     <row r="684">
-      <c s="4" r="E684"/>
+      <c s="3" r="E684"/>
     </row>
     <row r="685">
-      <c s="4" r="E685"/>
+      <c s="3" r="E685"/>
     </row>
     <row r="686">
-      <c s="4" r="E686"/>
+      <c s="3" r="E686"/>
     </row>
     <row r="687">
-      <c s="4" r="E687"/>
+      <c s="3" r="E687"/>
     </row>
     <row r="688">
-      <c s="4" r="E688"/>
+      <c s="3" r="E688"/>
     </row>
     <row r="689">
-      <c s="4" r="E689"/>
+      <c s="3" r="E689"/>
     </row>
     <row r="690">
-      <c s="4" r="E690"/>
+      <c s="3" r="E690"/>
     </row>
     <row r="691">
-      <c s="4" r="E691"/>
+      <c s="3" r="E691"/>
     </row>
     <row r="692">
-      <c s="4" r="E692"/>
+      <c s="3" r="E692"/>
     </row>
     <row r="693">
-      <c s="4" r="E693"/>
+      <c s="3" r="E693"/>
     </row>
     <row r="694">
-      <c s="4" r="E694"/>
+      <c s="3" r="E694"/>
     </row>
     <row r="695">
-      <c s="4" r="E695"/>
+      <c s="3" r="E695"/>
     </row>
     <row r="696">
-      <c s="4" r="E696"/>
+      <c s="3" r="E696"/>
     </row>
     <row r="697">
-      <c s="4" r="E697"/>
+      <c s="3" r="E697"/>
     </row>
     <row r="698">
-      <c s="4" r="E698"/>
+      <c s="3" r="E698"/>
     </row>
     <row r="699">
-      <c s="4" r="E699"/>
+      <c s="3" r="E699"/>
     </row>
     <row r="700">
-      <c s="4" r="E700"/>
+      <c s="3" r="E700"/>
     </row>
     <row r="701">
-      <c s="4" r="E701"/>
+      <c s="3" r="E701"/>
     </row>
     <row r="702">
-      <c s="4" r="E702"/>
+      <c s="3" r="E702"/>
     </row>
     <row r="703">
-      <c s="4" r="E703"/>
+      <c s="3" r="E703"/>
     </row>
     <row r="704">
-      <c s="4" r="E704"/>
+      <c s="3" r="E704"/>
     </row>
     <row r="705">
-      <c s="4" r="E705"/>
+      <c s="3" r="E705"/>
     </row>
     <row r="706">
-      <c s="4" r="E706"/>
+      <c s="3" r="E706"/>
     </row>
     <row r="707">
-      <c s="4" r="E707"/>
+      <c s="3" r="E707"/>
     </row>
     <row r="708">
-      <c s="4" r="E708"/>
+      <c s="3" r="E708"/>
     </row>
     <row r="709">
-      <c s="4" r="E709"/>
+      <c s="3" r="E709"/>
     </row>
     <row r="710">
-      <c s="4" r="E710"/>
+      <c s="3" r="E710"/>
     </row>
     <row r="711">
-      <c s="4" r="E711"/>
+      <c s="3" r="E711"/>
     </row>
     <row r="712">
-      <c s="4" r="E712"/>
+      <c s="3" r="E712"/>
     </row>
     <row r="713">
-      <c s="4" r="E713"/>
+      <c s="3" r="E713"/>
     </row>
     <row r="714">
-      <c s="4" r="E714"/>
+      <c s="3" r="E714"/>
     </row>
     <row r="715">
-      <c s="4" r="E715"/>
+      <c s="3" r="E715"/>
     </row>
     <row r="716">
-      <c s="4" r="E716"/>
+      <c s="3" r="E716"/>
     </row>
     <row r="717">
-      <c s="4" r="E717"/>
+      <c s="3" r="E717"/>
     </row>
     <row r="718">
-      <c s="4" r="E718"/>
+      <c s="3" r="E718"/>
     </row>
     <row r="719">
-      <c s="4" r="E719"/>
+      <c s="3" r="E719"/>
     </row>
     <row r="720">
-      <c s="4" r="E720"/>
+      <c s="3" r="E720"/>
     </row>
     <row r="721">
-      <c s="4" r="E721"/>
+      <c s="3" r="E721"/>
     </row>
     <row r="722">
-      <c s="4" r="E722"/>
+      <c s="3" r="E722"/>
     </row>
     <row r="723">
-      <c s="4" r="E723"/>
+      <c s="3" r="E723"/>
     </row>
     <row r="724">
-      <c s="4" r="E724"/>
+      <c s="3" r="E724"/>
     </row>
     <row r="725">
-      <c s="4" r="E725"/>
+      <c s="3" r="E725"/>
     </row>
     <row r="726">
-      <c s="4" r="E726"/>
+      <c s="3" r="E726"/>
     </row>
     <row r="727">
-      <c s="4" r="E727"/>
+      <c s="3" r="E727"/>
     </row>
     <row r="728">
-      <c s="4" r="E728"/>
+      <c s="3" r="E728"/>
     </row>
     <row r="729">
-      <c s="4" r="E729"/>
+      <c s="3" r="E729"/>
     </row>
     <row r="730">
-      <c s="4" r="E730"/>
+      <c s="3" r="E730"/>
     </row>
     <row r="731">
-      <c s="4" r="E731"/>
+      <c s="3" r="E731"/>
     </row>
     <row r="732">
-      <c s="4" r="E732"/>
+      <c s="3" r="E732"/>
     </row>
     <row r="733">
-      <c s="4" r="E733"/>
+      <c s="3" r="E733"/>
     </row>
     <row r="734">
-      <c s="4" r="E734"/>
+      <c s="3" r="E734"/>
     </row>
     <row r="735">
-      <c s="4" r="E735"/>
+      <c s="3" r="E735"/>
     </row>
     <row r="736">
-      <c s="4" r="E736"/>
+      <c s="3" r="E736"/>
     </row>
     <row r="737">
-      <c s="4" r="E737"/>
+      <c s="3" r="E737"/>
     </row>
     <row r="738">
-      <c s="4" r="E738"/>
+      <c s="3" r="E738"/>
     </row>
     <row r="739">
-      <c s="4" r="E739"/>
+      <c s="3" r="E739"/>
     </row>
     <row r="740">
-      <c s="4" r="E740"/>
+      <c s="3" r="E740"/>
     </row>
     <row r="741">
-      <c s="4" r="E741"/>
+      <c s="3" r="E741"/>
     </row>
     <row r="742">
-      <c s="4" r="E742"/>
+      <c s="3" r="E742"/>
     </row>
     <row r="743">
-      <c s="4" r="E743"/>
+      <c s="3" r="E743"/>
     </row>
     <row r="744">
-      <c s="4" r="E744"/>
+      <c s="3" r="E744"/>
     </row>
     <row r="745">
-      <c s="4" r="E745"/>
+      <c s="3" r="E745"/>
     </row>
     <row r="746">
-      <c s="4" r="E746"/>
+      <c s="3" r="E746"/>
     </row>
     <row r="747">
-      <c s="4" r="E747"/>
+      <c s="3" r="E747"/>
     </row>
     <row r="748">
-      <c s="4" r="E748"/>
+      <c s="3" r="E748"/>
     </row>
     <row r="749">
-      <c s="4" r="E749"/>
+      <c s="3" r="E749"/>
     </row>
     <row r="750">
-      <c s="4" r="E750"/>
+      <c s="3" r="E750"/>
     </row>
     <row r="751">
-      <c s="4" r="E751"/>
+      <c s="3" r="E751"/>
     </row>
     <row r="752">
-      <c s="4" r="E752"/>
+      <c s="3" r="E752"/>
     </row>
     <row r="753">
-      <c s="4" r="E753"/>
+      <c s="3" r="E753"/>
     </row>
     <row r="754">
-      <c s="4" r="E754"/>
+      <c s="3" r="E754"/>
     </row>
     <row r="755">
-      <c s="4" r="E755"/>
+      <c s="3" r="E755"/>
     </row>
     <row r="756">
-      <c s="4" r="E756"/>
+      <c s="3" r="E756"/>
     </row>
     <row r="757">
-      <c s="4" r="E757"/>
+      <c s="3" r="E757"/>
     </row>
     <row r="758">
-      <c s="4" r="E758"/>
+      <c s="3" r="E758"/>
     </row>
     <row r="759">
-      <c s="4" r="E759"/>
+      <c s="3" r="E759"/>
     </row>
     <row r="760">
-      <c s="4" r="E760"/>
+      <c s="3" r="E760"/>
     </row>
     <row r="761">
-      <c s="4" r="E761"/>
+      <c s="3" r="E761"/>
     </row>
     <row r="762">
-      <c s="4" r="E762"/>
+      <c s="3" r="E762"/>
     </row>
     <row r="763">
-      <c s="4" r="E763"/>
+      <c s="3" r="E763"/>
     </row>
     <row r="764">
-      <c s="4" r="E764"/>
+      <c s="3" r="E764"/>
     </row>
     <row r="765">
-      <c s="4" r="E765"/>
+      <c s="3" r="E765"/>
     </row>
     <row r="766">
-      <c s="4" r="E766"/>
+      <c s="3" r="E766"/>
     </row>
     <row r="767">
-      <c s="4" r="E767"/>
+      <c s="3" r="E767"/>
     </row>
     <row r="768">
-      <c s="4" r="E768"/>
+      <c s="3" r="E768"/>
     </row>
     <row r="769">
-      <c s="4" r="E769"/>
+      <c s="3" r="E769"/>
     </row>
     <row r="770">
-      <c s="4" r="E770"/>
+      <c s="3" r="E770"/>
     </row>
     <row r="771">
-      <c s="4" r="E771"/>
+      <c s="3" r="E771"/>
     </row>
     <row r="772">
-      <c s="4" r="E772"/>
+      <c s="3" r="E772"/>
     </row>
     <row r="773">
-      <c s="4" r="E773"/>
+      <c s="3" r="E773"/>
     </row>
     <row r="774">
-      <c s="4" r="E774"/>
+      <c s="3" r="E774"/>
     </row>
     <row r="775">
-      <c s="4" r="E775"/>
+      <c s="3" r="E775"/>
     </row>
     <row r="776">
-      <c s="4" r="E776"/>
+      <c s="3" r="E776"/>
     </row>
     <row r="777">
-      <c s="4" r="E777"/>
+      <c s="3" r="E777"/>
     </row>
     <row r="778">
-      <c s="4" r="E778"/>
+      <c s="3" r="E778"/>
     </row>
     <row r="779">
-      <c s="4" r="E779"/>
+      <c s="3" r="E779"/>
     </row>
     <row r="780">
-      <c s="4" r="E780"/>
+      <c s="3" r="E780"/>
     </row>
     <row r="781">
-      <c s="4" r="E781"/>
+      <c s="3" r="E781"/>
     </row>
     <row r="782">
-      <c s="4" r="E782"/>
+      <c s="3" r="E782"/>
     </row>
     <row r="783">
-      <c s="4" r="E783"/>
+      <c s="3" r="E783"/>
     </row>
     <row r="784">
-      <c s="4" r="E784"/>
+      <c s="3" r="E784"/>
     </row>
     <row r="785">
-      <c s="4" r="E785"/>
+      <c s="3" r="E785"/>
     </row>
     <row r="786">
-      <c s="4" r="E786"/>
+      <c s="3" r="E786"/>
     </row>
     <row r="787">
-      <c s="4" r="E787"/>
+      <c s="3" r="E787"/>
     </row>
     <row r="788">
-      <c s="4" r="E788"/>
+      <c s="3" r="E788"/>
     </row>
     <row r="789">
-      <c s="4" r="E789"/>
+      <c s="3" r="E789"/>
     </row>
     <row r="790">
-      <c s="4" r="E790"/>
+      <c s="3" r="E790"/>
     </row>
     <row r="791">
-      <c s="4" r="E791"/>
+      <c s="3" r="E791"/>
     </row>
     <row r="792">
-      <c s="4" r="E792"/>
+      <c s="3" r="E792"/>
     </row>
     <row r="793">
-      <c s="4" r="E793"/>
+      <c s="3" r="E793"/>
     </row>
     <row r="794">
-      <c s="4" r="E794"/>
+      <c s="3" r="E794"/>
     </row>
     <row r="795">
-      <c s="4" r="E795"/>
+      <c s="3" r="E795"/>
     </row>
     <row r="796">
-      <c s="4" r="E796"/>
+      <c s="3" r="E796"/>
     </row>
     <row r="797">
-      <c s="4" r="E797"/>
+      <c s="3" r="E797"/>
     </row>
     <row r="798">
-      <c s="4" r="E798"/>
+      <c s="3" r="E798"/>
     </row>
     <row r="799">
-      <c s="4" r="E799"/>
+      <c s="3" r="E799"/>
     </row>
     <row r="800">
-      <c s="4" r="E800"/>
+      <c s="3" r="E800"/>
     </row>
     <row r="801">
-      <c s="4" r="E801"/>
+      <c s="3" r="E801"/>
     </row>
     <row r="802">
-      <c s="4" r="E802"/>
+      <c s="3" r="E802"/>
     </row>
     <row r="803">
-      <c s="4" r="E803"/>
+      <c s="3" r="E803"/>
     </row>
     <row r="804">
-      <c s="4" r="E804"/>
+      <c s="3" r="E804"/>
     </row>
     <row r="805">
-      <c s="4" r="E805"/>
+      <c s="3" r="E805"/>
     </row>
     <row r="806">
-      <c s="4" r="E806"/>
+      <c s="3" r="E806"/>
     </row>
     <row r="807">
-      <c s="4" r="E807"/>
+      <c s="3" r="E807"/>
     </row>
     <row r="808">
-      <c s="4" r="E808"/>
+      <c s="3" r="E808"/>
     </row>
     <row r="809">
-      <c s="4" r="E809"/>
+      <c s="3" r="E809"/>
     </row>
     <row r="810">
-      <c s="4" r="E810"/>
+      <c s="3" r="E810"/>
     </row>
     <row r="811">
-      <c s="4" r="E811"/>
+      <c s="3" r="E811"/>
     </row>
     <row r="812">
-      <c s="4" r="E812"/>
+      <c s="3" r="E812"/>
     </row>
     <row r="813">
-      <c s="4" r="E813"/>
+      <c s="3" r="E813"/>
     </row>
     <row r="814">
-      <c s="4" r="E814"/>
+      <c s="3" r="E814"/>
     </row>
     <row r="815">
-      <c s="4" r="E815"/>
+      <c s="3" r="E815"/>
     </row>
     <row r="816">
-      <c s="4" r="E816"/>
+      <c s="3" r="E816"/>
     </row>
     <row r="817">
-      <c s="4" r="E817"/>
+      <c s="3" r="E817"/>
     </row>
     <row r="818">
-      <c s="4" r="E818"/>
+      <c s="3" r="E818"/>
     </row>
     <row r="819">
-      <c s="4" r="E819"/>
+      <c s="3" r="E819"/>
     </row>
     <row r="820">
-      <c s="4" r="E820"/>
+      <c s="3" r="E820"/>
     </row>
     <row r="821">
-      <c s="4" r="E821"/>
+      <c s="3" r="E821"/>
     </row>
     <row r="822">
-      <c s="4" r="E822"/>
+      <c s="3" r="E822"/>
     </row>
     <row r="823">
-      <c s="4" r="E823"/>
+      <c s="3" r="E823"/>
     </row>
     <row r="824">
-      <c s="4" r="E824"/>
+      <c s="3" r="E824"/>
     </row>
     <row r="825">
-      <c s="4" r="E825"/>
+      <c s="3" r="E825"/>
     </row>
     <row r="826">
-      <c s="4" r="E826"/>
+      <c s="3" r="E826"/>
     </row>
     <row r="827">
-      <c s="4" r="E827"/>
+      <c s="3" r="E827"/>
     </row>
     <row r="828">
-      <c s="4" r="E828"/>
+      <c s="3" r="E828"/>
     </row>
     <row r="829">
-      <c s="4" r="E829"/>
+      <c s="3" r="E829"/>
     </row>
     <row r="830">
-      <c s="4" r="E830"/>
+      <c s="3" r="E830"/>
     </row>
     <row r="831">
-      <c s="4" r="E831"/>
+      <c s="3" r="E831"/>
     </row>
     <row r="832">
-      <c s="4" r="E832"/>
+      <c s="3" r="E832"/>
     </row>
     <row r="833">
-      <c s="4" r="E833"/>
+      <c s="3" r="E833"/>
     </row>
     <row r="834">
-      <c s="4" r="E834"/>
+      <c s="3" r="E834"/>
     </row>
     <row r="835">
-      <c s="4" r="E835"/>
+      <c s="3" r="E835"/>
     </row>
     <row r="836">
-      <c s="4" r="E836"/>
+      <c s="3" r="E836"/>
     </row>
     <row r="837">
-      <c s="4" r="E837"/>
+      <c s="3" r="E837"/>
     </row>
     <row r="838">
-      <c s="4" r="E838"/>
+      <c s="3" r="E838"/>
     </row>
     <row r="839">
-      <c s="4" r="E839"/>
+      <c s="3" r="E839"/>
     </row>
     <row r="840">
-      <c s="4" r="E840"/>
+      <c s="3" r="E840"/>
     </row>
     <row r="841">
-      <c s="4" r="E841"/>
+      <c s="3" r="E841"/>
     </row>
     <row r="842">
-      <c s="4" r="E842"/>
+      <c s="3" r="E842"/>
     </row>
     <row r="843">
-      <c s="4" r="E843"/>
+      <c s="3" r="E843"/>
     </row>
     <row r="844">
-      <c s="4" r="E844"/>
+      <c s="3" r="E844"/>
     </row>
     <row r="845">
-      <c s="4" r="E845"/>
+      <c s="3" r="E845"/>
     </row>
     <row r="846">
-      <c s="4" r="E846"/>
+      <c s="3" r="E846"/>
     </row>
     <row r="847">
-      <c s="4" r="E847"/>
+      <c s="3" r="E847"/>
     </row>
     <row r="848">
-      <c s="4" r="E848"/>
+      <c s="3" r="E848"/>
     </row>
     <row r="849">
-      <c s="4" r="E849"/>
+      <c s="3" r="E849"/>
     </row>
     <row r="850">
-      <c s="4" r="E850"/>
+      <c s="3" r="E850"/>
     </row>
     <row r="851">
-      <c s="4" r="E851"/>
+      <c s="3" r="E851"/>
     </row>
     <row r="852">
-      <c s="4" r="E852"/>
+      <c s="3" r="E852"/>
     </row>
     <row r="853">
-      <c s="4" r="E853"/>
+      <c s="3" r="E853"/>
     </row>
     <row r="854">
-      <c s="4" r="E854"/>
+      <c s="3" r="E854"/>
     </row>
     <row r="855">
-      <c s="4" r="E855"/>
+      <c s="3" r="E855"/>
     </row>
     <row r="856">
-      <c s="4" r="E856"/>
+      <c s="3" r="E856"/>
     </row>
     <row r="857">
-      <c s="4" r="E857"/>
+      <c s="3" r="E857"/>
     </row>
     <row r="858">
-      <c s="4" r="E858"/>
+      <c s="3" r="E858"/>
     </row>
     <row r="859">
-      <c s="4" r="E859"/>
+      <c s="3" r="E859"/>
     </row>
     <row r="860">
-      <c s="4" r="E860"/>
+      <c s="3" r="E860"/>
     </row>
     <row r="861">
-      <c s="4" r="E861"/>
+      <c s="3" r="E861"/>
     </row>
     <row r="862">
-      <c s="4" r="E862"/>
+      <c s="3" r="E862"/>
     </row>
     <row r="863">
-      <c s="4" r="E863"/>
+      <c s="3" r="E863"/>
     </row>
     <row r="864">
-      <c s="4" r="E864"/>
+      <c s="3" r="E864"/>
     </row>
     <row r="865">
-      <c s="4" r="E865"/>
+      <c s="3" r="E865"/>
     </row>
     <row r="866">
-      <c s="4" r="E866"/>
+      <c s="3" r="E866"/>
     </row>
     <row r="867">
-      <c s="4" r="E867"/>
+      <c s="3" r="E867"/>
     </row>
     <row r="868">
-      <c s="4" r="E868"/>
+      <c s="3" r="E868"/>
     </row>
     <row r="869">
-      <c s="4" r="E869"/>
+      <c s="3" r="E869"/>
     </row>
     <row r="870">
-      <c s="4" r="E870"/>
+      <c s="3" r="E870"/>
     </row>
     <row r="871">
-      <c s="4" r="E871"/>
+      <c s="3" r="E871"/>
     </row>
     <row r="872">
-      <c s="4" r="E872"/>
+      <c s="3" r="E872"/>
     </row>
     <row r="873">
-      <c s="4" r="E873"/>
+      <c s="3" r="E873"/>
     </row>
     <row r="874">
-      <c s="4" r="E874"/>
+      <c s="3" r="E874"/>
     </row>
     <row r="875">
-      <c s="4" r="E875"/>
+      <c s="3" r="E875"/>
     </row>
     <row r="876">
-      <c s="4" r="E876"/>
+      <c s="3" r="E876"/>
     </row>
     <row r="877">
-      <c s="4" r="E877"/>
+      <c s="3" r="E877"/>
     </row>
     <row r="878">
-      <c s="4" r="E878"/>
+      <c s="3" r="E878"/>
     </row>
     <row r="879">
-      <c s="4" r="E879"/>
+      <c s="3" r="E879"/>
     </row>
     <row r="880">
-      <c s="4" r="E880"/>
+      <c s="3" r="E880"/>
     </row>
     <row r="881">
-      <c s="4" r="E881"/>
+      <c s="3" r="E881"/>
     </row>
     <row r="882">
-      <c s="4" r="E882"/>
+      <c s="3" r="E882"/>
     </row>
     <row r="883">
-      <c s="4" r="E883"/>
+      <c s="3" r="E883"/>
     </row>
     <row r="884">
-      <c s="4" r="E884"/>
+      <c s="3" r="E884"/>
     </row>
     <row r="885">
-      <c s="4" r="E885"/>
+      <c s="3" r="E885"/>
     </row>
     <row r="886">
-      <c s="4" r="E886"/>
+      <c s="3" r="E886"/>
     </row>
     <row r="887">
-      <c s="4" r="E887"/>
+      <c s="3" r="E887"/>
     </row>
     <row r="888">
-      <c s="4" r="E888"/>
+      <c s="3" r="E888"/>
     </row>
     <row r="889">
-      <c s="4" r="E889"/>
+      <c s="3" r="E889"/>
     </row>
     <row r="890">
-      <c s="4" r="E890"/>
+      <c s="3" r="E890"/>
     </row>
     <row r="891">
-      <c s="4" r="E891"/>
+      <c s="3" r="E891"/>
     </row>
     <row r="892">
-      <c s="4" r="E892"/>
+      <c s="3" r="E892"/>
     </row>
     <row r="893">
-      <c s="4" r="E893"/>
+      <c s="3" r="E893"/>
     </row>
     <row r="894">
-      <c s="4" r="E894"/>
+      <c s="3" r="E894"/>
     </row>
     <row r="895">
-      <c s="4" r="E895"/>
+      <c s="3" r="E895"/>
     </row>
     <row r="896">
-      <c s="4" r="E896"/>
+      <c s="3" r="E896"/>
     </row>
     <row r="897">
-      <c s="4" r="E897"/>
+      <c s="3" r="E897"/>
     </row>
     <row r="898">
-      <c s="4" r="E898"/>
+      <c s="3" r="E898"/>
     </row>
     <row r="899">
-      <c s="4" r="E899"/>
+      <c s="3" r="E899"/>
     </row>
     <row r="900">
-      <c s="4" r="E900"/>
+      <c s="3" r="E900"/>
     </row>
     <row r="901">
-      <c s="4" r="E901"/>
+      <c s="3" r="E901"/>
     </row>
     <row r="902">
-      <c s="4" r="E902"/>
+      <c s="3" r="E902"/>
     </row>
     <row r="903">
-      <c s="4" r="E903"/>
+      <c s="3" r="E903"/>
     </row>
     <row r="904">
-      <c s="4" r="E904"/>
+      <c s="3" r="E904"/>
     </row>
     <row r="905">
-      <c s="4" r="E905"/>
+      <c s="3" r="E905"/>
     </row>
     <row r="906">
-      <c s="4" r="E906"/>
+      <c s="3" r="E906"/>
     </row>
     <row r="907">
-      <c s="4" r="E907"/>
+      <c s="3" r="E907"/>
     </row>
     <row r="908">
-      <c s="4" r="E908"/>
+      <c s="3" r="E908"/>
     </row>
     <row r="909">
-      <c s="4" r="E909"/>
+      <c s="3" r="E909"/>
     </row>
     <row r="910">
-      <c s="4" r="E910"/>
+      <c s="3" r="E910"/>
     </row>
     <row r="911">
-      <c s="4" r="E911"/>
+      <c s="3" r="E911"/>
     </row>
     <row r="912">
-      <c s="4" r="E912"/>
+      <c s="3" r="E912"/>
     </row>
     <row r="913">
-      <c s="4" r="E913"/>
+      <c s="3" r="E913"/>
     </row>
     <row r="914">
-      <c s="4" r="E914"/>
+      <c s="3" r="E914"/>
     </row>
     <row r="915">
-      <c s="4" r="E915"/>
+      <c s="3" r="E915"/>
     </row>
     <row r="916">
-      <c s="4" r="E916"/>
+      <c s="3" r="E916"/>
     </row>
     <row r="917">
-      <c s="4" r="E917"/>
+      <c s="3" r="E917"/>
     </row>
     <row r="918">
-      <c s="4" r="E918"/>
+      <c s="3" r="E918"/>
     </row>
     <row r="919">
-      <c s="4" r="E919"/>
+      <c s="3" r="E919"/>
     </row>
     <row r="920">
-      <c s="4" r="E920"/>
+      <c s="3" r="E920"/>
     </row>
     <row r="921">
-      <c s="4" r="E921"/>
+      <c s="3" r="E921"/>
     </row>
     <row r="922">
-      <c s="4" r="E922"/>
+      <c s="3" r="E922"/>
     </row>
     <row r="923">
-      <c s="4" r="E923"/>
+      <c s="3" r="E923"/>
     </row>
     <row r="924">
-      <c s="4" r="E924"/>
+      <c s="3" r="E924"/>
     </row>
     <row r="925">
-      <c s="4" r="E925"/>
+      <c s="3" r="E925"/>
     </row>
     <row r="926">
-      <c s="4" r="E926"/>
+      <c s="3" r="E926"/>
     </row>
     <row r="927">
-      <c s="4" r="E927"/>
+      <c s="3" r="E927"/>
     </row>
     <row r="928">
-      <c s="4" r="E928"/>
+      <c s="3" r="E928"/>
     </row>
     <row r="929">
-      <c s="4" r="E929"/>
+      <c s="3" r="E929"/>
     </row>
     <row r="930">
-      <c s="4" r="E930"/>
+      <c s="3" r="E930"/>
     </row>
     <row r="931">
-      <c s="4" r="E931"/>
+      <c s="3" r="E931"/>
     </row>
     <row r="932">
-      <c s="4" r="E932"/>
+      <c s="3" r="E932"/>
     </row>
     <row r="933">
-      <c s="4" r="E933"/>
+      <c s="3" r="E933"/>
     </row>
     <row r="934">
-      <c s="4" r="E934"/>
+      <c s="3" r="E934"/>
     </row>
     <row r="935">
-      <c s="4" r="E935"/>
+      <c s="3" r="E935"/>
     </row>
     <row r="936">
-      <c s="4" r="E936"/>
+      <c s="3" r="E936"/>
     </row>
     <row r="937">
-      <c s="4" r="E937"/>
+      <c s="3" r="E937"/>
     </row>
     <row r="938">
-      <c s="4" r="E938"/>
+      <c s="3" r="E938"/>
     </row>
     <row r="939">
-      <c s="4" r="E939"/>
+      <c s="3" r="E939"/>
     </row>
     <row r="940">
-      <c s="4" r="E940"/>
+      <c s="3" r="E940"/>
     </row>
     <row r="941">
-      <c s="4" r="E941"/>
+      <c s="3" r="E941"/>
     </row>
     <row r="942">
-      <c s="4" r="E942"/>
+      <c s="3" r="E942"/>
     </row>
     <row r="943">
-      <c s="4" r="E943"/>
+      <c s="3" r="E943"/>
     </row>
     <row r="944">
-      <c s="4" r="E944"/>
+      <c s="3" r="E944"/>
     </row>
     <row r="945">
-      <c s="4" r="E945"/>
+      <c s="3" r="E945"/>
     </row>
     <row r="946">
-      <c s="4" r="E946"/>
+      <c s="3" r="E946"/>
     </row>
     <row r="947">
-      <c s="4" r="E947"/>
+      <c s="3" r="E947"/>
     </row>
     <row r="948">
-      <c s="4" r="E948"/>
+      <c s="3" r="E948"/>
     </row>
     <row r="949">
-      <c s="4" r="E949"/>
+      <c s="3" r="E949"/>
     </row>
     <row r="950">
-      <c s="4" r="E950"/>
+      <c s="3" r="E950"/>
     </row>
     <row r="951">
-      <c s="4" r="E951"/>
+      <c s="3" r="E951"/>
     </row>
     <row r="952">
-      <c s="4" r="E952"/>
+      <c s="3" r="E952"/>
     </row>
     <row r="953">
-      <c s="4" r="E953"/>
+      <c s="3" r="E953"/>
     </row>
     <row r="954">
-      <c s="4" r="E954"/>
+      <c s="3" r="E954"/>
     </row>
     <row r="955">
-      <c s="4" r="E955"/>
+      <c s="3" r="E955"/>
     </row>
     <row r="956">
-      <c s="4" r="E956"/>
+      <c s="3" r="E956"/>
     </row>
     <row r="957">
-      <c s="4" r="E957"/>
+      <c s="3" r="E957"/>
     </row>
     <row r="958">
-      <c s="4" r="E958"/>
+      <c s="3" r="E958"/>
     </row>
     <row r="959">
-      <c s="4" r="E959"/>
+      <c s="3" r="E959"/>
     </row>
     <row r="960">
-      <c s="4" r="E960"/>
+      <c s="3" r="E960"/>
     </row>
     <row r="961">
-      <c s="4" r="E961"/>
+      <c s="3" r="E961"/>
     </row>
     <row r="962">
-      <c s="4" r="E962"/>
+      <c s="3" r="E962"/>
     </row>
     <row r="963">
-      <c s="4" r="E963"/>
+      <c s="3" r="E963"/>
     </row>
     <row r="964">
-      <c s="4" r="E964"/>
+      <c s="3" r="E964"/>
     </row>
     <row r="965">
-      <c s="4" r="E965"/>
+      <c s="3" r="E965"/>
     </row>
     <row r="966">
-      <c s="4" r="E966"/>
+      <c s="3" r="E966"/>
     </row>
     <row r="967">
-      <c s="4" r="E967"/>
+      <c s="3" r="E967"/>
     </row>
     <row r="968">
-      <c s="4" r="E968"/>
+      <c s="3" r="E968"/>
     </row>
     <row r="969">
-      <c s="4" r="E969"/>
+      <c s="3" r="E969"/>
     </row>
     <row r="970">
-      <c s="4" r="E970"/>
+      <c s="3" r="E970"/>
     </row>
     <row r="971">
-      <c s="4" r="E971"/>
+      <c s="3" r="E971"/>
     </row>
     <row r="972">
-      <c s="4" r="E972"/>
+      <c s="3" r="E972"/>
     </row>
     <row r="973">
-      <c s="4" r="E973"/>
+      <c s="3" r="E973"/>
     </row>
     <row r="974">
-      <c s="4" r="E974"/>
+      <c s="3" r="E974"/>
     </row>
     <row r="975">
-      <c s="4" r="E975"/>
+      <c s="3" r="E975"/>
     </row>
     <row r="976">
-      <c s="4" r="E976"/>
+      <c s="3" r="E976"/>
     </row>
     <row r="977">
-      <c s="4" r="E977"/>
+      <c s="3" r="E977"/>
     </row>
     <row r="978">
-      <c s="4" r="E978"/>
+      <c s="3" r="E978"/>
     </row>
     <row r="979">
-      <c s="4" r="E979"/>
+      <c s="3" r="E979"/>
     </row>
     <row r="980">
-      <c s="4" r="E980"/>
+      <c s="3" r="E980"/>
     </row>
     <row r="981">
-      <c s="4" r="E981"/>
+      <c s="3" r="E981"/>
     </row>
     <row r="982">
-      <c s="4" r="E982"/>
+      <c s="3" r="E982"/>
     </row>
     <row r="983">
-      <c s="4" r="E983"/>
+      <c s="3" r="E983"/>
     </row>
     <row r="984">
-      <c s="4" r="E984"/>
+      <c s="3" r="E984"/>
     </row>
     <row r="985">
-      <c s="4" r="E985"/>
+      <c s="3" r="E985"/>
     </row>
     <row r="986">
-      <c s="4" r="E986"/>
+      <c s="3" r="E986"/>
     </row>
     <row r="987">
-      <c s="4" r="E987"/>
+      <c s="3" r="E987"/>
     </row>
     <row r="988">
-      <c s="4" r="E988"/>
+      <c s="3" r="E988"/>
     </row>
     <row r="989">
-      <c s="4" r="E989"/>
+      <c s="3" r="E989"/>
     </row>
     <row r="990">
-      <c s="4" r="E990"/>
+      <c s="3" r="E990"/>
     </row>
     <row r="991">
-      <c s="4" r="E991"/>
+      <c s="3" r="E991"/>
     </row>
     <row r="992">
-      <c s="4" r="E992"/>
+      <c s="3" r="E992"/>
     </row>
     <row r="993">
-      <c s="4" r="E993"/>
+      <c s="3" r="E993"/>
     </row>
     <row r="994">
-      <c s="4" r="E994"/>
+      <c s="3" r="E994"/>
     </row>
     <row r="995">
-      <c s="4" r="E995"/>
+      <c s="3" r="E995"/>
     </row>
     <row r="996">
-      <c s="4" r="E996"/>
+      <c s="3" r="E996"/>
     </row>
     <row r="997">
-      <c s="4" r="E997"/>
+      <c s="3" r="E997"/>
     </row>
     <row r="998">
-      <c s="4" r="E998"/>
+      <c s="3" r="E998"/>
     </row>
     <row r="999">
-      <c s="4" r="E999"/>
+      <c s="3" r="E999"/>
     </row>
     <row r="1000">
-      <c s="4" r="E1000"/>
+      <c s="3" r="E1000"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
edit styles, add images, favicon, update google analytics code
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -14,12 +14,30 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
+    <t>Series</t>
+  </si>
+  <si>
     <t>HEADLINE</t>
   </si>
   <si>
+    <t>Subtitle</t>
+  </si>
+  <si>
+    <t>facebook_text</t>
+  </si>
+  <si>
     <t>LOCATION</t>
   </si>
   <si>
+    <t>twitter_text</t>
+  </si>
+  <si>
+    <t>State of Mind</t>
+  </si>
+  <si>
+    <t>Community Concerns Come to the Capitol</t>
+  </si>
+  <si>
     <t>YOUTUBE_ID</t>
   </si>
   <si>
@@ -29,13 +47,37 @@
     <t>DATE_PUBLISHED</t>
   </si>
   <si>
+    <t>TRIB_URL</t>
+  </si>
+  <si>
+    <t>MAP_IMG</t>
+  </si>
+  <si>
+    <t>RECAP??</t>
+  </si>
+  <si>
+    <t>TEXAS</t>
+  </si>
+  <si>
+    <t>sfODm7QGOlA</t>
+  </si>
+  <si>
+    <t>Members of the 84th Legislature will take on a variety of issues that affect communities across Texas. Our multimedia team traveled the state — as it did ahead of the 83rd Legislature — to see what’s important where. As we prepare to look ahead at issues facing the current Legislature in our State of Mind series, here’s a look back at how some of last session’s priorities played out.</t>
+  </si>
+  <si>
+    <t>Jan. 18, 2015</t>
+  </si>
+  <si>
+    <t>http://www.texastribune.org/2015/01/17/state-mind-issues-then-and-now/</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
     <t>A New Bid to End Texting While Driving</t>
   </si>
   <si>
-    <t>Texas</t>
-  </si>
-  <si>
-    <t>Series</t>
+    <t>College Station</t>
   </si>
   <si>
     <t>INV9hShE-Bg</t>
@@ -47,25 +89,58 @@
     <t>Jan. 20, 2015</t>
   </si>
   <si>
-    <t>Subtitle</t>
-  </si>
-  <si>
-    <t>facebook_text</t>
-  </si>
-  <si>
-    <t>twitter_text</t>
-  </si>
-  <si>
-    <t>State of Mind</t>
-  </si>
-  <si>
-    <t>Community Concerns Come to the Capitol</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur </t>
-  </si>
-  <si>
-    <t>College Station</t>
+    <t>http://www.texastribune.org/2015/01/20/state-mind-banning-texting-behind-wheel/</t>
+  </si>
+  <si>
+    <t>CollegeStation</t>
+  </si>
+  <si>
+    <t>Finding a Way to Cover the Uninsured</t>
+  </si>
+  <si>
+    <t>San Antonio</t>
+  </si>
+  <si>
+    <t>aU9PW5k-IWg</t>
+  </si>
+  <si>
+    <t>Texas hospitals want state lawmakers to figure out a way for the state to draw down billions in federal Affordable Care Act dollars to cover the uninsured and alleviate the burden on local taxpayers. Health officials hope the Legislature looks at a program in San Antonio that has the makings of a Texas solution.</t>
+  </si>
+  <si>
+    <t>Jan. 22, 2015</t>
+  </si>
+  <si>
+    <t>http://www.texastribune.org/2015/01/22/state-mind-finding-way-cover-uninsured/</t>
+  </si>
+  <si>
+    <t>SanAntonio</t>
+  </si>
+  <si>
+    <t>A Debate Over Fracking and Local Control</t>
+  </si>
+  <si>
+    <t>Mansfield</t>
+  </si>
+  <si>
+    <t>YPi6iSq77lc</t>
+  </si>
+  <si>
+    <t>After Denton voters decided to ban fracking, other Texas cities could weigh similar moves. Worried that Denton’s actions could lead to similar bans in other cities, state officials vowed more oversight of the oil and gas industry. And it’s caused some leaders and lawmakers to question exactly how "local control" should apply. </t>
+  </si>
+  <si>
+    <t>Jan. 23, 2015</t>
+  </si>
+  <si>
+    <t>http://www.texastribune.org/2015/01/23/regulating-local-control-oil-gas/</t>
+  </si>
+  <si>
+    <t>Mansfield</t>
+  </si>
+  <si>
+    <t>Hazelwood</t>
+  </si>
+  <si>
+    <t>San Marcos</t>
   </si>
   <si>
     <t>_XhNS2Vk9OQ</t>
@@ -74,13 +149,16 @@
     <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Sed at lectus et justo pharetra congue quis id arcu. Vestibulum feugiat lectus id urna accumsan tincidunt. Integer eleifend odio vitae nisi cursus convallis. </t>
   </si>
   <si>
-    <t>Jan. 20, 2015</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur </t>
-  </si>
-  <si>
-    <t>San Antonio</t>
+    <t>Jan. 27, 2015</t>
+  </si>
+  <si>
+    <t>SanMarcos</t>
+  </si>
+  <si>
+    <t>Lessons Learned from Ebola</t>
+  </si>
+  <si>
+    <t>Dallas</t>
   </si>
   <si>
     <t>_XhNS2Vk9OQ</t>
@@ -89,13 +167,16 @@
     <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Sed at lectus et justo pharetra congue quis id arcu. Vestibulum feugiat lectus id urna accumsan tincidunt. Integer eleifend odio vitae nisi cursus convallis. </t>
   </si>
   <si>
-    <t>Jan. 20, 2015</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur </t>
-  </si>
-  <si>
-    <t>Mansfield</t>
+    <t>Jan. 28, 2015</t>
+  </si>
+  <si>
+    <t>Dallas</t>
+  </si>
+  <si>
+    <t>Property Tax Reform</t>
+  </si>
+  <si>
+    <t>Beaumont</t>
   </si>
   <si>
     <t>_XhNS2Vk9OQ</t>
@@ -104,13 +185,16 @@
     <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Sed at lectus et justo pharetra congue quis id arcu. Vestibulum feugiat lectus id urna accumsan tincidunt. Integer eleifend odio vitae nisi cursus convallis. </t>
   </si>
   <si>
-    <t>Jan. 20, 2015</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur </t>
-  </si>
-  <si>
-    <t>Dallas</t>
+    <t>Jan. 29, 2015</t>
+  </si>
+  <si>
+    <t>Beaumont</t>
+  </si>
+  <si>
+    <t>PreK</t>
+  </si>
+  <si>
+    <t>Spring Branch</t>
   </si>
   <si>
     <t>_XhNS2Vk9OQ</t>
@@ -119,62 +203,23 @@
     <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Sed at lectus et justo pharetra congue quis id arcu. Vestibulum feugiat lectus id urna accumsan tincidunt. Integer eleifend odio vitae nisi cursus convallis. </t>
   </si>
   <si>
-    <t>Jan. 20, 2015</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur </t>
-  </si>
-  <si>
-    <t>Beaumont</t>
-  </si>
-  <si>
-    <t>_XhNS2Vk9OQ</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Sed at lectus et justo pharetra congue quis id arcu. Vestibulum feugiat lectus id urna accumsan tincidunt. Integer eleifend odio vitae nisi cursus convallis. </t>
-  </si>
-  <si>
-    <t>Jan. 20, 2015</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur </t>
-  </si>
-  <si>
-    <t>Spring Branch</t>
-  </si>
-  <si>
-    <t>_XhNS2Vk9OQ</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Sed at lectus et justo pharetra congue quis id arcu. Vestibulum feugiat lectus id urna accumsan tincidunt. Integer eleifend odio vitae nisi cursus convallis. </t>
-  </si>
-  <si>
-    <t>Jan. 20, 2015</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur </t>
-  </si>
-  <si>
-    <t>Waco</t>
-  </si>
-  <si>
-    <t>_XhNS2Vk9OQ</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Sed at lectus et justo pharetra congue quis id arcu. Vestibulum feugiat lectus id urna accumsan tincidunt. Integer eleifend odio vitae nisi cursus convallis. </t>
-  </si>
-  <si>
-    <t>Jan. 20, 2015</t>
+    <t>Jan. 30, 2015</t>
+  </si>
+  <si>
+    <t>SpringBranch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
     </font>
     <font/>
     <font>
@@ -185,7 +230,8 @@
       <sz val="10.0"/>
     </font>
     <font>
-      <b/>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
   </fonts>
   <fills count="2">
@@ -214,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
       <alignment/>
@@ -222,14 +268,24 @@
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
       <alignment/>
     </xf>
-    <xf fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1"/>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3">
       <alignment/>
     </xf>
+    <xf fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2"/>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="4">
       <alignment/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
+      <alignment/>
+    </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="5">
+      <alignment/>
+    </xf>
+    <xf fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2"/>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="4">
       <alignment/>
     </xf>
   </cellXfs>
@@ -260,25 +316,25 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c t="s" s="5" r="A1">
+      <c t="s" s="1" r="A1">
+        <v>0</v>
+      </c>
+      <c t="s" s="1" r="B1">
+        <v>2</v>
+      </c>
+      <c t="s" s="2" r="C1">
+        <v>3</v>
+      </c>
+      <c t="s" s="2" r="D1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c t="s" s="2" r="A2">
+        <v>6</v>
+      </c>
+      <c t="s" s="2" r="B2">
         <v>7</v>
-      </c>
-      <c t="s" s="5" r="B1">
-        <v>11</v>
-      </c>
-      <c t="s" s="1" r="C1">
-        <v>12</v>
-      </c>
-      <c t="s" s="1" r="D1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2">
-      <c t="s" s="1" r="A2">
-        <v>14</v>
-      </c>
-      <c t="s" s="1" r="B2">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -293,3136 +349,3186 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
+    <col min="1" customWidth="1" max="1" width="36.29"/>
+    <col min="4" customWidth="1" max="4" width="46.0"/>
     <col min="5" customWidth="1" max="5" width="17.57"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c t="s" s="1" r="A1">
-        <v>0</v>
-      </c>
-      <c t="s" s="2" r="B1">
+      <c t="s" s="2" r="A1">
         <v>1</v>
       </c>
-      <c t="s" s="1" r="C1">
-        <v>2</v>
-      </c>
-      <c t="s" s="1" r="D1">
-        <v>3</v>
-      </c>
-      <c t="s" s="3" r="E1">
+      <c t="s" s="3" r="B1">
         <v>4</v>
       </c>
+      <c t="s" s="2" r="C1">
+        <v>8</v>
+      </c>
+      <c t="s" s="2" r="D1">
+        <v>9</v>
+      </c>
+      <c t="s" s="4" r="E1">
+        <v>10</v>
+      </c>
+      <c t="s" s="2" r="F1">
+        <v>11</v>
+      </c>
+      <c t="s" s="2" r="G1">
+        <v>12</v>
+      </c>
     </row>
     <row r="2">
-      <c t="s" s="1" r="A2">
-        <v>5</v>
-      </c>
-      <c t="s" s="4" r="B2">
-        <v>6</v>
-      </c>
-      <c t="s" s="1" r="C2">
-        <v>8</v>
-      </c>
-      <c t="s" s="1" r="D2">
-        <v>9</v>
-      </c>
-      <c t="s" s="6" r="E2">
-        <v>10</v>
+      <c t="s" s="2" r="A2">
+        <v>13</v>
+      </c>
+      <c t="s" s="5" r="B2">
+        <v>14</v>
+      </c>
+      <c t="s" s="2" r="C2">
+        <v>15</v>
+      </c>
+      <c t="s" s="6" r="D2">
+        <v>16</v>
+      </c>
+      <c t="s" s="7" r="E2">
+        <v>17</v>
+      </c>
+      <c t="s" s="8" r="F2">
+        <v>18</v>
+      </c>
+      <c t="s" s="2" r="G2">
+        <v>19</v>
       </c>
     </row>
     <row r="3">
-      <c t="s" s="1" r="A3">
-        <v>16</v>
-      </c>
-      <c t="s" s="4" r="B3">
-        <v>17</v>
-      </c>
-      <c t="s" s="1" r="C3">
-        <v>18</v>
-      </c>
-      <c t="s" s="1" r="D3">
-        <v>19</v>
-      </c>
-      <c t="s" s="6" r="E3">
+      <c t="s" s="2" r="A3">
         <v>20</v>
       </c>
+      <c t="s" s="5" r="B3">
+        <v>21</v>
+      </c>
+      <c t="s" s="2" r="C3">
+        <v>22</v>
+      </c>
+      <c t="s" s="6" r="D3">
+        <v>23</v>
+      </c>
+      <c t="s" s="7" r="E3">
+        <v>24</v>
+      </c>
+      <c t="s" s="8" r="F3">
+        <v>25</v>
+      </c>
+      <c t="s" s="2" r="G3">
+        <v>26</v>
+      </c>
     </row>
     <row r="4">
-      <c t="s" s="1" r="A4">
-        <v>21</v>
-      </c>
-      <c t="s" s="4" r="B4">
-        <v>22</v>
-      </c>
-      <c t="s" s="1" r="C4">
-        <v>23</v>
-      </c>
-      <c t="s" s="1" r="D4">
-        <v>24</v>
-      </c>
-      <c t="s" s="6" r="E4">
-        <v>25</v>
+      <c t="s" s="9" r="A4">
+        <v>27</v>
+      </c>
+      <c t="s" s="10" r="B4">
+        <v>28</v>
+      </c>
+      <c t="s" s="2" r="C4">
+        <v>29</v>
+      </c>
+      <c t="s" s="6" r="D4">
+        <v>30</v>
+      </c>
+      <c t="s" s="4" r="E4">
+        <v>31</v>
+      </c>
+      <c t="s" s="8" r="F4">
+        <v>32</v>
+      </c>
+      <c t="s" s="2" r="G4">
+        <v>33</v>
       </c>
     </row>
     <row r="5">
-      <c t="s" s="1" r="A5">
-        <v>26</v>
-      </c>
-      <c t="s" s="4" r="B5">
-        <v>27</v>
-      </c>
-      <c t="s" s="1" r="C5">
-        <v>28</v>
-      </c>
-      <c t="s" s="1" r="D5">
-        <v>29</v>
-      </c>
-      <c t="s" s="6" r="E5">
-        <v>30</v>
+      <c t="s" s="2" r="A5">
+        <v>34</v>
+      </c>
+      <c t="s" s="2" r="B5">
+        <v>35</v>
+      </c>
+      <c t="s" s="2" r="C5">
+        <v>36</v>
+      </c>
+      <c t="s" s="6" r="D5">
+        <v>37</v>
+      </c>
+      <c t="s" s="7" r="E5">
+        <v>38</v>
+      </c>
+      <c t="s" s="8" r="F5">
+        <v>39</v>
+      </c>
+      <c t="s" s="2" r="G5">
+        <v>40</v>
       </c>
     </row>
     <row r="6">
-      <c t="s" s="1" r="A6">
-        <v>31</v>
-      </c>
-      <c t="s" s="4" r="B6">
-        <v>32</v>
-      </c>
-      <c t="s" s="1" r="C6">
-        <v>33</v>
-      </c>
-      <c t="s" s="1" r="D6">
-        <v>34</v>
-      </c>
-      <c t="s" s="6" r="E6">
-        <v>35</v>
+      <c t="s" s="2" r="A6">
+        <v>41</v>
+      </c>
+      <c t="s" s="5" r="B6">
+        <v>42</v>
+      </c>
+      <c t="s" s="2" r="C6">
+        <v>43</v>
+      </c>
+      <c t="s" s="6" r="D6">
+        <v>44</v>
+      </c>
+      <c t="s" s="7" r="E6">
+        <v>45</v>
+      </c>
+      <c t="s" s="2" r="G6">
+        <v>46</v>
       </c>
     </row>
     <row r="7">
-      <c t="s" s="1" r="A7">
-        <v>36</v>
-      </c>
-      <c t="s" s="4" r="B7">
-        <v>37</v>
-      </c>
-      <c t="s" s="1" r="C7">
-        <v>38</v>
-      </c>
-      <c t="s" s="1" r="D7">
-        <v>39</v>
-      </c>
-      <c t="s" s="6" r="E7">
-        <v>40</v>
+      <c t="s" s="2" r="A7">
+        <v>47</v>
+      </c>
+      <c t="s" s="10" r="B7">
+        <v>48</v>
+      </c>
+      <c t="s" s="2" r="C7">
+        <v>49</v>
+      </c>
+      <c t="s" s="6" r="D7">
+        <v>50</v>
+      </c>
+      <c t="s" s="7" r="E7">
+        <v>51</v>
+      </c>
+      <c t="s" s="2" r="G7">
+        <v>52</v>
       </c>
     </row>
     <row r="8">
-      <c t="s" s="1" r="A8">
-        <v>41</v>
-      </c>
-      <c t="s" s="4" r="B8">
-        <v>42</v>
-      </c>
-      <c t="s" s="1" r="C8">
-        <v>43</v>
-      </c>
-      <c t="s" s="1" r="D8">
-        <v>44</v>
-      </c>
-      <c t="s" s="6" r="E8">
-        <v>45</v>
+      <c t="s" s="2" r="A8">
+        <v>53</v>
+      </c>
+      <c t="s" s="10" r="B8">
+        <v>54</v>
+      </c>
+      <c t="s" s="2" r="C8">
+        <v>55</v>
+      </c>
+      <c t="s" s="6" r="D8">
+        <v>56</v>
+      </c>
+      <c t="s" s="7" r="E8">
+        <v>57</v>
+      </c>
+      <c t="s" s="2" r="G8">
+        <v>58</v>
       </c>
     </row>
     <row r="9">
-      <c t="s" s="1" r="A9">
-        <v>46</v>
-      </c>
-      <c t="s" s="4" r="B9">
-        <v>47</v>
-      </c>
-      <c t="s" s="1" r="C9">
-        <v>48</v>
-      </c>
-      <c t="s" s="1" r="D9">
-        <v>49</v>
-      </c>
-      <c t="s" s="6" r="E9">
-        <v>50</v>
+      <c t="s" s="2" r="A9">
+        <v>59</v>
+      </c>
+      <c t="s" s="10" r="B9">
+        <v>60</v>
+      </c>
+      <c t="s" s="2" r="C9">
+        <v>61</v>
+      </c>
+      <c t="s" s="6" r="D9">
+        <v>62</v>
+      </c>
+      <c t="s" s="7" r="E9">
+        <v>63</v>
+      </c>
+      <c t="s" s="2" r="G9">
+        <v>64</v>
       </c>
     </row>
     <row r="10">
-      <c s="3" r="E10"/>
+      <c s="4" r="E10"/>
     </row>
     <row r="11">
-      <c s="3" r="E11"/>
+      <c s="4" r="E11"/>
     </row>
     <row r="12">
-      <c s="3" r="E12"/>
+      <c s="4" r="E12"/>
     </row>
     <row r="13">
-      <c s="3" r="E13"/>
+      <c s="4" r="E13"/>
     </row>
     <row r="14">
-      <c s="3" r="E14"/>
+      <c s="4" r="E14"/>
     </row>
     <row r="15">
-      <c s="3" r="E15"/>
+      <c s="4" r="E15"/>
     </row>
     <row r="16">
-      <c s="3" r="E16"/>
+      <c s="4" r="E16"/>
     </row>
     <row r="17">
-      <c s="3" r="E17"/>
+      <c s="4" r="E17"/>
     </row>
     <row r="18">
-      <c s="3" r="E18"/>
+      <c s="4" r="E18"/>
     </row>
     <row r="19">
-      <c s="3" r="E19"/>
+      <c s="4" r="E19"/>
     </row>
     <row r="20">
-      <c s="3" r="E20"/>
+      <c s="4" r="E20"/>
     </row>
     <row r="21">
-      <c s="3" r="E21"/>
+      <c s="4" r="E21"/>
     </row>
     <row r="22">
-      <c s="3" r="E22"/>
+      <c s="4" r="E22"/>
     </row>
     <row r="23">
-      <c s="3" r="E23"/>
+      <c s="4" r="E23"/>
     </row>
     <row r="24">
-      <c s="3" r="E24"/>
+      <c s="4" r="E24"/>
     </row>
     <row r="25">
-      <c s="3" r="E25"/>
+      <c s="4" r="E25"/>
     </row>
     <row r="26">
-      <c s="3" r="E26"/>
+      <c s="4" r="E26"/>
     </row>
     <row r="27">
-      <c s="3" r="E27"/>
+      <c s="4" r="E27"/>
     </row>
     <row r="28">
-      <c s="3" r="E28"/>
+      <c s="4" r="E28"/>
     </row>
     <row r="29">
-      <c s="3" r="E29"/>
+      <c s="4" r="E29"/>
     </row>
     <row r="30">
-      <c s="3" r="E30"/>
+      <c s="4" r="E30"/>
     </row>
     <row r="31">
-      <c s="3" r="E31"/>
+      <c s="4" r="E31"/>
     </row>
     <row r="32">
-      <c s="3" r="E32"/>
+      <c s="4" r="E32"/>
     </row>
     <row r="33">
-      <c s="3" r="E33"/>
+      <c s="4" r="E33"/>
     </row>
     <row r="34">
-      <c s="3" r="E34"/>
+      <c s="4" r="E34"/>
     </row>
     <row r="35">
-      <c s="3" r="E35"/>
+      <c s="4" r="E35"/>
     </row>
     <row r="36">
-      <c s="3" r="E36"/>
+      <c s="4" r="E36"/>
     </row>
     <row r="37">
-      <c s="3" r="E37"/>
+      <c s="4" r="E37"/>
     </row>
     <row r="38">
-      <c s="3" r="E38"/>
+      <c s="4" r="E38"/>
     </row>
     <row r="39">
-      <c s="3" r="E39"/>
+      <c s="4" r="E39"/>
     </row>
     <row r="40">
-      <c s="3" r="E40"/>
+      <c s="4" r="E40"/>
     </row>
     <row r="41">
-      <c s="3" r="E41"/>
+      <c s="4" r="E41"/>
     </row>
     <row r="42">
-      <c s="3" r="E42"/>
+      <c s="4" r="E42"/>
     </row>
     <row r="43">
-      <c s="3" r="E43"/>
+      <c s="4" r="E43"/>
     </row>
     <row r="44">
-      <c s="3" r="E44"/>
+      <c s="4" r="E44"/>
     </row>
     <row r="45">
-      <c s="3" r="E45"/>
+      <c s="4" r="E45"/>
     </row>
     <row r="46">
-      <c s="3" r="E46"/>
+      <c s="4" r="E46"/>
     </row>
     <row r="47">
-      <c s="3" r="E47"/>
+      <c s="4" r="E47"/>
     </row>
     <row r="48">
-      <c s="3" r="E48"/>
+      <c s="4" r="E48"/>
     </row>
     <row r="49">
-      <c s="3" r="E49"/>
+      <c s="4" r="E49"/>
     </row>
     <row r="50">
-      <c s="3" r="E50"/>
+      <c s="4" r="E50"/>
     </row>
     <row r="51">
-      <c s="3" r="E51"/>
+      <c s="4" r="E51"/>
     </row>
     <row r="52">
-      <c s="3" r="E52"/>
+      <c s="4" r="E52"/>
     </row>
     <row r="53">
-      <c s="3" r="E53"/>
+      <c s="4" r="E53"/>
     </row>
     <row r="54">
-      <c s="3" r="E54"/>
+      <c s="4" r="E54"/>
     </row>
     <row r="55">
-      <c s="3" r="E55"/>
+      <c s="4" r="E55"/>
     </row>
     <row r="56">
-      <c s="3" r="E56"/>
+      <c s="4" r="E56"/>
     </row>
     <row r="57">
-      <c s="3" r="E57"/>
+      <c s="4" r="E57"/>
     </row>
     <row r="58">
-      <c s="3" r="E58"/>
+      <c s="4" r="E58"/>
     </row>
     <row r="59">
-      <c s="3" r="E59"/>
+      <c s="4" r="E59"/>
     </row>
     <row r="60">
-      <c s="3" r="E60"/>
+      <c s="4" r="E60"/>
     </row>
     <row r="61">
-      <c s="3" r="E61"/>
+      <c s="4" r="E61"/>
     </row>
     <row r="62">
-      <c s="3" r="E62"/>
+      <c s="4" r="E62"/>
     </row>
     <row r="63">
-      <c s="3" r="E63"/>
+      <c s="4" r="E63"/>
     </row>
     <row r="64">
-      <c s="3" r="E64"/>
+      <c s="4" r="E64"/>
     </row>
     <row r="65">
-      <c s="3" r="E65"/>
+      <c s="4" r="E65"/>
     </row>
     <row r="66">
-      <c s="3" r="E66"/>
+      <c s="4" r="E66"/>
     </row>
     <row r="67">
-      <c s="3" r="E67"/>
+      <c s="4" r="E67"/>
     </row>
     <row r="68">
-      <c s="3" r="E68"/>
+      <c s="4" r="E68"/>
     </row>
     <row r="69">
-      <c s="3" r="E69"/>
+      <c s="4" r="E69"/>
     </row>
     <row r="70">
-      <c s="3" r="E70"/>
+      <c s="4" r="E70"/>
     </row>
     <row r="71">
-      <c s="3" r="E71"/>
+      <c s="4" r="E71"/>
     </row>
     <row r="72">
-      <c s="3" r="E72"/>
+      <c s="4" r="E72"/>
     </row>
     <row r="73">
-      <c s="3" r="E73"/>
+      <c s="4" r="E73"/>
     </row>
     <row r="74">
-      <c s="3" r="E74"/>
+      <c s="4" r="E74"/>
     </row>
     <row r="75">
-      <c s="3" r="E75"/>
+      <c s="4" r="E75"/>
     </row>
     <row r="76">
-      <c s="3" r="E76"/>
+      <c s="4" r="E76"/>
     </row>
     <row r="77">
-      <c s="3" r="E77"/>
+      <c s="4" r="E77"/>
     </row>
     <row r="78">
-      <c s="3" r="E78"/>
+      <c s="4" r="E78"/>
     </row>
     <row r="79">
-      <c s="3" r="E79"/>
+      <c s="4" r="E79"/>
     </row>
     <row r="80">
-      <c s="3" r="E80"/>
+      <c s="4" r="E80"/>
     </row>
     <row r="81">
-      <c s="3" r="E81"/>
+      <c s="4" r="E81"/>
     </row>
     <row r="82">
-      <c s="3" r="E82"/>
+      <c s="4" r="E82"/>
     </row>
     <row r="83">
-      <c s="3" r="E83"/>
+      <c s="4" r="E83"/>
     </row>
     <row r="84">
-      <c s="3" r="E84"/>
+      <c s="4" r="E84"/>
     </row>
     <row r="85">
-      <c s="3" r="E85"/>
+      <c s="4" r="E85"/>
     </row>
     <row r="86">
-      <c s="3" r="E86"/>
+      <c s="4" r="E86"/>
     </row>
     <row r="87">
-      <c s="3" r="E87"/>
+      <c s="4" r="E87"/>
     </row>
     <row r="88">
-      <c s="3" r="E88"/>
+      <c s="4" r="E88"/>
     </row>
     <row r="89">
-      <c s="3" r="E89"/>
+      <c s="4" r="E89"/>
     </row>
     <row r="90">
-      <c s="3" r="E90"/>
+      <c s="4" r="E90"/>
     </row>
     <row r="91">
-      <c s="3" r="E91"/>
+      <c s="4" r="E91"/>
     </row>
     <row r="92">
-      <c s="3" r="E92"/>
+      <c s="4" r="E92"/>
     </row>
     <row r="93">
-      <c s="3" r="E93"/>
+      <c s="4" r="E93"/>
     </row>
     <row r="94">
-      <c s="3" r="E94"/>
+      <c s="4" r="E94"/>
     </row>
     <row r="95">
-      <c s="3" r="E95"/>
+      <c s="4" r="E95"/>
     </row>
     <row r="96">
-      <c s="3" r="E96"/>
+      <c s="4" r="E96"/>
     </row>
     <row r="97">
-      <c s="3" r="E97"/>
+      <c s="4" r="E97"/>
     </row>
     <row r="98">
-      <c s="3" r="E98"/>
+      <c s="4" r="E98"/>
     </row>
     <row r="99">
-      <c s="3" r="E99"/>
+      <c s="4" r="E99"/>
     </row>
     <row r="100">
-      <c s="3" r="E100"/>
+      <c s="4" r="E100"/>
     </row>
     <row r="101">
-      <c s="3" r="E101"/>
+      <c s="4" r="E101"/>
     </row>
     <row r="102">
-      <c s="3" r="E102"/>
+      <c s="4" r="E102"/>
     </row>
     <row r="103">
-      <c s="3" r="E103"/>
+      <c s="4" r="E103"/>
     </row>
     <row r="104">
-      <c s="3" r="E104"/>
+      <c s="4" r="E104"/>
     </row>
     <row r="105">
-      <c s="3" r="E105"/>
+      <c s="4" r="E105"/>
     </row>
     <row r="106">
-      <c s="3" r="E106"/>
+      <c s="4" r="E106"/>
     </row>
     <row r="107">
-      <c s="3" r="E107"/>
+      <c s="4" r="E107"/>
     </row>
     <row r="108">
-      <c s="3" r="E108"/>
+      <c s="4" r="E108"/>
     </row>
     <row r="109">
-      <c s="3" r="E109"/>
+      <c s="4" r="E109"/>
     </row>
     <row r="110">
-      <c s="3" r="E110"/>
+      <c s="4" r="E110"/>
     </row>
     <row r="111">
-      <c s="3" r="E111"/>
+      <c s="4" r="E111"/>
     </row>
     <row r="112">
-      <c s="3" r="E112"/>
+      <c s="4" r="E112"/>
     </row>
     <row r="113">
-      <c s="3" r="E113"/>
+      <c s="4" r="E113"/>
     </row>
     <row r="114">
-      <c s="3" r="E114"/>
+      <c s="4" r="E114"/>
     </row>
     <row r="115">
-      <c s="3" r="E115"/>
+      <c s="4" r="E115"/>
     </row>
     <row r="116">
-      <c s="3" r="E116"/>
+      <c s="4" r="E116"/>
     </row>
     <row r="117">
-      <c s="3" r="E117"/>
+      <c s="4" r="E117"/>
     </row>
     <row r="118">
-      <c s="3" r="E118"/>
+      <c s="4" r="E118"/>
     </row>
     <row r="119">
-      <c s="3" r="E119"/>
+      <c s="4" r="E119"/>
     </row>
     <row r="120">
-      <c s="3" r="E120"/>
+      <c s="4" r="E120"/>
     </row>
     <row r="121">
-      <c s="3" r="E121"/>
+      <c s="4" r="E121"/>
     </row>
     <row r="122">
-      <c s="3" r="E122"/>
+      <c s="4" r="E122"/>
     </row>
     <row r="123">
-      <c s="3" r="E123"/>
+      <c s="4" r="E123"/>
     </row>
     <row r="124">
-      <c s="3" r="E124"/>
+      <c s="4" r="E124"/>
     </row>
     <row r="125">
-      <c s="3" r="E125"/>
+      <c s="4" r="E125"/>
     </row>
     <row r="126">
-      <c s="3" r="E126"/>
+      <c s="4" r="E126"/>
     </row>
     <row r="127">
-      <c s="3" r="E127"/>
+      <c s="4" r="E127"/>
     </row>
     <row r="128">
-      <c s="3" r="E128"/>
+      <c s="4" r="E128"/>
     </row>
     <row r="129">
-      <c s="3" r="E129"/>
+      <c s="4" r="E129"/>
     </row>
     <row r="130">
-      <c s="3" r="E130"/>
+      <c s="4" r="E130"/>
     </row>
     <row r="131">
-      <c s="3" r="E131"/>
+      <c s="4" r="E131"/>
     </row>
     <row r="132">
-      <c s="3" r="E132"/>
+      <c s="4" r="E132"/>
     </row>
     <row r="133">
-      <c s="3" r="E133"/>
+      <c s="4" r="E133"/>
     </row>
     <row r="134">
-      <c s="3" r="E134"/>
+      <c s="4" r="E134"/>
     </row>
     <row r="135">
-      <c s="3" r="E135"/>
+      <c s="4" r="E135"/>
     </row>
     <row r="136">
-      <c s="3" r="E136"/>
+      <c s="4" r="E136"/>
     </row>
     <row r="137">
-      <c s="3" r="E137"/>
+      <c s="4" r="E137"/>
     </row>
     <row r="138">
-      <c s="3" r="E138"/>
+      <c s="4" r="E138"/>
     </row>
     <row r="139">
-      <c s="3" r="E139"/>
+      <c s="4" r="E139"/>
     </row>
     <row r="140">
-      <c s="3" r="E140"/>
+      <c s="4" r="E140"/>
     </row>
     <row r="141">
-      <c s="3" r="E141"/>
+      <c s="4" r="E141"/>
     </row>
     <row r="142">
-      <c s="3" r="E142"/>
+      <c s="4" r="E142"/>
     </row>
     <row r="143">
-      <c s="3" r="E143"/>
+      <c s="4" r="E143"/>
     </row>
     <row r="144">
-      <c s="3" r="E144"/>
+      <c s="4" r="E144"/>
     </row>
     <row r="145">
-      <c s="3" r="E145"/>
+      <c s="4" r="E145"/>
     </row>
     <row r="146">
-      <c s="3" r="E146"/>
+      <c s="4" r="E146"/>
     </row>
     <row r="147">
-      <c s="3" r="E147"/>
+      <c s="4" r="E147"/>
     </row>
     <row r="148">
-      <c s="3" r="E148"/>
+      <c s="4" r="E148"/>
     </row>
     <row r="149">
-      <c s="3" r="E149"/>
+      <c s="4" r="E149"/>
     </row>
     <row r="150">
-      <c s="3" r="E150"/>
+      <c s="4" r="E150"/>
     </row>
     <row r="151">
-      <c s="3" r="E151"/>
+      <c s="4" r="E151"/>
     </row>
     <row r="152">
-      <c s="3" r="E152"/>
+      <c s="4" r="E152"/>
     </row>
     <row r="153">
-      <c s="3" r="E153"/>
+      <c s="4" r="E153"/>
     </row>
     <row r="154">
-      <c s="3" r="E154"/>
+      <c s="4" r="E154"/>
     </row>
     <row r="155">
-      <c s="3" r="E155"/>
+      <c s="4" r="E155"/>
     </row>
     <row r="156">
-      <c s="3" r="E156"/>
+      <c s="4" r="E156"/>
     </row>
     <row r="157">
-      <c s="3" r="E157"/>
+      <c s="4" r="E157"/>
     </row>
     <row r="158">
-      <c s="3" r="E158"/>
+      <c s="4" r="E158"/>
     </row>
     <row r="159">
-      <c s="3" r="E159"/>
+      <c s="4" r="E159"/>
     </row>
     <row r="160">
-      <c s="3" r="E160"/>
+      <c s="4" r="E160"/>
     </row>
     <row r="161">
-      <c s="3" r="E161"/>
+      <c s="4" r="E161"/>
     </row>
     <row r="162">
-      <c s="3" r="E162"/>
+      <c s="4" r="E162"/>
     </row>
     <row r="163">
-      <c s="3" r="E163"/>
+      <c s="4" r="E163"/>
     </row>
     <row r="164">
-      <c s="3" r="E164"/>
+      <c s="4" r="E164"/>
     </row>
     <row r="165">
-      <c s="3" r="E165"/>
+      <c s="4" r="E165"/>
     </row>
     <row r="166">
-      <c s="3" r="E166"/>
+      <c s="4" r="E166"/>
     </row>
     <row r="167">
-      <c s="3" r="E167"/>
+      <c s="4" r="E167"/>
     </row>
     <row r="168">
-      <c s="3" r="E168"/>
+      <c s="4" r="E168"/>
     </row>
     <row r="169">
-      <c s="3" r="E169"/>
+      <c s="4" r="E169"/>
     </row>
     <row r="170">
-      <c s="3" r="E170"/>
+      <c s="4" r="E170"/>
     </row>
     <row r="171">
-      <c s="3" r="E171"/>
+      <c s="4" r="E171"/>
     </row>
     <row r="172">
-      <c s="3" r="E172"/>
+      <c s="4" r="E172"/>
     </row>
     <row r="173">
-      <c s="3" r="E173"/>
+      <c s="4" r="E173"/>
     </row>
     <row r="174">
-      <c s="3" r="E174"/>
+      <c s="4" r="E174"/>
     </row>
     <row r="175">
-      <c s="3" r="E175"/>
+      <c s="4" r="E175"/>
     </row>
     <row r="176">
-      <c s="3" r="E176"/>
+      <c s="4" r="E176"/>
     </row>
     <row r="177">
-      <c s="3" r="E177"/>
+      <c s="4" r="E177"/>
     </row>
     <row r="178">
-      <c s="3" r="E178"/>
+      <c s="4" r="E178"/>
     </row>
     <row r="179">
-      <c s="3" r="E179"/>
+      <c s="4" r="E179"/>
     </row>
     <row r="180">
-      <c s="3" r="E180"/>
+      <c s="4" r="E180"/>
     </row>
     <row r="181">
-      <c s="3" r="E181"/>
+      <c s="4" r="E181"/>
     </row>
     <row r="182">
-      <c s="3" r="E182"/>
+      <c s="4" r="E182"/>
     </row>
     <row r="183">
-      <c s="3" r="E183"/>
+      <c s="4" r="E183"/>
     </row>
     <row r="184">
-      <c s="3" r="E184"/>
+      <c s="4" r="E184"/>
     </row>
     <row r="185">
-      <c s="3" r="E185"/>
+      <c s="4" r="E185"/>
     </row>
     <row r="186">
-      <c s="3" r="E186"/>
+      <c s="4" r="E186"/>
     </row>
     <row r="187">
-      <c s="3" r="E187"/>
+      <c s="4" r="E187"/>
     </row>
     <row r="188">
-      <c s="3" r="E188"/>
+      <c s="4" r="E188"/>
     </row>
     <row r="189">
-      <c s="3" r="E189"/>
+      <c s="4" r="E189"/>
     </row>
     <row r="190">
-      <c s="3" r="E190"/>
+      <c s="4" r="E190"/>
     </row>
     <row r="191">
-      <c s="3" r="E191"/>
+      <c s="4" r="E191"/>
     </row>
     <row r="192">
-      <c s="3" r="E192"/>
+      <c s="4" r="E192"/>
     </row>
     <row r="193">
-      <c s="3" r="E193"/>
+      <c s="4" r="E193"/>
     </row>
     <row r="194">
-      <c s="3" r="E194"/>
+      <c s="4" r="E194"/>
     </row>
     <row r="195">
-      <c s="3" r="E195"/>
+      <c s="4" r="E195"/>
     </row>
     <row r="196">
-      <c s="3" r="E196"/>
+      <c s="4" r="E196"/>
     </row>
     <row r="197">
-      <c s="3" r="E197"/>
+      <c s="4" r="E197"/>
     </row>
     <row r="198">
-      <c s="3" r="E198"/>
+      <c s="4" r="E198"/>
     </row>
     <row r="199">
-      <c s="3" r="E199"/>
+      <c s="4" r="E199"/>
     </row>
     <row r="200">
-      <c s="3" r="E200"/>
+      <c s="4" r="E200"/>
     </row>
     <row r="201">
-      <c s="3" r="E201"/>
+      <c s="4" r="E201"/>
     </row>
     <row r="202">
-      <c s="3" r="E202"/>
+      <c s="4" r="E202"/>
     </row>
     <row r="203">
-      <c s="3" r="E203"/>
+      <c s="4" r="E203"/>
     </row>
     <row r="204">
-      <c s="3" r="E204"/>
+      <c s="4" r="E204"/>
     </row>
     <row r="205">
-      <c s="3" r="E205"/>
+      <c s="4" r="E205"/>
     </row>
     <row r="206">
-      <c s="3" r="E206"/>
+      <c s="4" r="E206"/>
     </row>
     <row r="207">
-      <c s="3" r="E207"/>
+      <c s="4" r="E207"/>
     </row>
     <row r="208">
-      <c s="3" r="E208"/>
+      <c s="4" r="E208"/>
     </row>
     <row r="209">
-      <c s="3" r="E209"/>
+      <c s="4" r="E209"/>
     </row>
     <row r="210">
-      <c s="3" r="E210"/>
+      <c s="4" r="E210"/>
     </row>
     <row r="211">
-      <c s="3" r="E211"/>
+      <c s="4" r="E211"/>
     </row>
     <row r="212">
-      <c s="3" r="E212"/>
+      <c s="4" r="E212"/>
     </row>
     <row r="213">
-      <c s="3" r="E213"/>
+      <c s="4" r="E213"/>
     </row>
     <row r="214">
-      <c s="3" r="E214"/>
+      <c s="4" r="E214"/>
     </row>
     <row r="215">
-      <c s="3" r="E215"/>
+      <c s="4" r="E215"/>
     </row>
     <row r="216">
-      <c s="3" r="E216"/>
+      <c s="4" r="E216"/>
     </row>
     <row r="217">
-      <c s="3" r="E217"/>
+      <c s="4" r="E217"/>
     </row>
     <row r="218">
-      <c s="3" r="E218"/>
+      <c s="4" r="E218"/>
     </row>
     <row r="219">
-      <c s="3" r="E219"/>
+      <c s="4" r="E219"/>
     </row>
     <row r="220">
-      <c s="3" r="E220"/>
+      <c s="4" r="E220"/>
     </row>
     <row r="221">
-      <c s="3" r="E221"/>
+      <c s="4" r="E221"/>
     </row>
     <row r="222">
-      <c s="3" r="E222"/>
+      <c s="4" r="E222"/>
     </row>
     <row r="223">
-      <c s="3" r="E223"/>
+      <c s="4" r="E223"/>
     </row>
     <row r="224">
-      <c s="3" r="E224"/>
+      <c s="4" r="E224"/>
     </row>
     <row r="225">
-      <c s="3" r="E225"/>
+      <c s="4" r="E225"/>
     </row>
     <row r="226">
-      <c s="3" r="E226"/>
+      <c s="4" r="E226"/>
     </row>
     <row r="227">
-      <c s="3" r="E227"/>
+      <c s="4" r="E227"/>
     </row>
     <row r="228">
-      <c s="3" r="E228"/>
+      <c s="4" r="E228"/>
     </row>
     <row r="229">
-      <c s="3" r="E229"/>
+      <c s="4" r="E229"/>
     </row>
     <row r="230">
-      <c s="3" r="E230"/>
+      <c s="4" r="E230"/>
     </row>
     <row r="231">
-      <c s="3" r="E231"/>
+      <c s="4" r="E231"/>
     </row>
     <row r="232">
-      <c s="3" r="E232"/>
+      <c s="4" r="E232"/>
     </row>
     <row r="233">
-      <c s="3" r="E233"/>
+      <c s="4" r="E233"/>
     </row>
     <row r="234">
-      <c s="3" r="E234"/>
+      <c s="4" r="E234"/>
     </row>
     <row r="235">
-      <c s="3" r="E235"/>
+      <c s="4" r="E235"/>
     </row>
     <row r="236">
-      <c s="3" r="E236"/>
+      <c s="4" r="E236"/>
     </row>
     <row r="237">
-      <c s="3" r="E237"/>
+      <c s="4" r="E237"/>
     </row>
     <row r="238">
-      <c s="3" r="E238"/>
+      <c s="4" r="E238"/>
     </row>
     <row r="239">
-      <c s="3" r="E239"/>
+      <c s="4" r="E239"/>
     </row>
     <row r="240">
-      <c s="3" r="E240"/>
+      <c s="4" r="E240"/>
     </row>
     <row r="241">
-      <c s="3" r="E241"/>
+      <c s="4" r="E241"/>
     </row>
     <row r="242">
-      <c s="3" r="E242"/>
+      <c s="4" r="E242"/>
     </row>
     <row r="243">
-      <c s="3" r="E243"/>
+      <c s="4" r="E243"/>
     </row>
     <row r="244">
-      <c s="3" r="E244"/>
+      <c s="4" r="E244"/>
     </row>
     <row r="245">
-      <c s="3" r="E245"/>
+      <c s="4" r="E245"/>
     </row>
     <row r="246">
-      <c s="3" r="E246"/>
+      <c s="4" r="E246"/>
     </row>
     <row r="247">
-      <c s="3" r="E247"/>
+      <c s="4" r="E247"/>
     </row>
     <row r="248">
-      <c s="3" r="E248"/>
+      <c s="4" r="E248"/>
     </row>
     <row r="249">
-      <c s="3" r="E249"/>
+      <c s="4" r="E249"/>
     </row>
     <row r="250">
-      <c s="3" r="E250"/>
+      <c s="4" r="E250"/>
     </row>
     <row r="251">
-      <c s="3" r="E251"/>
+      <c s="4" r="E251"/>
     </row>
     <row r="252">
-      <c s="3" r="E252"/>
+      <c s="4" r="E252"/>
     </row>
     <row r="253">
-      <c s="3" r="E253"/>
+      <c s="4" r="E253"/>
     </row>
     <row r="254">
-      <c s="3" r="E254"/>
+      <c s="4" r="E254"/>
     </row>
     <row r="255">
-      <c s="3" r="E255"/>
+      <c s="4" r="E255"/>
     </row>
     <row r="256">
-      <c s="3" r="E256"/>
+      <c s="4" r="E256"/>
     </row>
     <row r="257">
-      <c s="3" r="E257"/>
+      <c s="4" r="E257"/>
     </row>
     <row r="258">
-      <c s="3" r="E258"/>
+      <c s="4" r="E258"/>
     </row>
     <row r="259">
-      <c s="3" r="E259"/>
+      <c s="4" r="E259"/>
     </row>
     <row r="260">
-      <c s="3" r="E260"/>
+      <c s="4" r="E260"/>
     </row>
     <row r="261">
-      <c s="3" r="E261"/>
+      <c s="4" r="E261"/>
     </row>
     <row r="262">
-      <c s="3" r="E262"/>
+      <c s="4" r="E262"/>
     </row>
     <row r="263">
-      <c s="3" r="E263"/>
+      <c s="4" r="E263"/>
     </row>
     <row r="264">
-      <c s="3" r="E264"/>
+      <c s="4" r="E264"/>
     </row>
     <row r="265">
-      <c s="3" r="E265"/>
+      <c s="4" r="E265"/>
     </row>
     <row r="266">
-      <c s="3" r="E266"/>
+      <c s="4" r="E266"/>
     </row>
     <row r="267">
-      <c s="3" r="E267"/>
+      <c s="4" r="E267"/>
     </row>
     <row r="268">
-      <c s="3" r="E268"/>
+      <c s="4" r="E268"/>
     </row>
     <row r="269">
-      <c s="3" r="E269"/>
+      <c s="4" r="E269"/>
     </row>
     <row r="270">
-      <c s="3" r="E270"/>
+      <c s="4" r="E270"/>
     </row>
     <row r="271">
-      <c s="3" r="E271"/>
+      <c s="4" r="E271"/>
     </row>
     <row r="272">
-      <c s="3" r="E272"/>
+      <c s="4" r="E272"/>
     </row>
     <row r="273">
-      <c s="3" r="E273"/>
+      <c s="4" r="E273"/>
     </row>
     <row r="274">
-      <c s="3" r="E274"/>
+      <c s="4" r="E274"/>
     </row>
     <row r="275">
-      <c s="3" r="E275"/>
+      <c s="4" r="E275"/>
     </row>
     <row r="276">
-      <c s="3" r="E276"/>
+      <c s="4" r="E276"/>
     </row>
     <row r="277">
-      <c s="3" r="E277"/>
+      <c s="4" r="E277"/>
     </row>
     <row r="278">
-      <c s="3" r="E278"/>
+      <c s="4" r="E278"/>
     </row>
     <row r="279">
-      <c s="3" r="E279"/>
+      <c s="4" r="E279"/>
     </row>
     <row r="280">
-      <c s="3" r="E280"/>
+      <c s="4" r="E280"/>
     </row>
     <row r="281">
-      <c s="3" r="E281"/>
+      <c s="4" r="E281"/>
     </row>
     <row r="282">
-      <c s="3" r="E282"/>
+      <c s="4" r="E282"/>
     </row>
     <row r="283">
-      <c s="3" r="E283"/>
+      <c s="4" r="E283"/>
     </row>
     <row r="284">
-      <c s="3" r="E284"/>
+      <c s="4" r="E284"/>
     </row>
     <row r="285">
-      <c s="3" r="E285"/>
+      <c s="4" r="E285"/>
     </row>
     <row r="286">
-      <c s="3" r="E286"/>
+      <c s="4" r="E286"/>
     </row>
     <row r="287">
-      <c s="3" r="E287"/>
+      <c s="4" r="E287"/>
     </row>
     <row r="288">
-      <c s="3" r="E288"/>
+      <c s="4" r="E288"/>
     </row>
     <row r="289">
-      <c s="3" r="E289"/>
+      <c s="4" r="E289"/>
     </row>
     <row r="290">
-      <c s="3" r="E290"/>
+      <c s="4" r="E290"/>
     </row>
     <row r="291">
-      <c s="3" r="E291"/>
+      <c s="4" r="E291"/>
     </row>
     <row r="292">
-      <c s="3" r="E292"/>
+      <c s="4" r="E292"/>
     </row>
     <row r="293">
-      <c s="3" r="E293"/>
+      <c s="4" r="E293"/>
     </row>
     <row r="294">
-      <c s="3" r="E294"/>
+      <c s="4" r="E294"/>
     </row>
     <row r="295">
-      <c s="3" r="E295"/>
+      <c s="4" r="E295"/>
     </row>
     <row r="296">
-      <c s="3" r="E296"/>
+      <c s="4" r="E296"/>
     </row>
     <row r="297">
-      <c s="3" r="E297"/>
+      <c s="4" r="E297"/>
     </row>
     <row r="298">
-      <c s="3" r="E298"/>
+      <c s="4" r="E298"/>
     </row>
     <row r="299">
-      <c s="3" r="E299"/>
+      <c s="4" r="E299"/>
     </row>
     <row r="300">
-      <c s="3" r="E300"/>
+      <c s="4" r="E300"/>
     </row>
     <row r="301">
-      <c s="3" r="E301"/>
+      <c s="4" r="E301"/>
     </row>
     <row r="302">
-      <c s="3" r="E302"/>
+      <c s="4" r="E302"/>
     </row>
     <row r="303">
-      <c s="3" r="E303"/>
+      <c s="4" r="E303"/>
     </row>
     <row r="304">
-      <c s="3" r="E304"/>
+      <c s="4" r="E304"/>
     </row>
     <row r="305">
-      <c s="3" r="E305"/>
+      <c s="4" r="E305"/>
     </row>
     <row r="306">
-      <c s="3" r="E306"/>
+      <c s="4" r="E306"/>
     </row>
     <row r="307">
-      <c s="3" r="E307"/>
+      <c s="4" r="E307"/>
     </row>
     <row r="308">
-      <c s="3" r="E308"/>
+      <c s="4" r="E308"/>
     </row>
     <row r="309">
-      <c s="3" r="E309"/>
+      <c s="4" r="E309"/>
     </row>
     <row r="310">
-      <c s="3" r="E310"/>
+      <c s="4" r="E310"/>
     </row>
     <row r="311">
-      <c s="3" r="E311"/>
+      <c s="4" r="E311"/>
     </row>
     <row r="312">
-      <c s="3" r="E312"/>
+      <c s="4" r="E312"/>
     </row>
     <row r="313">
-      <c s="3" r="E313"/>
+      <c s="4" r="E313"/>
     </row>
     <row r="314">
-      <c s="3" r="E314"/>
+      <c s="4" r="E314"/>
     </row>
     <row r="315">
-      <c s="3" r="E315"/>
+      <c s="4" r="E315"/>
     </row>
     <row r="316">
-      <c s="3" r="E316"/>
+      <c s="4" r="E316"/>
     </row>
     <row r="317">
-      <c s="3" r="E317"/>
+      <c s="4" r="E317"/>
     </row>
     <row r="318">
-      <c s="3" r="E318"/>
+      <c s="4" r="E318"/>
     </row>
     <row r="319">
-      <c s="3" r="E319"/>
+      <c s="4" r="E319"/>
     </row>
     <row r="320">
-      <c s="3" r="E320"/>
+      <c s="4" r="E320"/>
     </row>
     <row r="321">
-      <c s="3" r="E321"/>
+      <c s="4" r="E321"/>
     </row>
     <row r="322">
-      <c s="3" r="E322"/>
+      <c s="4" r="E322"/>
     </row>
     <row r="323">
-      <c s="3" r="E323"/>
+      <c s="4" r="E323"/>
     </row>
     <row r="324">
-      <c s="3" r="E324"/>
+      <c s="4" r="E324"/>
     </row>
     <row r="325">
-      <c s="3" r="E325"/>
+      <c s="4" r="E325"/>
     </row>
     <row r="326">
-      <c s="3" r="E326"/>
+      <c s="4" r="E326"/>
     </row>
     <row r="327">
-      <c s="3" r="E327"/>
+      <c s="4" r="E327"/>
     </row>
     <row r="328">
-      <c s="3" r="E328"/>
+      <c s="4" r="E328"/>
     </row>
     <row r="329">
-      <c s="3" r="E329"/>
+      <c s="4" r="E329"/>
     </row>
     <row r="330">
-      <c s="3" r="E330"/>
+      <c s="4" r="E330"/>
     </row>
     <row r="331">
-      <c s="3" r="E331"/>
+      <c s="4" r="E331"/>
     </row>
     <row r="332">
-      <c s="3" r="E332"/>
+      <c s="4" r="E332"/>
     </row>
     <row r="333">
-      <c s="3" r="E333"/>
+      <c s="4" r="E333"/>
     </row>
     <row r="334">
-      <c s="3" r="E334"/>
+      <c s="4" r="E334"/>
     </row>
     <row r="335">
-      <c s="3" r="E335"/>
+      <c s="4" r="E335"/>
     </row>
     <row r="336">
-      <c s="3" r="E336"/>
+      <c s="4" r="E336"/>
     </row>
     <row r="337">
-      <c s="3" r="E337"/>
+      <c s="4" r="E337"/>
     </row>
     <row r="338">
-      <c s="3" r="E338"/>
+      <c s="4" r="E338"/>
     </row>
     <row r="339">
-      <c s="3" r="E339"/>
+      <c s="4" r="E339"/>
     </row>
     <row r="340">
-      <c s="3" r="E340"/>
+      <c s="4" r="E340"/>
     </row>
     <row r="341">
-      <c s="3" r="E341"/>
+      <c s="4" r="E341"/>
     </row>
     <row r="342">
-      <c s="3" r="E342"/>
+      <c s="4" r="E342"/>
     </row>
     <row r="343">
-      <c s="3" r="E343"/>
+      <c s="4" r="E343"/>
     </row>
     <row r="344">
-      <c s="3" r="E344"/>
+      <c s="4" r="E344"/>
     </row>
     <row r="345">
-      <c s="3" r="E345"/>
+      <c s="4" r="E345"/>
     </row>
     <row r="346">
-      <c s="3" r="E346"/>
+      <c s="4" r="E346"/>
     </row>
     <row r="347">
-      <c s="3" r="E347"/>
+      <c s="4" r="E347"/>
     </row>
     <row r="348">
-      <c s="3" r="E348"/>
+      <c s="4" r="E348"/>
     </row>
     <row r="349">
-      <c s="3" r="E349"/>
+      <c s="4" r="E349"/>
     </row>
     <row r="350">
-      <c s="3" r="E350"/>
+      <c s="4" r="E350"/>
     </row>
     <row r="351">
-      <c s="3" r="E351"/>
+      <c s="4" r="E351"/>
     </row>
     <row r="352">
-      <c s="3" r="E352"/>
+      <c s="4" r="E352"/>
     </row>
     <row r="353">
-      <c s="3" r="E353"/>
+      <c s="4" r="E353"/>
     </row>
     <row r="354">
-      <c s="3" r="E354"/>
+      <c s="4" r="E354"/>
     </row>
     <row r="355">
-      <c s="3" r="E355"/>
+      <c s="4" r="E355"/>
     </row>
     <row r="356">
-      <c s="3" r="E356"/>
+      <c s="4" r="E356"/>
     </row>
     <row r="357">
-      <c s="3" r="E357"/>
+      <c s="4" r="E357"/>
     </row>
     <row r="358">
-      <c s="3" r="E358"/>
+      <c s="4" r="E358"/>
     </row>
     <row r="359">
-      <c s="3" r="E359"/>
+      <c s="4" r="E359"/>
     </row>
     <row r="360">
-      <c s="3" r="E360"/>
+      <c s="4" r="E360"/>
     </row>
     <row r="361">
-      <c s="3" r="E361"/>
+      <c s="4" r="E361"/>
     </row>
     <row r="362">
-      <c s="3" r="E362"/>
+      <c s="4" r="E362"/>
     </row>
     <row r="363">
-      <c s="3" r="E363"/>
+      <c s="4" r="E363"/>
     </row>
     <row r="364">
-      <c s="3" r="E364"/>
+      <c s="4" r="E364"/>
     </row>
     <row r="365">
-      <c s="3" r="E365"/>
+      <c s="4" r="E365"/>
     </row>
     <row r="366">
-      <c s="3" r="E366"/>
+      <c s="4" r="E366"/>
     </row>
     <row r="367">
-      <c s="3" r="E367"/>
+      <c s="4" r="E367"/>
     </row>
     <row r="368">
-      <c s="3" r="E368"/>
+      <c s="4" r="E368"/>
     </row>
     <row r="369">
-      <c s="3" r="E369"/>
+      <c s="4" r="E369"/>
     </row>
     <row r="370">
-      <c s="3" r="E370"/>
+      <c s="4" r="E370"/>
     </row>
     <row r="371">
-      <c s="3" r="E371"/>
+      <c s="4" r="E371"/>
     </row>
     <row r="372">
-      <c s="3" r="E372"/>
+      <c s="4" r="E372"/>
     </row>
     <row r="373">
-      <c s="3" r="E373"/>
+      <c s="4" r="E373"/>
     </row>
     <row r="374">
-      <c s="3" r="E374"/>
+      <c s="4" r="E374"/>
     </row>
     <row r="375">
-      <c s="3" r="E375"/>
+      <c s="4" r="E375"/>
     </row>
     <row r="376">
-      <c s="3" r="E376"/>
+      <c s="4" r="E376"/>
     </row>
     <row r="377">
-      <c s="3" r="E377"/>
+      <c s="4" r="E377"/>
     </row>
     <row r="378">
-      <c s="3" r="E378"/>
+      <c s="4" r="E378"/>
     </row>
     <row r="379">
-      <c s="3" r="E379"/>
+      <c s="4" r="E379"/>
     </row>
     <row r="380">
-      <c s="3" r="E380"/>
+      <c s="4" r="E380"/>
     </row>
     <row r="381">
-      <c s="3" r="E381"/>
+      <c s="4" r="E381"/>
     </row>
     <row r="382">
-      <c s="3" r="E382"/>
+      <c s="4" r="E382"/>
     </row>
     <row r="383">
-      <c s="3" r="E383"/>
+      <c s="4" r="E383"/>
     </row>
     <row r="384">
-      <c s="3" r="E384"/>
+      <c s="4" r="E384"/>
     </row>
     <row r="385">
-      <c s="3" r="E385"/>
+      <c s="4" r="E385"/>
     </row>
     <row r="386">
-      <c s="3" r="E386"/>
+      <c s="4" r="E386"/>
     </row>
     <row r="387">
-      <c s="3" r="E387"/>
+      <c s="4" r="E387"/>
     </row>
     <row r="388">
-      <c s="3" r="E388"/>
+      <c s="4" r="E388"/>
     </row>
     <row r="389">
-      <c s="3" r="E389"/>
+      <c s="4" r="E389"/>
     </row>
     <row r="390">
-      <c s="3" r="E390"/>
+      <c s="4" r="E390"/>
     </row>
     <row r="391">
-      <c s="3" r="E391"/>
+      <c s="4" r="E391"/>
     </row>
     <row r="392">
-      <c s="3" r="E392"/>
+      <c s="4" r="E392"/>
     </row>
     <row r="393">
-      <c s="3" r="E393"/>
+      <c s="4" r="E393"/>
     </row>
     <row r="394">
-      <c s="3" r="E394"/>
+      <c s="4" r="E394"/>
     </row>
     <row r="395">
-      <c s="3" r="E395"/>
+      <c s="4" r="E395"/>
     </row>
     <row r="396">
-      <c s="3" r="E396"/>
+      <c s="4" r="E396"/>
     </row>
     <row r="397">
-      <c s="3" r="E397"/>
+      <c s="4" r="E397"/>
     </row>
     <row r="398">
-      <c s="3" r="E398"/>
+      <c s="4" r="E398"/>
     </row>
     <row r="399">
-      <c s="3" r="E399"/>
+      <c s="4" r="E399"/>
     </row>
     <row r="400">
-      <c s="3" r="E400"/>
+      <c s="4" r="E400"/>
     </row>
     <row r="401">
-      <c s="3" r="E401"/>
+      <c s="4" r="E401"/>
     </row>
     <row r="402">
-      <c s="3" r="E402"/>
+      <c s="4" r="E402"/>
     </row>
     <row r="403">
-      <c s="3" r="E403"/>
+      <c s="4" r="E403"/>
     </row>
     <row r="404">
-      <c s="3" r="E404"/>
+      <c s="4" r="E404"/>
     </row>
     <row r="405">
-      <c s="3" r="E405"/>
+      <c s="4" r="E405"/>
     </row>
     <row r="406">
-      <c s="3" r="E406"/>
+      <c s="4" r="E406"/>
     </row>
     <row r="407">
-      <c s="3" r="E407"/>
+      <c s="4" r="E407"/>
     </row>
     <row r="408">
-      <c s="3" r="E408"/>
+      <c s="4" r="E408"/>
     </row>
     <row r="409">
-      <c s="3" r="E409"/>
+      <c s="4" r="E409"/>
     </row>
     <row r="410">
-      <c s="3" r="E410"/>
+      <c s="4" r="E410"/>
     </row>
     <row r="411">
-      <c s="3" r="E411"/>
+      <c s="4" r="E411"/>
     </row>
     <row r="412">
-      <c s="3" r="E412"/>
+      <c s="4" r="E412"/>
     </row>
     <row r="413">
-      <c s="3" r="E413"/>
+      <c s="4" r="E413"/>
     </row>
     <row r="414">
-      <c s="3" r="E414"/>
+      <c s="4" r="E414"/>
     </row>
     <row r="415">
-      <c s="3" r="E415"/>
+      <c s="4" r="E415"/>
     </row>
     <row r="416">
-      <c s="3" r="E416"/>
+      <c s="4" r="E416"/>
     </row>
     <row r="417">
-      <c s="3" r="E417"/>
+      <c s="4" r="E417"/>
     </row>
     <row r="418">
-      <c s="3" r="E418"/>
+      <c s="4" r="E418"/>
     </row>
     <row r="419">
-      <c s="3" r="E419"/>
+      <c s="4" r="E419"/>
     </row>
     <row r="420">
-      <c s="3" r="E420"/>
+      <c s="4" r="E420"/>
     </row>
     <row r="421">
-      <c s="3" r="E421"/>
+      <c s="4" r="E421"/>
     </row>
     <row r="422">
-      <c s="3" r="E422"/>
+      <c s="4" r="E422"/>
     </row>
     <row r="423">
-      <c s="3" r="E423"/>
+      <c s="4" r="E423"/>
     </row>
     <row r="424">
-      <c s="3" r="E424"/>
+      <c s="4" r="E424"/>
     </row>
     <row r="425">
-      <c s="3" r="E425"/>
+      <c s="4" r="E425"/>
     </row>
     <row r="426">
-      <c s="3" r="E426"/>
+      <c s="4" r="E426"/>
     </row>
     <row r="427">
-      <c s="3" r="E427"/>
+      <c s="4" r="E427"/>
     </row>
     <row r="428">
-      <c s="3" r="E428"/>
+      <c s="4" r="E428"/>
     </row>
     <row r="429">
-      <c s="3" r="E429"/>
+      <c s="4" r="E429"/>
     </row>
     <row r="430">
-      <c s="3" r="E430"/>
+      <c s="4" r="E430"/>
     </row>
     <row r="431">
-      <c s="3" r="E431"/>
+      <c s="4" r="E431"/>
     </row>
     <row r="432">
-      <c s="3" r="E432"/>
+      <c s="4" r="E432"/>
     </row>
     <row r="433">
-      <c s="3" r="E433"/>
+      <c s="4" r="E433"/>
     </row>
     <row r="434">
-      <c s="3" r="E434"/>
+      <c s="4" r="E434"/>
     </row>
     <row r="435">
-      <c s="3" r="E435"/>
+      <c s="4" r="E435"/>
     </row>
     <row r="436">
-      <c s="3" r="E436"/>
+      <c s="4" r="E436"/>
     </row>
     <row r="437">
-      <c s="3" r="E437"/>
+      <c s="4" r="E437"/>
     </row>
     <row r="438">
-      <c s="3" r="E438"/>
+      <c s="4" r="E438"/>
     </row>
     <row r="439">
-      <c s="3" r="E439"/>
+      <c s="4" r="E439"/>
     </row>
     <row r="440">
-      <c s="3" r="E440"/>
+      <c s="4" r="E440"/>
     </row>
     <row r="441">
-      <c s="3" r="E441"/>
+      <c s="4" r="E441"/>
     </row>
     <row r="442">
-      <c s="3" r="E442"/>
+      <c s="4" r="E442"/>
     </row>
     <row r="443">
-      <c s="3" r="E443"/>
+      <c s="4" r="E443"/>
     </row>
     <row r="444">
-      <c s="3" r="E444"/>
+      <c s="4" r="E444"/>
     </row>
     <row r="445">
-      <c s="3" r="E445"/>
+      <c s="4" r="E445"/>
     </row>
     <row r="446">
-      <c s="3" r="E446"/>
+      <c s="4" r="E446"/>
     </row>
     <row r="447">
-      <c s="3" r="E447"/>
+      <c s="4" r="E447"/>
     </row>
     <row r="448">
-      <c s="3" r="E448"/>
+      <c s="4" r="E448"/>
     </row>
     <row r="449">
-      <c s="3" r="E449"/>
+      <c s="4" r="E449"/>
     </row>
     <row r="450">
-      <c s="3" r="E450"/>
+      <c s="4" r="E450"/>
     </row>
     <row r="451">
-      <c s="3" r="E451"/>
+      <c s="4" r="E451"/>
     </row>
     <row r="452">
-      <c s="3" r="E452"/>
+      <c s="4" r="E452"/>
     </row>
     <row r="453">
-      <c s="3" r="E453"/>
+      <c s="4" r="E453"/>
     </row>
     <row r="454">
-      <c s="3" r="E454"/>
+      <c s="4" r="E454"/>
     </row>
     <row r="455">
-      <c s="3" r="E455"/>
+      <c s="4" r="E455"/>
     </row>
     <row r="456">
-      <c s="3" r="E456"/>
+      <c s="4" r="E456"/>
     </row>
     <row r="457">
-      <c s="3" r="E457"/>
+      <c s="4" r="E457"/>
     </row>
     <row r="458">
-      <c s="3" r="E458"/>
+      <c s="4" r="E458"/>
     </row>
     <row r="459">
-      <c s="3" r="E459"/>
+      <c s="4" r="E459"/>
     </row>
     <row r="460">
-      <c s="3" r="E460"/>
+      <c s="4" r="E460"/>
     </row>
     <row r="461">
-      <c s="3" r="E461"/>
+      <c s="4" r="E461"/>
     </row>
     <row r="462">
-      <c s="3" r="E462"/>
+      <c s="4" r="E462"/>
     </row>
     <row r="463">
-      <c s="3" r="E463"/>
+      <c s="4" r="E463"/>
     </row>
     <row r="464">
-      <c s="3" r="E464"/>
+      <c s="4" r="E464"/>
     </row>
     <row r="465">
-      <c s="3" r="E465"/>
+      <c s="4" r="E465"/>
     </row>
     <row r="466">
-      <c s="3" r="E466"/>
+      <c s="4" r="E466"/>
     </row>
     <row r="467">
-      <c s="3" r="E467"/>
+      <c s="4" r="E467"/>
     </row>
     <row r="468">
-      <c s="3" r="E468"/>
+      <c s="4" r="E468"/>
     </row>
     <row r="469">
-      <c s="3" r="E469"/>
+      <c s="4" r="E469"/>
     </row>
     <row r="470">
-      <c s="3" r="E470"/>
+      <c s="4" r="E470"/>
     </row>
     <row r="471">
-      <c s="3" r="E471"/>
+      <c s="4" r="E471"/>
     </row>
     <row r="472">
-      <c s="3" r="E472"/>
+      <c s="4" r="E472"/>
     </row>
     <row r="473">
-      <c s="3" r="E473"/>
+      <c s="4" r="E473"/>
     </row>
     <row r="474">
-      <c s="3" r="E474"/>
+      <c s="4" r="E474"/>
     </row>
     <row r="475">
-      <c s="3" r="E475"/>
+      <c s="4" r="E475"/>
     </row>
     <row r="476">
-      <c s="3" r="E476"/>
+      <c s="4" r="E476"/>
     </row>
     <row r="477">
-      <c s="3" r="E477"/>
+      <c s="4" r="E477"/>
     </row>
     <row r="478">
-      <c s="3" r="E478"/>
+      <c s="4" r="E478"/>
     </row>
     <row r="479">
-      <c s="3" r="E479"/>
+      <c s="4" r="E479"/>
     </row>
     <row r="480">
-      <c s="3" r="E480"/>
+      <c s="4" r="E480"/>
     </row>
     <row r="481">
-      <c s="3" r="E481"/>
+      <c s="4" r="E481"/>
     </row>
     <row r="482">
-      <c s="3" r="E482"/>
+      <c s="4" r="E482"/>
     </row>
     <row r="483">
-      <c s="3" r="E483"/>
+      <c s="4" r="E483"/>
     </row>
     <row r="484">
-      <c s="3" r="E484"/>
+      <c s="4" r="E484"/>
     </row>
     <row r="485">
-      <c s="3" r="E485"/>
+      <c s="4" r="E485"/>
     </row>
     <row r="486">
-      <c s="3" r="E486"/>
+      <c s="4" r="E486"/>
     </row>
     <row r="487">
-      <c s="3" r="E487"/>
+      <c s="4" r="E487"/>
     </row>
     <row r="488">
-      <c s="3" r="E488"/>
+      <c s="4" r="E488"/>
     </row>
     <row r="489">
-      <c s="3" r="E489"/>
+      <c s="4" r="E489"/>
     </row>
     <row r="490">
-      <c s="3" r="E490"/>
+      <c s="4" r="E490"/>
     </row>
     <row r="491">
-      <c s="3" r="E491"/>
+      <c s="4" r="E491"/>
     </row>
     <row r="492">
-      <c s="3" r="E492"/>
+      <c s="4" r="E492"/>
     </row>
     <row r="493">
-      <c s="3" r="E493"/>
+      <c s="4" r="E493"/>
     </row>
     <row r="494">
-      <c s="3" r="E494"/>
+      <c s="4" r="E494"/>
     </row>
     <row r="495">
-      <c s="3" r="E495"/>
+      <c s="4" r="E495"/>
     </row>
     <row r="496">
-      <c s="3" r="E496"/>
+      <c s="4" r="E496"/>
     </row>
     <row r="497">
-      <c s="3" r="E497"/>
+      <c s="4" r="E497"/>
     </row>
     <row r="498">
-      <c s="3" r="E498"/>
+      <c s="4" r="E498"/>
     </row>
     <row r="499">
-      <c s="3" r="E499"/>
+      <c s="4" r="E499"/>
     </row>
     <row r="500">
-      <c s="3" r="E500"/>
+      <c s="4" r="E500"/>
     </row>
     <row r="501">
-      <c s="3" r="E501"/>
+      <c s="4" r="E501"/>
     </row>
     <row r="502">
-      <c s="3" r="E502"/>
+      <c s="4" r="E502"/>
     </row>
     <row r="503">
-      <c s="3" r="E503"/>
+      <c s="4" r="E503"/>
     </row>
     <row r="504">
-      <c s="3" r="E504"/>
+      <c s="4" r="E504"/>
     </row>
     <row r="505">
-      <c s="3" r="E505"/>
+      <c s="4" r="E505"/>
     </row>
     <row r="506">
-      <c s="3" r="E506"/>
+      <c s="4" r="E506"/>
     </row>
     <row r="507">
-      <c s="3" r="E507"/>
+      <c s="4" r="E507"/>
     </row>
     <row r="508">
-      <c s="3" r="E508"/>
+      <c s="4" r="E508"/>
     </row>
     <row r="509">
-      <c s="3" r="E509"/>
+      <c s="4" r="E509"/>
     </row>
     <row r="510">
-      <c s="3" r="E510"/>
+      <c s="4" r="E510"/>
     </row>
     <row r="511">
-      <c s="3" r="E511"/>
+      <c s="4" r="E511"/>
     </row>
     <row r="512">
-      <c s="3" r="E512"/>
+      <c s="4" r="E512"/>
     </row>
     <row r="513">
-      <c s="3" r="E513"/>
+      <c s="4" r="E513"/>
     </row>
     <row r="514">
-      <c s="3" r="E514"/>
+      <c s="4" r="E514"/>
     </row>
     <row r="515">
-      <c s="3" r="E515"/>
+      <c s="4" r="E515"/>
     </row>
     <row r="516">
-      <c s="3" r="E516"/>
+      <c s="4" r="E516"/>
     </row>
     <row r="517">
-      <c s="3" r="E517"/>
+      <c s="4" r="E517"/>
     </row>
     <row r="518">
-      <c s="3" r="E518"/>
+      <c s="4" r="E518"/>
     </row>
     <row r="519">
-      <c s="3" r="E519"/>
+      <c s="4" r="E519"/>
     </row>
     <row r="520">
-      <c s="3" r="E520"/>
+      <c s="4" r="E520"/>
     </row>
     <row r="521">
-      <c s="3" r="E521"/>
+      <c s="4" r="E521"/>
     </row>
     <row r="522">
-      <c s="3" r="E522"/>
+      <c s="4" r="E522"/>
     </row>
     <row r="523">
-      <c s="3" r="E523"/>
+      <c s="4" r="E523"/>
     </row>
     <row r="524">
-      <c s="3" r="E524"/>
+      <c s="4" r="E524"/>
     </row>
     <row r="525">
-      <c s="3" r="E525"/>
+      <c s="4" r="E525"/>
     </row>
     <row r="526">
-      <c s="3" r="E526"/>
+      <c s="4" r="E526"/>
     </row>
     <row r="527">
-      <c s="3" r="E527"/>
+      <c s="4" r="E527"/>
     </row>
     <row r="528">
-      <c s="3" r="E528"/>
+      <c s="4" r="E528"/>
     </row>
     <row r="529">
-      <c s="3" r="E529"/>
+      <c s="4" r="E529"/>
     </row>
     <row r="530">
-      <c s="3" r="E530"/>
+      <c s="4" r="E530"/>
     </row>
     <row r="531">
-      <c s="3" r="E531"/>
+      <c s="4" r="E531"/>
     </row>
     <row r="532">
-      <c s="3" r="E532"/>
+      <c s="4" r="E532"/>
     </row>
     <row r="533">
-      <c s="3" r="E533"/>
+      <c s="4" r="E533"/>
     </row>
     <row r="534">
-      <c s="3" r="E534"/>
+      <c s="4" r="E534"/>
     </row>
     <row r="535">
-      <c s="3" r="E535"/>
+      <c s="4" r="E535"/>
     </row>
     <row r="536">
-      <c s="3" r="E536"/>
+      <c s="4" r="E536"/>
     </row>
     <row r="537">
-      <c s="3" r="E537"/>
+      <c s="4" r="E537"/>
     </row>
     <row r="538">
-      <c s="3" r="E538"/>
+      <c s="4" r="E538"/>
     </row>
     <row r="539">
-      <c s="3" r="E539"/>
+      <c s="4" r="E539"/>
     </row>
     <row r="540">
-      <c s="3" r="E540"/>
+      <c s="4" r="E540"/>
     </row>
     <row r="541">
-      <c s="3" r="E541"/>
+      <c s="4" r="E541"/>
     </row>
     <row r="542">
-      <c s="3" r="E542"/>
+      <c s="4" r="E542"/>
     </row>
     <row r="543">
-      <c s="3" r="E543"/>
+      <c s="4" r="E543"/>
     </row>
     <row r="544">
-      <c s="3" r="E544"/>
+      <c s="4" r="E544"/>
     </row>
     <row r="545">
-      <c s="3" r="E545"/>
+      <c s="4" r="E545"/>
     </row>
     <row r="546">
-      <c s="3" r="E546"/>
+      <c s="4" r="E546"/>
     </row>
     <row r="547">
-      <c s="3" r="E547"/>
+      <c s="4" r="E547"/>
     </row>
     <row r="548">
-      <c s="3" r="E548"/>
+      <c s="4" r="E548"/>
     </row>
     <row r="549">
-      <c s="3" r="E549"/>
+      <c s="4" r="E549"/>
     </row>
     <row r="550">
-      <c s="3" r="E550"/>
+      <c s="4" r="E550"/>
     </row>
     <row r="551">
-      <c s="3" r="E551"/>
+      <c s="4" r="E551"/>
     </row>
     <row r="552">
-      <c s="3" r="E552"/>
+      <c s="4" r="E552"/>
     </row>
     <row r="553">
-      <c s="3" r="E553"/>
+      <c s="4" r="E553"/>
     </row>
     <row r="554">
-      <c s="3" r="E554"/>
+      <c s="4" r="E554"/>
     </row>
     <row r="555">
-      <c s="3" r="E555"/>
+      <c s="4" r="E555"/>
     </row>
     <row r="556">
-      <c s="3" r="E556"/>
+      <c s="4" r="E556"/>
     </row>
     <row r="557">
-      <c s="3" r="E557"/>
+      <c s="4" r="E557"/>
     </row>
     <row r="558">
-      <c s="3" r="E558"/>
+      <c s="4" r="E558"/>
     </row>
     <row r="559">
-      <c s="3" r="E559"/>
+      <c s="4" r="E559"/>
     </row>
     <row r="560">
-      <c s="3" r="E560"/>
+      <c s="4" r="E560"/>
     </row>
     <row r="561">
-      <c s="3" r="E561"/>
+      <c s="4" r="E561"/>
     </row>
     <row r="562">
-      <c s="3" r="E562"/>
+      <c s="4" r="E562"/>
     </row>
     <row r="563">
-      <c s="3" r="E563"/>
+      <c s="4" r="E563"/>
     </row>
     <row r="564">
-      <c s="3" r="E564"/>
+      <c s="4" r="E564"/>
     </row>
     <row r="565">
-      <c s="3" r="E565"/>
+      <c s="4" r="E565"/>
     </row>
     <row r="566">
-      <c s="3" r="E566"/>
+      <c s="4" r="E566"/>
     </row>
     <row r="567">
-      <c s="3" r="E567"/>
+      <c s="4" r="E567"/>
     </row>
     <row r="568">
-      <c s="3" r="E568"/>
+      <c s="4" r="E568"/>
     </row>
     <row r="569">
-      <c s="3" r="E569"/>
+      <c s="4" r="E569"/>
     </row>
     <row r="570">
-      <c s="3" r="E570"/>
+      <c s="4" r="E570"/>
     </row>
     <row r="571">
-      <c s="3" r="E571"/>
+      <c s="4" r="E571"/>
     </row>
     <row r="572">
-      <c s="3" r="E572"/>
+      <c s="4" r="E572"/>
     </row>
     <row r="573">
-      <c s="3" r="E573"/>
+      <c s="4" r="E573"/>
     </row>
     <row r="574">
-      <c s="3" r="E574"/>
+      <c s="4" r="E574"/>
     </row>
     <row r="575">
-      <c s="3" r="E575"/>
+      <c s="4" r="E575"/>
     </row>
     <row r="576">
-      <c s="3" r="E576"/>
+      <c s="4" r="E576"/>
     </row>
     <row r="577">
-      <c s="3" r="E577"/>
+      <c s="4" r="E577"/>
     </row>
     <row r="578">
-      <c s="3" r="E578"/>
+      <c s="4" r="E578"/>
     </row>
     <row r="579">
-      <c s="3" r="E579"/>
+      <c s="4" r="E579"/>
     </row>
     <row r="580">
-      <c s="3" r="E580"/>
+      <c s="4" r="E580"/>
     </row>
     <row r="581">
-      <c s="3" r="E581"/>
+      <c s="4" r="E581"/>
     </row>
     <row r="582">
-      <c s="3" r="E582"/>
+      <c s="4" r="E582"/>
     </row>
     <row r="583">
-      <c s="3" r="E583"/>
+      <c s="4" r="E583"/>
     </row>
     <row r="584">
-      <c s="3" r="E584"/>
+      <c s="4" r="E584"/>
     </row>
     <row r="585">
-      <c s="3" r="E585"/>
+      <c s="4" r="E585"/>
     </row>
     <row r="586">
-      <c s="3" r="E586"/>
+      <c s="4" r="E586"/>
     </row>
     <row r="587">
-      <c s="3" r="E587"/>
+      <c s="4" r="E587"/>
     </row>
     <row r="588">
-      <c s="3" r="E588"/>
+      <c s="4" r="E588"/>
     </row>
     <row r="589">
-      <c s="3" r="E589"/>
+      <c s="4" r="E589"/>
     </row>
     <row r="590">
-      <c s="3" r="E590"/>
+      <c s="4" r="E590"/>
     </row>
     <row r="591">
-      <c s="3" r="E591"/>
+      <c s="4" r="E591"/>
     </row>
     <row r="592">
-      <c s="3" r="E592"/>
+      <c s="4" r="E592"/>
     </row>
     <row r="593">
-      <c s="3" r="E593"/>
+      <c s="4" r="E593"/>
     </row>
     <row r="594">
-      <c s="3" r="E594"/>
+      <c s="4" r="E594"/>
     </row>
     <row r="595">
-      <c s="3" r="E595"/>
+      <c s="4" r="E595"/>
     </row>
     <row r="596">
-      <c s="3" r="E596"/>
+      <c s="4" r="E596"/>
     </row>
     <row r="597">
-      <c s="3" r="E597"/>
+      <c s="4" r="E597"/>
     </row>
     <row r="598">
-      <c s="3" r="E598"/>
+      <c s="4" r="E598"/>
     </row>
     <row r="599">
-      <c s="3" r="E599"/>
+      <c s="4" r="E599"/>
     </row>
     <row r="600">
-      <c s="3" r="E600"/>
+      <c s="4" r="E600"/>
     </row>
     <row r="601">
-      <c s="3" r="E601"/>
+      <c s="4" r="E601"/>
     </row>
     <row r="602">
-      <c s="3" r="E602"/>
+      <c s="4" r="E602"/>
     </row>
     <row r="603">
-      <c s="3" r="E603"/>
+      <c s="4" r="E603"/>
     </row>
     <row r="604">
-      <c s="3" r="E604"/>
+      <c s="4" r="E604"/>
     </row>
     <row r="605">
-      <c s="3" r="E605"/>
+      <c s="4" r="E605"/>
     </row>
     <row r="606">
-      <c s="3" r="E606"/>
+      <c s="4" r="E606"/>
     </row>
     <row r="607">
-      <c s="3" r="E607"/>
+      <c s="4" r="E607"/>
     </row>
     <row r="608">
-      <c s="3" r="E608"/>
+      <c s="4" r="E608"/>
     </row>
     <row r="609">
-      <c s="3" r="E609"/>
+      <c s="4" r="E609"/>
     </row>
     <row r="610">
-      <c s="3" r="E610"/>
+      <c s="4" r="E610"/>
     </row>
     <row r="611">
-      <c s="3" r="E611"/>
+      <c s="4" r="E611"/>
     </row>
     <row r="612">
-      <c s="3" r="E612"/>
+      <c s="4" r="E612"/>
     </row>
     <row r="613">
-      <c s="3" r="E613"/>
+      <c s="4" r="E613"/>
     </row>
     <row r="614">
-      <c s="3" r="E614"/>
+      <c s="4" r="E614"/>
     </row>
     <row r="615">
-      <c s="3" r="E615"/>
+      <c s="4" r="E615"/>
     </row>
     <row r="616">
-      <c s="3" r="E616"/>
+      <c s="4" r="E616"/>
     </row>
     <row r="617">
-      <c s="3" r="E617"/>
+      <c s="4" r="E617"/>
     </row>
     <row r="618">
-      <c s="3" r="E618"/>
+      <c s="4" r="E618"/>
     </row>
     <row r="619">
-      <c s="3" r="E619"/>
+      <c s="4" r="E619"/>
     </row>
     <row r="620">
-      <c s="3" r="E620"/>
+      <c s="4" r="E620"/>
     </row>
     <row r="621">
-      <c s="3" r="E621"/>
+      <c s="4" r="E621"/>
     </row>
     <row r="622">
-      <c s="3" r="E622"/>
+      <c s="4" r="E622"/>
     </row>
     <row r="623">
-      <c s="3" r="E623"/>
+      <c s="4" r="E623"/>
     </row>
     <row r="624">
-      <c s="3" r="E624"/>
+      <c s="4" r="E624"/>
     </row>
     <row r="625">
-      <c s="3" r="E625"/>
+      <c s="4" r="E625"/>
     </row>
     <row r="626">
-      <c s="3" r="E626"/>
+      <c s="4" r="E626"/>
     </row>
     <row r="627">
-      <c s="3" r="E627"/>
+      <c s="4" r="E627"/>
     </row>
     <row r="628">
-      <c s="3" r="E628"/>
+      <c s="4" r="E628"/>
     </row>
     <row r="629">
-      <c s="3" r="E629"/>
+      <c s="4" r="E629"/>
     </row>
     <row r="630">
-      <c s="3" r="E630"/>
+      <c s="4" r="E630"/>
     </row>
     <row r="631">
-      <c s="3" r="E631"/>
+      <c s="4" r="E631"/>
     </row>
     <row r="632">
-      <c s="3" r="E632"/>
+      <c s="4" r="E632"/>
     </row>
     <row r="633">
-      <c s="3" r="E633"/>
+      <c s="4" r="E633"/>
     </row>
     <row r="634">
-      <c s="3" r="E634"/>
+      <c s="4" r="E634"/>
     </row>
     <row r="635">
-      <c s="3" r="E635"/>
+      <c s="4" r="E635"/>
     </row>
     <row r="636">
-      <c s="3" r="E636"/>
+      <c s="4" r="E636"/>
     </row>
     <row r="637">
-      <c s="3" r="E637"/>
+      <c s="4" r="E637"/>
     </row>
     <row r="638">
-      <c s="3" r="E638"/>
+      <c s="4" r="E638"/>
     </row>
     <row r="639">
-      <c s="3" r="E639"/>
+      <c s="4" r="E639"/>
     </row>
     <row r="640">
-      <c s="3" r="E640"/>
+      <c s="4" r="E640"/>
     </row>
     <row r="641">
-      <c s="3" r="E641"/>
+      <c s="4" r="E641"/>
     </row>
     <row r="642">
-      <c s="3" r="E642"/>
+      <c s="4" r="E642"/>
     </row>
     <row r="643">
-      <c s="3" r="E643"/>
+      <c s="4" r="E643"/>
     </row>
     <row r="644">
-      <c s="3" r="E644"/>
+      <c s="4" r="E644"/>
     </row>
     <row r="645">
-      <c s="3" r="E645"/>
+      <c s="4" r="E645"/>
     </row>
     <row r="646">
-      <c s="3" r="E646"/>
+      <c s="4" r="E646"/>
     </row>
     <row r="647">
-      <c s="3" r="E647"/>
+      <c s="4" r="E647"/>
     </row>
     <row r="648">
-      <c s="3" r="E648"/>
+      <c s="4" r="E648"/>
     </row>
     <row r="649">
-      <c s="3" r="E649"/>
+      <c s="4" r="E649"/>
     </row>
     <row r="650">
-      <c s="3" r="E650"/>
+      <c s="4" r="E650"/>
     </row>
     <row r="651">
-      <c s="3" r="E651"/>
+      <c s="4" r="E651"/>
     </row>
     <row r="652">
-      <c s="3" r="E652"/>
+      <c s="4" r="E652"/>
     </row>
     <row r="653">
-      <c s="3" r="E653"/>
+      <c s="4" r="E653"/>
     </row>
     <row r="654">
-      <c s="3" r="E654"/>
+      <c s="4" r="E654"/>
     </row>
     <row r="655">
-      <c s="3" r="E655"/>
+      <c s="4" r="E655"/>
     </row>
     <row r="656">
-      <c s="3" r="E656"/>
+      <c s="4" r="E656"/>
     </row>
     <row r="657">
-      <c s="3" r="E657"/>
+      <c s="4" r="E657"/>
     </row>
     <row r="658">
-      <c s="3" r="E658"/>
+      <c s="4" r="E658"/>
     </row>
     <row r="659">
-      <c s="3" r="E659"/>
+      <c s="4" r="E659"/>
     </row>
     <row r="660">
-      <c s="3" r="E660"/>
+      <c s="4" r="E660"/>
     </row>
     <row r="661">
-      <c s="3" r="E661"/>
+      <c s="4" r="E661"/>
     </row>
     <row r="662">
-      <c s="3" r="E662"/>
+      <c s="4" r="E662"/>
     </row>
     <row r="663">
-      <c s="3" r="E663"/>
+      <c s="4" r="E663"/>
     </row>
     <row r="664">
-      <c s="3" r="E664"/>
+      <c s="4" r="E664"/>
     </row>
     <row r="665">
-      <c s="3" r="E665"/>
+      <c s="4" r="E665"/>
     </row>
     <row r="666">
-      <c s="3" r="E666"/>
+      <c s="4" r="E666"/>
     </row>
     <row r="667">
-      <c s="3" r="E667"/>
+      <c s="4" r="E667"/>
     </row>
     <row r="668">
-      <c s="3" r="E668"/>
+      <c s="4" r="E668"/>
     </row>
     <row r="669">
-      <c s="3" r="E669"/>
+      <c s="4" r="E669"/>
     </row>
     <row r="670">
-      <c s="3" r="E670"/>
+      <c s="4" r="E670"/>
     </row>
     <row r="671">
-      <c s="3" r="E671"/>
+      <c s="4" r="E671"/>
     </row>
     <row r="672">
-      <c s="3" r="E672"/>
+      <c s="4" r="E672"/>
     </row>
     <row r="673">
-      <c s="3" r="E673"/>
+      <c s="4" r="E673"/>
     </row>
     <row r="674">
-      <c s="3" r="E674"/>
+      <c s="4" r="E674"/>
     </row>
     <row r="675">
-      <c s="3" r="E675"/>
+      <c s="4" r="E675"/>
     </row>
     <row r="676">
-      <c s="3" r="E676"/>
+      <c s="4" r="E676"/>
     </row>
     <row r="677">
-      <c s="3" r="E677"/>
+      <c s="4" r="E677"/>
     </row>
     <row r="678">
-      <c s="3" r="E678"/>
+      <c s="4" r="E678"/>
     </row>
     <row r="679">
-      <c s="3" r="E679"/>
+      <c s="4" r="E679"/>
     </row>
     <row r="680">
-      <c s="3" r="E680"/>
+      <c s="4" r="E680"/>
     </row>
     <row r="681">
-      <c s="3" r="E681"/>
+      <c s="4" r="E681"/>
     </row>
     <row r="682">
-      <c s="3" r="E682"/>
+      <c s="4" r="E682"/>
     </row>
     <row r="683">
-      <c s="3" r="E683"/>
+      <c s="4" r="E683"/>
     </row>
     <row r="684">
-      <c s="3" r="E684"/>
+      <c s="4" r="E684"/>
     </row>
     <row r="685">
-      <c s="3" r="E685"/>
+      <c s="4" r="E685"/>
     </row>
     <row r="686">
-      <c s="3" r="E686"/>
+      <c s="4" r="E686"/>
     </row>
     <row r="687">
-      <c s="3" r="E687"/>
+      <c s="4" r="E687"/>
     </row>
     <row r="688">
-      <c s="3" r="E688"/>
+      <c s="4" r="E688"/>
     </row>
     <row r="689">
-      <c s="3" r="E689"/>
+      <c s="4" r="E689"/>
     </row>
     <row r="690">
-      <c s="3" r="E690"/>
+      <c s="4" r="E690"/>
     </row>
     <row r="691">
-      <c s="3" r="E691"/>
+      <c s="4" r="E691"/>
     </row>
     <row r="692">
-      <c s="3" r="E692"/>
+      <c s="4" r="E692"/>
     </row>
     <row r="693">
-      <c s="3" r="E693"/>
+      <c s="4" r="E693"/>
     </row>
     <row r="694">
-      <c s="3" r="E694"/>
+      <c s="4" r="E694"/>
     </row>
     <row r="695">
-      <c s="3" r="E695"/>
+      <c s="4" r="E695"/>
     </row>
     <row r="696">
-      <c s="3" r="E696"/>
+      <c s="4" r="E696"/>
     </row>
     <row r="697">
-      <c s="3" r="E697"/>
+      <c s="4" r="E697"/>
     </row>
     <row r="698">
-      <c s="3" r="E698"/>
+      <c s="4" r="E698"/>
     </row>
     <row r="699">
-      <c s="3" r="E699"/>
+      <c s="4" r="E699"/>
     </row>
     <row r="700">
-      <c s="3" r="E700"/>
+      <c s="4" r="E700"/>
     </row>
     <row r="701">
-      <c s="3" r="E701"/>
+      <c s="4" r="E701"/>
     </row>
     <row r="702">
-      <c s="3" r="E702"/>
+      <c s="4" r="E702"/>
     </row>
     <row r="703">
-      <c s="3" r="E703"/>
+      <c s="4" r="E703"/>
     </row>
     <row r="704">
-      <c s="3" r="E704"/>
+      <c s="4" r="E704"/>
     </row>
     <row r="705">
-      <c s="3" r="E705"/>
+      <c s="4" r="E705"/>
     </row>
     <row r="706">
-      <c s="3" r="E706"/>
+      <c s="4" r="E706"/>
     </row>
     <row r="707">
-      <c s="3" r="E707"/>
+      <c s="4" r="E707"/>
     </row>
     <row r="708">
-      <c s="3" r="E708"/>
+      <c s="4" r="E708"/>
     </row>
     <row r="709">
-      <c s="3" r="E709"/>
+      <c s="4" r="E709"/>
     </row>
     <row r="710">
-      <c s="3" r="E710"/>
+      <c s="4" r="E710"/>
     </row>
     <row r="711">
-      <c s="3" r="E711"/>
+      <c s="4" r="E711"/>
     </row>
     <row r="712">
-      <c s="3" r="E712"/>
+      <c s="4" r="E712"/>
     </row>
     <row r="713">
-      <c s="3" r="E713"/>
+      <c s="4" r="E713"/>
     </row>
     <row r="714">
-      <c s="3" r="E714"/>
+      <c s="4" r="E714"/>
     </row>
     <row r="715">
-      <c s="3" r="E715"/>
+      <c s="4" r="E715"/>
     </row>
     <row r="716">
-      <c s="3" r="E716"/>
+      <c s="4" r="E716"/>
     </row>
     <row r="717">
-      <c s="3" r="E717"/>
+      <c s="4" r="E717"/>
     </row>
     <row r="718">
-      <c s="3" r="E718"/>
+      <c s="4" r="E718"/>
     </row>
     <row r="719">
-      <c s="3" r="E719"/>
+      <c s="4" r="E719"/>
     </row>
     <row r="720">
-      <c s="3" r="E720"/>
+      <c s="4" r="E720"/>
     </row>
     <row r="721">
-      <c s="3" r="E721"/>
+      <c s="4" r="E721"/>
     </row>
     <row r="722">
-      <c s="3" r="E722"/>
+      <c s="4" r="E722"/>
     </row>
     <row r="723">
-      <c s="3" r="E723"/>
+      <c s="4" r="E723"/>
     </row>
     <row r="724">
-      <c s="3" r="E724"/>
+      <c s="4" r="E724"/>
     </row>
     <row r="725">
-      <c s="3" r="E725"/>
+      <c s="4" r="E725"/>
     </row>
     <row r="726">
-      <c s="3" r="E726"/>
+      <c s="4" r="E726"/>
     </row>
     <row r="727">
-      <c s="3" r="E727"/>
+      <c s="4" r="E727"/>
     </row>
     <row r="728">
-      <c s="3" r="E728"/>
+      <c s="4" r="E728"/>
     </row>
     <row r="729">
-      <c s="3" r="E729"/>
+      <c s="4" r="E729"/>
     </row>
     <row r="730">
-      <c s="3" r="E730"/>
+      <c s="4" r="E730"/>
     </row>
     <row r="731">
-      <c s="3" r="E731"/>
+      <c s="4" r="E731"/>
     </row>
     <row r="732">
-      <c s="3" r="E732"/>
+      <c s="4" r="E732"/>
     </row>
     <row r="733">
-      <c s="3" r="E733"/>
+      <c s="4" r="E733"/>
     </row>
     <row r="734">
-      <c s="3" r="E734"/>
+      <c s="4" r="E734"/>
     </row>
     <row r="735">
-      <c s="3" r="E735"/>
+      <c s="4" r="E735"/>
     </row>
     <row r="736">
-      <c s="3" r="E736"/>
+      <c s="4" r="E736"/>
     </row>
     <row r="737">
-      <c s="3" r="E737"/>
+      <c s="4" r="E737"/>
     </row>
     <row r="738">
-      <c s="3" r="E738"/>
+      <c s="4" r="E738"/>
     </row>
     <row r="739">
-      <c s="3" r="E739"/>
+      <c s="4" r="E739"/>
     </row>
     <row r="740">
-      <c s="3" r="E740"/>
+      <c s="4" r="E740"/>
     </row>
     <row r="741">
-      <c s="3" r="E741"/>
+      <c s="4" r="E741"/>
     </row>
     <row r="742">
-      <c s="3" r="E742"/>
+      <c s="4" r="E742"/>
     </row>
     <row r="743">
-      <c s="3" r="E743"/>
+      <c s="4" r="E743"/>
     </row>
     <row r="744">
-      <c s="3" r="E744"/>
+      <c s="4" r="E744"/>
     </row>
     <row r="745">
-      <c s="3" r="E745"/>
+      <c s="4" r="E745"/>
     </row>
     <row r="746">
-      <c s="3" r="E746"/>
+      <c s="4" r="E746"/>
     </row>
     <row r="747">
-      <c s="3" r="E747"/>
+      <c s="4" r="E747"/>
     </row>
     <row r="748">
-      <c s="3" r="E748"/>
+      <c s="4" r="E748"/>
     </row>
     <row r="749">
-      <c s="3" r="E749"/>
+      <c s="4" r="E749"/>
     </row>
     <row r="750">
-      <c s="3" r="E750"/>
+      <c s="4" r="E750"/>
     </row>
     <row r="751">
-      <c s="3" r="E751"/>
+      <c s="4" r="E751"/>
     </row>
     <row r="752">
-      <c s="3" r="E752"/>
+      <c s="4" r="E752"/>
     </row>
     <row r="753">
-      <c s="3" r="E753"/>
+      <c s="4" r="E753"/>
     </row>
     <row r="754">
-      <c s="3" r="E754"/>
+      <c s="4" r="E754"/>
     </row>
     <row r="755">
-      <c s="3" r="E755"/>
+      <c s="4" r="E755"/>
     </row>
     <row r="756">
-      <c s="3" r="E756"/>
+      <c s="4" r="E756"/>
     </row>
     <row r="757">
-      <c s="3" r="E757"/>
+      <c s="4" r="E757"/>
     </row>
     <row r="758">
-      <c s="3" r="E758"/>
+      <c s="4" r="E758"/>
     </row>
     <row r="759">
-      <c s="3" r="E759"/>
+      <c s="4" r="E759"/>
     </row>
     <row r="760">
-      <c s="3" r="E760"/>
+      <c s="4" r="E760"/>
     </row>
     <row r="761">
-      <c s="3" r="E761"/>
+      <c s="4" r="E761"/>
     </row>
     <row r="762">
-      <c s="3" r="E762"/>
+      <c s="4" r="E762"/>
     </row>
     <row r="763">
-      <c s="3" r="E763"/>
+      <c s="4" r="E763"/>
     </row>
     <row r="764">
-      <c s="3" r="E764"/>
+      <c s="4" r="E764"/>
     </row>
     <row r="765">
-      <c s="3" r="E765"/>
+      <c s="4" r="E765"/>
     </row>
     <row r="766">
-      <c s="3" r="E766"/>
+      <c s="4" r="E766"/>
     </row>
     <row r="767">
-      <c s="3" r="E767"/>
+      <c s="4" r="E767"/>
     </row>
     <row r="768">
-      <c s="3" r="E768"/>
+      <c s="4" r="E768"/>
     </row>
     <row r="769">
-      <c s="3" r="E769"/>
+      <c s="4" r="E769"/>
     </row>
     <row r="770">
-      <c s="3" r="E770"/>
+      <c s="4" r="E770"/>
     </row>
     <row r="771">
-      <c s="3" r="E771"/>
+      <c s="4" r="E771"/>
     </row>
     <row r="772">
-      <c s="3" r="E772"/>
+      <c s="4" r="E772"/>
     </row>
     <row r="773">
-      <c s="3" r="E773"/>
+      <c s="4" r="E773"/>
     </row>
     <row r="774">
-      <c s="3" r="E774"/>
+      <c s="4" r="E774"/>
     </row>
     <row r="775">
-      <c s="3" r="E775"/>
+      <c s="4" r="E775"/>
     </row>
     <row r="776">
-      <c s="3" r="E776"/>
+      <c s="4" r="E776"/>
     </row>
     <row r="777">
-      <c s="3" r="E777"/>
+      <c s="4" r="E777"/>
     </row>
     <row r="778">
-      <c s="3" r="E778"/>
+      <c s="4" r="E778"/>
     </row>
     <row r="779">
-      <c s="3" r="E779"/>
+      <c s="4" r="E779"/>
     </row>
     <row r="780">
-      <c s="3" r="E780"/>
+      <c s="4" r="E780"/>
     </row>
     <row r="781">
-      <c s="3" r="E781"/>
+      <c s="4" r="E781"/>
     </row>
     <row r="782">
-      <c s="3" r="E782"/>
+      <c s="4" r="E782"/>
     </row>
     <row r="783">
-      <c s="3" r="E783"/>
+      <c s="4" r="E783"/>
     </row>
     <row r="784">
-      <c s="3" r="E784"/>
+      <c s="4" r="E784"/>
     </row>
     <row r="785">
-      <c s="3" r="E785"/>
+      <c s="4" r="E785"/>
     </row>
     <row r="786">
-      <c s="3" r="E786"/>
+      <c s="4" r="E786"/>
     </row>
     <row r="787">
-      <c s="3" r="E787"/>
+      <c s="4" r="E787"/>
     </row>
     <row r="788">
-      <c s="3" r="E788"/>
+      <c s="4" r="E788"/>
     </row>
     <row r="789">
-      <c s="3" r="E789"/>
+      <c s="4" r="E789"/>
     </row>
     <row r="790">
-      <c s="3" r="E790"/>
+      <c s="4" r="E790"/>
     </row>
     <row r="791">
-      <c s="3" r="E791"/>
+      <c s="4" r="E791"/>
     </row>
     <row r="792">
-      <c s="3" r="E792"/>
+      <c s="4" r="E792"/>
     </row>
     <row r="793">
-      <c s="3" r="E793"/>
+      <c s="4" r="E793"/>
     </row>
     <row r="794">
-      <c s="3" r="E794"/>
+      <c s="4" r="E794"/>
     </row>
     <row r="795">
-      <c s="3" r="E795"/>
+      <c s="4" r="E795"/>
     </row>
     <row r="796">
-      <c s="3" r="E796"/>
+      <c s="4" r="E796"/>
     </row>
     <row r="797">
-      <c s="3" r="E797"/>
+      <c s="4" r="E797"/>
     </row>
     <row r="798">
-      <c s="3" r="E798"/>
+      <c s="4" r="E798"/>
     </row>
     <row r="799">
-      <c s="3" r="E799"/>
+      <c s="4" r="E799"/>
     </row>
     <row r="800">
-      <c s="3" r="E800"/>
+      <c s="4" r="E800"/>
     </row>
     <row r="801">
-      <c s="3" r="E801"/>
+      <c s="4" r="E801"/>
     </row>
     <row r="802">
-      <c s="3" r="E802"/>
+      <c s="4" r="E802"/>
     </row>
     <row r="803">
-      <c s="3" r="E803"/>
+      <c s="4" r="E803"/>
     </row>
     <row r="804">
-      <c s="3" r="E804"/>
+      <c s="4" r="E804"/>
     </row>
     <row r="805">
-      <c s="3" r="E805"/>
+      <c s="4" r="E805"/>
     </row>
     <row r="806">
-      <c s="3" r="E806"/>
+      <c s="4" r="E806"/>
     </row>
     <row r="807">
-      <c s="3" r="E807"/>
+      <c s="4" r="E807"/>
     </row>
     <row r="808">
-      <c s="3" r="E808"/>
+      <c s="4" r="E808"/>
     </row>
     <row r="809">
-      <c s="3" r="E809"/>
+      <c s="4" r="E809"/>
     </row>
     <row r="810">
-      <c s="3" r="E810"/>
+      <c s="4" r="E810"/>
     </row>
     <row r="811">
-      <c s="3" r="E811"/>
+      <c s="4" r="E811"/>
     </row>
     <row r="812">
-      <c s="3" r="E812"/>
+      <c s="4" r="E812"/>
     </row>
     <row r="813">
-      <c s="3" r="E813"/>
+      <c s="4" r="E813"/>
     </row>
     <row r="814">
-      <c s="3" r="E814"/>
+      <c s="4" r="E814"/>
     </row>
     <row r="815">
-      <c s="3" r="E815"/>
+      <c s="4" r="E815"/>
     </row>
     <row r="816">
-      <c s="3" r="E816"/>
+      <c s="4" r="E816"/>
     </row>
     <row r="817">
-      <c s="3" r="E817"/>
+      <c s="4" r="E817"/>
     </row>
     <row r="818">
-      <c s="3" r="E818"/>
+      <c s="4" r="E818"/>
     </row>
     <row r="819">
-      <c s="3" r="E819"/>
+      <c s="4" r="E819"/>
     </row>
     <row r="820">
-      <c s="3" r="E820"/>
+      <c s="4" r="E820"/>
     </row>
     <row r="821">
-      <c s="3" r="E821"/>
+      <c s="4" r="E821"/>
     </row>
     <row r="822">
-      <c s="3" r="E822"/>
+      <c s="4" r="E822"/>
     </row>
     <row r="823">
-      <c s="3" r="E823"/>
+      <c s="4" r="E823"/>
     </row>
     <row r="824">
-      <c s="3" r="E824"/>
+      <c s="4" r="E824"/>
     </row>
     <row r="825">
-      <c s="3" r="E825"/>
+      <c s="4" r="E825"/>
     </row>
     <row r="826">
-      <c s="3" r="E826"/>
+      <c s="4" r="E826"/>
     </row>
     <row r="827">
-      <c s="3" r="E827"/>
+      <c s="4" r="E827"/>
     </row>
     <row r="828">
-      <c s="3" r="E828"/>
+      <c s="4" r="E828"/>
     </row>
     <row r="829">
-      <c s="3" r="E829"/>
+      <c s="4" r="E829"/>
     </row>
     <row r="830">
-      <c s="3" r="E830"/>
+      <c s="4" r="E830"/>
     </row>
     <row r="831">
-      <c s="3" r="E831"/>
+      <c s="4" r="E831"/>
     </row>
     <row r="832">
-      <c s="3" r="E832"/>
+      <c s="4" r="E832"/>
     </row>
     <row r="833">
-      <c s="3" r="E833"/>
+      <c s="4" r="E833"/>
     </row>
     <row r="834">
-      <c s="3" r="E834"/>
+      <c s="4" r="E834"/>
     </row>
     <row r="835">
-      <c s="3" r="E835"/>
+      <c s="4" r="E835"/>
     </row>
     <row r="836">
-      <c s="3" r="E836"/>
+      <c s="4" r="E836"/>
     </row>
     <row r="837">
-      <c s="3" r="E837"/>
+      <c s="4" r="E837"/>
     </row>
     <row r="838">
-      <c s="3" r="E838"/>
+      <c s="4" r="E838"/>
     </row>
     <row r="839">
-      <c s="3" r="E839"/>
+      <c s="4" r="E839"/>
     </row>
     <row r="840">
-      <c s="3" r="E840"/>
+      <c s="4" r="E840"/>
     </row>
     <row r="841">
-      <c s="3" r="E841"/>
+      <c s="4" r="E841"/>
     </row>
     <row r="842">
-      <c s="3" r="E842"/>
+      <c s="4" r="E842"/>
     </row>
     <row r="843">
-      <c s="3" r="E843"/>
+      <c s="4" r="E843"/>
     </row>
     <row r="844">
-      <c s="3" r="E844"/>
+      <c s="4" r="E844"/>
     </row>
     <row r="845">
-      <c s="3" r="E845"/>
+      <c s="4" r="E845"/>
     </row>
     <row r="846">
-      <c s="3" r="E846"/>
+      <c s="4" r="E846"/>
     </row>
     <row r="847">
-      <c s="3" r="E847"/>
+      <c s="4" r="E847"/>
     </row>
     <row r="848">
-      <c s="3" r="E848"/>
+      <c s="4" r="E848"/>
     </row>
     <row r="849">
-      <c s="3" r="E849"/>
+      <c s="4" r="E849"/>
     </row>
     <row r="850">
-      <c s="3" r="E850"/>
+      <c s="4" r="E850"/>
     </row>
     <row r="851">
-      <c s="3" r="E851"/>
+      <c s="4" r="E851"/>
     </row>
     <row r="852">
-      <c s="3" r="E852"/>
+      <c s="4" r="E852"/>
     </row>
     <row r="853">
-      <c s="3" r="E853"/>
+      <c s="4" r="E853"/>
     </row>
     <row r="854">
-      <c s="3" r="E854"/>
+      <c s="4" r="E854"/>
     </row>
     <row r="855">
-      <c s="3" r="E855"/>
+      <c s="4" r="E855"/>
     </row>
     <row r="856">
-      <c s="3" r="E856"/>
+      <c s="4" r="E856"/>
     </row>
     <row r="857">
-      <c s="3" r="E857"/>
+      <c s="4" r="E857"/>
     </row>
     <row r="858">
-      <c s="3" r="E858"/>
+      <c s="4" r="E858"/>
     </row>
     <row r="859">
-      <c s="3" r="E859"/>
+      <c s="4" r="E859"/>
     </row>
     <row r="860">
-      <c s="3" r="E860"/>
+      <c s="4" r="E860"/>
     </row>
     <row r="861">
-      <c s="3" r="E861"/>
+      <c s="4" r="E861"/>
     </row>
     <row r="862">
-      <c s="3" r="E862"/>
+      <c s="4" r="E862"/>
     </row>
     <row r="863">
-      <c s="3" r="E863"/>
+      <c s="4" r="E863"/>
     </row>
     <row r="864">
-      <c s="3" r="E864"/>
+      <c s="4" r="E864"/>
     </row>
     <row r="865">
-      <c s="3" r="E865"/>
+      <c s="4" r="E865"/>
     </row>
     <row r="866">
-      <c s="3" r="E866"/>
+      <c s="4" r="E866"/>
     </row>
     <row r="867">
-      <c s="3" r="E867"/>
+      <c s="4" r="E867"/>
     </row>
     <row r="868">
-      <c s="3" r="E868"/>
+      <c s="4" r="E868"/>
     </row>
     <row r="869">
-      <c s="3" r="E869"/>
+      <c s="4" r="E869"/>
     </row>
     <row r="870">
-      <c s="3" r="E870"/>
+      <c s="4" r="E870"/>
     </row>
     <row r="871">
-      <c s="3" r="E871"/>
+      <c s="4" r="E871"/>
     </row>
     <row r="872">
-      <c s="3" r="E872"/>
+      <c s="4" r="E872"/>
     </row>
     <row r="873">
-      <c s="3" r="E873"/>
+      <c s="4" r="E873"/>
     </row>
     <row r="874">
-      <c s="3" r="E874"/>
+      <c s="4" r="E874"/>
     </row>
     <row r="875">
-      <c s="3" r="E875"/>
+      <c s="4" r="E875"/>
     </row>
     <row r="876">
-      <c s="3" r="E876"/>
+      <c s="4" r="E876"/>
     </row>
     <row r="877">
-      <c s="3" r="E877"/>
+      <c s="4" r="E877"/>
     </row>
     <row r="878">
-      <c s="3" r="E878"/>
+      <c s="4" r="E878"/>
     </row>
     <row r="879">
-      <c s="3" r="E879"/>
+      <c s="4" r="E879"/>
     </row>
     <row r="880">
-      <c s="3" r="E880"/>
+      <c s="4" r="E880"/>
     </row>
     <row r="881">
-      <c s="3" r="E881"/>
+      <c s="4" r="E881"/>
     </row>
     <row r="882">
-      <c s="3" r="E882"/>
+      <c s="4" r="E882"/>
     </row>
     <row r="883">
-      <c s="3" r="E883"/>
+      <c s="4" r="E883"/>
     </row>
     <row r="884">
-      <c s="3" r="E884"/>
+      <c s="4" r="E884"/>
     </row>
     <row r="885">
-      <c s="3" r="E885"/>
+      <c s="4" r="E885"/>
     </row>
     <row r="886">
-      <c s="3" r="E886"/>
+      <c s="4" r="E886"/>
     </row>
     <row r="887">
-      <c s="3" r="E887"/>
+      <c s="4" r="E887"/>
     </row>
     <row r="888">
-      <c s="3" r="E888"/>
+      <c s="4" r="E888"/>
     </row>
     <row r="889">
-      <c s="3" r="E889"/>
+      <c s="4" r="E889"/>
     </row>
     <row r="890">
-      <c s="3" r="E890"/>
+      <c s="4" r="E890"/>
     </row>
     <row r="891">
-      <c s="3" r="E891"/>
+      <c s="4" r="E891"/>
     </row>
     <row r="892">
-      <c s="3" r="E892"/>
+      <c s="4" r="E892"/>
     </row>
     <row r="893">
-      <c s="3" r="E893"/>
+      <c s="4" r="E893"/>
     </row>
     <row r="894">
-      <c s="3" r="E894"/>
+      <c s="4" r="E894"/>
     </row>
     <row r="895">
-      <c s="3" r="E895"/>
+      <c s="4" r="E895"/>
     </row>
     <row r="896">
-      <c s="3" r="E896"/>
+      <c s="4" r="E896"/>
     </row>
     <row r="897">
-      <c s="3" r="E897"/>
+      <c s="4" r="E897"/>
     </row>
     <row r="898">
-      <c s="3" r="E898"/>
+      <c s="4" r="E898"/>
     </row>
     <row r="899">
-      <c s="3" r="E899"/>
+      <c s="4" r="E899"/>
     </row>
     <row r="900">
-      <c s="3" r="E900"/>
+      <c s="4" r="E900"/>
     </row>
     <row r="901">
-      <c s="3" r="E901"/>
+      <c s="4" r="E901"/>
     </row>
     <row r="902">
-      <c s="3" r="E902"/>
+      <c s="4" r="E902"/>
     </row>
     <row r="903">
-      <c s="3" r="E903"/>
+      <c s="4" r="E903"/>
     </row>
     <row r="904">
-      <c s="3" r="E904"/>
+      <c s="4" r="E904"/>
     </row>
     <row r="905">
-      <c s="3" r="E905"/>
+      <c s="4" r="E905"/>
     </row>
     <row r="906">
-      <c s="3" r="E906"/>
+      <c s="4" r="E906"/>
     </row>
     <row r="907">
-      <c s="3" r="E907"/>
+      <c s="4" r="E907"/>
     </row>
     <row r="908">
-      <c s="3" r="E908"/>
+      <c s="4" r="E908"/>
     </row>
     <row r="909">
-      <c s="3" r="E909"/>
+      <c s="4" r="E909"/>
     </row>
     <row r="910">
-      <c s="3" r="E910"/>
+      <c s="4" r="E910"/>
     </row>
     <row r="911">
-      <c s="3" r="E911"/>
+      <c s="4" r="E911"/>
     </row>
     <row r="912">
-      <c s="3" r="E912"/>
+      <c s="4" r="E912"/>
     </row>
     <row r="913">
-      <c s="3" r="E913"/>
+      <c s="4" r="E913"/>
     </row>
     <row r="914">
-      <c s="3" r="E914"/>
+      <c s="4" r="E914"/>
     </row>
     <row r="915">
-      <c s="3" r="E915"/>
+      <c s="4" r="E915"/>
     </row>
     <row r="916">
-      <c s="3" r="E916"/>
+      <c s="4" r="E916"/>
     </row>
     <row r="917">
-      <c s="3" r="E917"/>
+      <c s="4" r="E917"/>
     </row>
     <row r="918">
-      <c s="3" r="E918"/>
+      <c s="4" r="E918"/>
     </row>
     <row r="919">
-      <c s="3" r="E919"/>
+      <c s="4" r="E919"/>
     </row>
     <row r="920">
-      <c s="3" r="E920"/>
+      <c s="4" r="E920"/>
     </row>
     <row r="921">
-      <c s="3" r="E921"/>
+      <c s="4" r="E921"/>
     </row>
     <row r="922">
-      <c s="3" r="E922"/>
+      <c s="4" r="E922"/>
     </row>
     <row r="923">
-      <c s="3" r="E923"/>
+      <c s="4" r="E923"/>
     </row>
     <row r="924">
-      <c s="3" r="E924"/>
+      <c s="4" r="E924"/>
     </row>
     <row r="925">
-      <c s="3" r="E925"/>
+      <c s="4" r="E925"/>
     </row>
     <row r="926">
-      <c s="3" r="E926"/>
+      <c s="4" r="E926"/>
     </row>
     <row r="927">
-      <c s="3" r="E927"/>
+      <c s="4" r="E927"/>
     </row>
     <row r="928">
-      <c s="3" r="E928"/>
+      <c s="4" r="E928"/>
     </row>
     <row r="929">
-      <c s="3" r="E929"/>
+      <c s="4" r="E929"/>
     </row>
     <row r="930">
-      <c s="3" r="E930"/>
+      <c s="4" r="E930"/>
     </row>
     <row r="931">
-      <c s="3" r="E931"/>
+      <c s="4" r="E931"/>
     </row>
     <row r="932">
-      <c s="3" r="E932"/>
+      <c s="4" r="E932"/>
     </row>
     <row r="933">
-      <c s="3" r="E933"/>
+      <c s="4" r="E933"/>
     </row>
     <row r="934">
-      <c s="3" r="E934"/>
+      <c s="4" r="E934"/>
     </row>
     <row r="935">
-      <c s="3" r="E935"/>
+      <c s="4" r="E935"/>
     </row>
     <row r="936">
-      <c s="3" r="E936"/>
+      <c s="4" r="E936"/>
     </row>
     <row r="937">
-      <c s="3" r="E937"/>
+      <c s="4" r="E937"/>
     </row>
     <row r="938">
-      <c s="3" r="E938"/>
+      <c s="4" r="E938"/>
     </row>
     <row r="939">
-      <c s="3" r="E939"/>
+      <c s="4" r="E939"/>
     </row>
     <row r="940">
-      <c s="3" r="E940"/>
+      <c s="4" r="E940"/>
     </row>
     <row r="941">
-      <c s="3" r="E941"/>
+      <c s="4" r="E941"/>
     </row>
     <row r="942">
-      <c s="3" r="E942"/>
+      <c s="4" r="E942"/>
     </row>
     <row r="943">
-      <c s="3" r="E943"/>
+      <c s="4" r="E943"/>
     </row>
     <row r="944">
-      <c s="3" r="E944"/>
+      <c s="4" r="E944"/>
     </row>
     <row r="945">
-      <c s="3" r="E945"/>
+      <c s="4" r="E945"/>
     </row>
     <row r="946">
-      <c s="3" r="E946"/>
+      <c s="4" r="E946"/>
     </row>
     <row r="947">
-      <c s="3" r="E947"/>
+      <c s="4" r="E947"/>
     </row>
     <row r="948">
-      <c s="3" r="E948"/>
+      <c s="4" r="E948"/>
     </row>
     <row r="949">
-      <c s="3" r="E949"/>
+      <c s="4" r="E949"/>
     </row>
     <row r="950">
-      <c s="3" r="E950"/>
+      <c s="4" r="E950"/>
     </row>
     <row r="951">
-      <c s="3" r="E951"/>
+      <c s="4" r="E951"/>
     </row>
     <row r="952">
-      <c s="3" r="E952"/>
+      <c s="4" r="E952"/>
     </row>
     <row r="953">
-      <c s="3" r="E953"/>
+      <c s="4" r="E953"/>
     </row>
     <row r="954">
-      <c s="3" r="E954"/>
+      <c s="4" r="E954"/>
     </row>
     <row r="955">
-      <c s="3" r="E955"/>
+      <c s="4" r="E955"/>
     </row>
     <row r="956">
-      <c s="3" r="E956"/>
+      <c s="4" r="E956"/>
     </row>
     <row r="957">
-      <c s="3" r="E957"/>
+      <c s="4" r="E957"/>
     </row>
     <row r="958">
-      <c s="3" r="E958"/>
+      <c s="4" r="E958"/>
     </row>
     <row r="959">
-      <c s="3" r="E959"/>
+      <c s="4" r="E959"/>
     </row>
     <row r="960">
-      <c s="3" r="E960"/>
+      <c s="4" r="E960"/>
     </row>
     <row r="961">
-      <c s="3" r="E961"/>
+      <c s="4" r="E961"/>
     </row>
     <row r="962">
-      <c s="3" r="E962"/>
+      <c s="4" r="E962"/>
     </row>
     <row r="963">
-      <c s="3" r="E963"/>
+      <c s="4" r="E963"/>
     </row>
     <row r="964">
-      <c s="3" r="E964"/>
+      <c s="4" r="E964"/>
     </row>
     <row r="965">
-      <c s="3" r="E965"/>
+      <c s="4" r="E965"/>
     </row>
     <row r="966">
-      <c s="3" r="E966"/>
+      <c s="4" r="E966"/>
     </row>
     <row r="967">
-      <c s="3" r="E967"/>
+      <c s="4" r="E967"/>
     </row>
     <row r="968">
-      <c s="3" r="E968"/>
+      <c s="4" r="E968"/>
     </row>
     <row r="969">
-      <c s="3" r="E969"/>
+      <c s="4" r="E969"/>
     </row>
     <row r="970">
-      <c s="3" r="E970"/>
+      <c s="4" r="E970"/>
     </row>
     <row r="971">
-      <c s="3" r="E971"/>
+      <c s="4" r="E971"/>
     </row>
     <row r="972">
-      <c s="3" r="E972"/>
+      <c s="4" r="E972"/>
     </row>
     <row r="973">
-      <c s="3" r="E973"/>
+      <c s="4" r="E973"/>
     </row>
     <row r="974">
-      <c s="3" r="E974"/>
+      <c s="4" r="E974"/>
     </row>
     <row r="975">
-      <c s="3" r="E975"/>
+      <c s="4" r="E975"/>
     </row>
     <row r="976">
-      <c s="3" r="E976"/>
+      <c s="4" r="E976"/>
     </row>
     <row r="977">
-      <c s="3" r="E977"/>
+      <c s="4" r="E977"/>
     </row>
     <row r="978">
-      <c s="3" r="E978"/>
+      <c s="4" r="E978"/>
     </row>
     <row r="979">
-      <c s="3" r="E979"/>
+      <c s="4" r="E979"/>
     </row>
     <row r="980">
-      <c s="3" r="E980"/>
+      <c s="4" r="E980"/>
     </row>
     <row r="981">
-      <c s="3" r="E981"/>
+      <c s="4" r="E981"/>
     </row>
     <row r="982">
-      <c s="3" r="E982"/>
+      <c s="4" r="E982"/>
     </row>
     <row r="983">
-      <c s="3" r="E983"/>
+      <c s="4" r="E983"/>
     </row>
     <row r="984">
-      <c s="3" r="E984"/>
+      <c s="4" r="E984"/>
     </row>
     <row r="985">
-      <c s="3" r="E985"/>
+      <c s="4" r="E985"/>
     </row>
     <row r="986">
-      <c s="3" r="E986"/>
+      <c s="4" r="E986"/>
     </row>
     <row r="987">
-      <c s="3" r="E987"/>
+      <c s="4" r="E987"/>
     </row>
     <row r="988">
-      <c s="3" r="E988"/>
+      <c s="4" r="E988"/>
     </row>
     <row r="989">
-      <c s="3" r="E989"/>
+      <c s="4" r="E989"/>
     </row>
     <row r="990">
-      <c s="3" r="E990"/>
+      <c s="4" r="E990"/>
     </row>
     <row r="991">
-      <c s="3" r="E991"/>
+      <c s="4" r="E991"/>
     </row>
     <row r="992">
-      <c s="3" r="E992"/>
+      <c s="4" r="E992"/>
     </row>
     <row r="993">
-      <c s="3" r="E993"/>
+      <c s="4" r="E993"/>
     </row>
     <row r="994">
-      <c s="3" r="E994"/>
+      <c s="4" r="E994"/>
     </row>
     <row r="995">
-      <c s="3" r="E995"/>
+      <c s="4" r="E995"/>
     </row>
     <row r="996">
-      <c s="3" r="E996"/>
+      <c s="4" r="E996"/>
     </row>
     <row r="997">
-      <c s="3" r="E997"/>
+      <c s="4" r="E997"/>
     </row>
     <row r="998">
-      <c s="3" r="E998"/>
+      <c s="4" r="E998"/>
     </row>
     <row r="999">
-      <c s="3" r="E999"/>
+      <c s="4" r="E999"/>
     </row>
     <row r="1000">
-      <c s="3" r="E1000"/>
+      <c s="4" r="E1000"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F5" r:id="rId4"/>
+  </hyperlinks>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>